<commit_message>
docs: stats for delivery time (v1, v2) completed
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fedebrando\SORTproject\SantaClausProblem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27126E43-7937-4CC5-946E-53D7677FA04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832B5C1F-C609-4A65-B556-D140A644AD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery time (v1, v2)" sheetId="1" r:id="rId1"/>
     <sheet name="Santa busy probability (v1)" sheetId="2" r:id="rId2"/>
+    <sheet name="Delivery delay (v1)" sheetId="3" r:id="rId3"/>
+    <sheet name="Delivery delay (v3)" sheetId="5" r:id="rId4"/>
+    <sheet name="Info" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Delivery time (v1, v2)</t>
   </si>
@@ -66,19 +69,100 @@
     <t>The statistic probabilty, in function of number of elves, that Santa is busy when last rein arrives at North Pole</t>
   </si>
   <si>
-    <t>Average and Standard Deviation for 200 delivery times in v1 and v2 executed with 9 reindeer and 10 elves</t>
-  </si>
-  <si>
-    <t>Each probability point is a statistic probability computed with 200 samples executing v1 with 9 reindeer and 10 elves</t>
-  </si>
-  <si>
     <t>#elves</t>
   </si>
   <si>
     <t>busy probability</t>
   </si>
   <si>
-    <t>samples</t>
+    <t>Delivery delay (v1)</t>
+  </si>
+  <si>
+    <t>The time period between last rein arrival and the beginning of delivery</t>
+  </si>
+  <si>
+    <t>Delivery delay (v3)</t>
+  </si>
+  <si>
+    <t>The time period, in function of number of Santa entities and number of elves, between last rein arrival and the beginning of delivery</t>
+  </si>
+  <si>
+    <t>#santa</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Average and Standard Deviation of 200 time measurments for each reasonable (#santa, #elves) pair, 9 reindeer and 3 elves in a consulting group</t>
+  </si>
+  <si>
+    <t>Average and Standard Deviation for 200 delivery times in v1 and v2 executed with 9 reindeer, 10 elves and 3 elves in a consulting group</t>
+  </si>
+  <si>
+    <t>Average and Standard Deviation of 200 measurements in v1 with 9 reindeer, 10 elves and 3 elves in a consulting group</t>
+  </si>
+  <si>
+    <t>Each probability point is a statistic probability computed with 200 samples executing v1 with 9 reindeer, 10 elves and 3 elves in a consulting group</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>In this page there are some information about system used to execute the experiments</t>
+  </si>
+  <si>
+    <t>Kernel version</t>
+  </si>
+  <si>
+    <t>5.15.167.4-1</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Ubuntu (version 2)</t>
+  </si>
+  <si>
+    <t>Windows 11 Pro (build 26100.3194)</t>
+  </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>7,7 Gbyte</t>
+  </si>
+  <si>
+    <t>The experiments take place in guest system</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>WSL (Windows Subsystem for Linux)  (version 2.3.26.0)</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i7-10750H CPU @ 2.60GHz</t>
+  </si>
+  <si>
+    <t>15,8 Gbyte</t>
   </si>
 </sst>
 </file>
@@ -158,16 +242,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1519,7 +1606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1543,47 +1630,47 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <f>AVERAGE(C10:C209)</f>
-        <v>98.856933459999993</v>
-      </c>
-      <c r="E7" s="5" t="s">
+        <v>99.420908570000009</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f>AVERAGE(F10:F209)</f>
         <v>293.90788766499981</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f>_xlfn.STDEV.S(C10:C209)</f>
-        <v>106.50433110684713</v>
-      </c>
-      <c r="E8" s="5" t="s">
+        <v>87.696224203788773</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>_xlfn.STDEV.S(F10:F209)</f>
         <v>130.31891276337979</v>
       </c>
@@ -1593,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>30.364530999999999</v>
+        <v>41.642242000000003</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>3</v>
@@ -1604,7 +1691,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
-        <v>91.607118</v>
+        <v>44.511645999999999</v>
       </c>
       <c r="F11" s="1">
         <v>275.911227</v>
@@ -1612,7 +1699,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
-        <v>174.11973699999999</v>
+        <v>6.2237929999999997</v>
       </c>
       <c r="F12" s="1">
         <v>156.00310500000001</v>
@@ -1620,7 +1707,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
-        <v>186.737955</v>
+        <v>40.814673999999997</v>
       </c>
       <c r="F13" s="1">
         <v>374.570763</v>
@@ -1628,7 +1715,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
-        <v>172.27825000000001</v>
+        <v>37.943975999999999</v>
       </c>
       <c r="F14" s="1">
         <v>434.03449999999998</v>
@@ -1636,7 +1723,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
-        <v>47.687012000000003</v>
+        <v>9.8922089999999994</v>
       </c>
       <c r="F15" s="1">
         <v>247.565561</v>
@@ -1644,7 +1731,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
-        <v>10.551392</v>
+        <v>393.09140200000002</v>
       </c>
       <c r="F16" s="1">
         <v>261.57752499999998</v>
@@ -1652,7 +1739,7 @@
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="1">
-        <v>12.812894999999999</v>
+        <v>151.845564</v>
       </c>
       <c r="F17" s="1">
         <v>209.921831</v>
@@ -1660,7 +1747,7 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="1">
-        <v>53.146568000000002</v>
+        <v>204.78099599999999</v>
       </c>
       <c r="F18" s="1">
         <v>386.47410500000001</v>
@@ -1668,7 +1755,7 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="1">
-        <v>115.804872</v>
+        <v>245.990084</v>
       </c>
       <c r="F19" s="1">
         <v>247.690077</v>
@@ -1676,7 +1763,7 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="1">
-        <v>4.9468620000000003</v>
+        <v>128.64718999999999</v>
       </c>
       <c r="F20" s="1">
         <v>316.37589300000002</v>
@@ -1684,7 +1771,7 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C21" s="1">
-        <v>210.70689300000001</v>
+        <v>92.037328000000002</v>
       </c>
       <c r="F21" s="1">
         <v>363.55479200000002</v>
@@ -1692,7 +1779,7 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="1">
-        <v>27.694227999999999</v>
+        <v>91.059515000000005</v>
       </c>
       <c r="F22" s="1">
         <v>99.819243</v>
@@ -1700,7 +1787,7 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" s="1">
-        <v>229.10537500000001</v>
+        <v>48.464236999999997</v>
       </c>
       <c r="F23" s="1">
         <v>363.67911600000002</v>
@@ -1708,7 +1795,7 @@
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C24" s="1">
-        <v>70.144103999999999</v>
+        <v>44.758051999999999</v>
       </c>
       <c r="F24" s="1">
         <v>391.45359400000001</v>
@@ -1716,7 +1803,7 @@
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25" s="1">
-        <v>42.896495999999999</v>
+        <v>282.835016</v>
       </c>
       <c r="F25" s="1">
         <v>286.807366</v>
@@ -1724,7 +1811,7 @@
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
-        <v>173.481122</v>
+        <v>62.37424</v>
       </c>
       <c r="F26" s="1">
         <v>248.33920000000001</v>
@@ -1732,7 +1819,7 @@
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27" s="1">
-        <v>176.58071899999999</v>
+        <v>115.785732</v>
       </c>
       <c r="F27" s="1">
         <v>533.769541</v>
@@ -1740,7 +1827,7 @@
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C28" s="1">
-        <v>13.620224</v>
+        <v>98.726399000000001</v>
       </c>
       <c r="F28" s="1">
         <v>336.45120800000001</v>
@@ -1748,7 +1835,7 @@
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" s="1">
-        <v>56.730071000000002</v>
+        <v>3.5232779999999999</v>
       </c>
       <c r="F29" s="1">
         <v>191.358092</v>
@@ -1756,7 +1843,7 @@
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C30" s="1">
-        <v>57.207017999999998</v>
+        <v>160.68085300000001</v>
       </c>
       <c r="F30" s="1">
         <v>262.82657499999999</v>
@@ -1764,7 +1851,7 @@
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C31" s="1">
-        <v>16.936931000000001</v>
+        <v>70.693942000000007</v>
       </c>
       <c r="F31" s="1">
         <v>224.452741</v>
@@ -1772,7 +1859,7 @@
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C32" s="1">
-        <v>16.824829999999999</v>
+        <v>4.0155010000000004</v>
       </c>
       <c r="F32" s="1">
         <v>309.61175900000001</v>
@@ -1780,7 +1867,7 @@
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
-        <v>106.750084</v>
+        <v>1.8250029999999999</v>
       </c>
       <c r="F33" s="1">
         <v>202.35454899999999</v>
@@ -1788,7 +1875,7 @@
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C34" s="1">
-        <v>0.57499500000000003</v>
+        <v>70.196586999999994</v>
       </c>
       <c r="F34" s="1">
         <v>231.39310900000001</v>
@@ -1796,7 +1883,7 @@
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C35" s="1">
-        <v>4.994332</v>
+        <v>58.835532000000001</v>
       </c>
       <c r="F35" s="1">
         <v>184.41810599999999</v>
@@ -1804,7 +1891,7 @@
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C36" s="1">
-        <v>14.645496</v>
+        <v>26.921417000000002</v>
       </c>
       <c r="F36" s="1">
         <v>229.517944</v>
@@ -1812,7 +1899,7 @@
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
-        <v>38.566369999999999</v>
+        <v>202.84929099999999</v>
       </c>
       <c r="F37" s="1">
         <v>135.34553099999999</v>
@@ -1820,7 +1907,7 @@
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C38" s="1">
-        <v>57.562018999999999</v>
+        <v>88.939025999999998</v>
       </c>
       <c r="F38" s="1">
         <v>1046.8146630000001</v>
@@ -1828,7 +1915,7 @@
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C39" s="1">
-        <v>42.435366999999999</v>
+        <v>181.10600099999999</v>
       </c>
       <c r="F39" s="1">
         <v>129.849974</v>
@@ -1836,7 +1923,7 @@
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C40" s="1">
-        <v>18.888769</v>
+        <v>341.74405300000001</v>
       </c>
       <c r="F40" s="1">
         <v>435.30235399999998</v>
@@ -1844,7 +1931,7 @@
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C41" s="1">
-        <v>79.982990000000001</v>
+        <v>28.885664999999999</v>
       </c>
       <c r="F41" s="1">
         <v>655.06666299999995</v>
@@ -1852,7 +1939,7 @@
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C42" s="1">
-        <v>233.31099900000001</v>
+        <v>62.548431999999998</v>
       </c>
       <c r="F42" s="1">
         <v>290.61379699999998</v>
@@ -1860,7 +1947,7 @@
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C43" s="1">
-        <v>42.405836999999998</v>
+        <v>59.452939000000001</v>
       </c>
       <c r="F43" s="1">
         <v>276.242164</v>
@@ -1868,7 +1955,7 @@
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C44" s="1">
-        <v>56.023733</v>
+        <v>175.990994</v>
       </c>
       <c r="F44" s="1">
         <v>185.97538599999999</v>
@@ -1876,7 +1963,7 @@
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C45" s="1">
-        <v>21.512713000000002</v>
+        <v>50.280313999999997</v>
       </c>
       <c r="F45" s="1">
         <v>166.06198699999999</v>
@@ -1884,7 +1971,7 @@
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C46" s="1">
-        <v>108.259175</v>
+        <v>58.788006000000003</v>
       </c>
       <c r="F46" s="1">
         <v>323.03314599999999</v>
@@ -1892,7 +1979,7 @@
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C47" s="1">
-        <v>15.791176</v>
+        <v>21.771999999999998</v>
       </c>
       <c r="F47" s="1">
         <v>208.388713</v>
@@ -1900,7 +1987,7 @@
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C48" s="1">
-        <v>16.737363999999999</v>
+        <v>14.4482</v>
       </c>
       <c r="F48" s="1">
         <v>547.54020100000002</v>
@@ -1908,7 +1995,7 @@
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C49" s="1">
-        <v>41.350479999999997</v>
+        <v>153.36685900000001</v>
       </c>
       <c r="F49" s="1">
         <v>491.87410899999998</v>
@@ -1916,7 +2003,7 @@
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C50" s="1">
-        <v>118.465716</v>
+        <v>245.784684</v>
       </c>
       <c r="F50" s="1">
         <v>482.46617800000001</v>
@@ -1924,7 +2011,7 @@
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C51" s="1">
-        <v>2.06473</v>
+        <v>8.6852029999999996</v>
       </c>
       <c r="F51" s="1">
         <v>235.41824600000001</v>
@@ -1932,7 +2019,7 @@
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C52" s="1">
-        <v>23.354671</v>
+        <v>67.397024000000002</v>
       </c>
       <c r="F52" s="1">
         <v>444.78371600000003</v>
@@ -1940,7 +2027,7 @@
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C53" s="1">
-        <v>76.586083000000002</v>
+        <v>169.09713300000001</v>
       </c>
       <c r="F53" s="1">
         <v>165.28153599999999</v>
@@ -1948,7 +2035,7 @@
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C54" s="1">
-        <v>14.214570999999999</v>
+        <v>109.24320899999999</v>
       </c>
       <c r="F54" s="1">
         <v>254.184471</v>
@@ -1956,7 +2043,7 @@
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C55" s="1">
-        <v>88.980574000000004</v>
+        <v>100.336516</v>
       </c>
       <c r="F55" s="1">
         <v>270.29332399999998</v>
@@ -1964,7 +2051,7 @@
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C56" s="1">
-        <v>151.30196599999999</v>
+        <v>34.427705000000003</v>
       </c>
       <c r="F56" s="1">
         <v>323.48178000000001</v>
@@ -1972,7 +2059,7 @@
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C57" s="1">
-        <v>182.53677400000001</v>
+        <v>94.844695999999999</v>
       </c>
       <c r="F57" s="1">
         <v>228.86275699999999</v>
@@ -1980,7 +2067,7 @@
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C58" s="1">
-        <v>11.515772</v>
+        <v>2.4864999999999999</v>
       </c>
       <c r="F58" s="1">
         <v>138.84008499999999</v>
@@ -1988,7 +2075,7 @@
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C59" s="1">
-        <v>1.591278</v>
+        <v>75.028715000000005</v>
       </c>
       <c r="F59" s="1">
         <v>341.05988400000001</v>
@@ -1996,7 +2083,7 @@
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C60" s="1">
-        <v>22.497171999999999</v>
+        <v>92.75121</v>
       </c>
       <c r="F60" s="1">
         <v>265.65097300000002</v>
@@ -2004,7 +2091,7 @@
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C61" s="1">
-        <v>141.62195</v>
+        <v>182.52613099999999</v>
       </c>
       <c r="F61" s="1">
         <v>174.638904</v>
@@ -2012,7 +2099,7 @@
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C62" s="1">
-        <v>212.022918</v>
+        <v>34.332909999999998</v>
       </c>
       <c r="F62" s="1">
         <v>111.177622</v>
@@ -2020,7 +2107,7 @@
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C63" s="1">
-        <v>79.437847000000005</v>
+        <v>22.305606999999998</v>
       </c>
       <c r="F63" s="1">
         <v>246.66624400000001</v>
@@ -2028,7 +2115,7 @@
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C64" s="1">
-        <v>105.72016600000001</v>
+        <v>39.602812999999998</v>
       </c>
       <c r="F64" s="1">
         <v>316.01929699999999</v>
@@ -2036,7 +2123,7 @@
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C65" s="1">
-        <v>73.016433000000006</v>
+        <v>52.204116999999997</v>
       </c>
       <c r="F65" s="1">
         <v>242.18806699999999</v>
@@ -2044,7 +2131,7 @@
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C66" s="1">
-        <v>213.51305600000001</v>
+        <v>152.71075300000001</v>
       </c>
       <c r="F66" s="1">
         <v>324.15372400000001</v>
@@ -2052,7 +2139,7 @@
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C67" s="1">
-        <v>12.247332999999999</v>
+        <v>67.354322999999994</v>
       </c>
       <c r="F67" s="1">
         <v>334.04348700000003</v>
@@ -2060,7 +2147,7 @@
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C68" s="1">
-        <v>221.607911</v>
+        <v>90.486632999999998</v>
       </c>
       <c r="F68" s="1">
         <v>421.66314</v>
@@ -2068,7 +2155,7 @@
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C69" s="1">
-        <v>257.19677899999999</v>
+        <v>4.4087009999999998</v>
       </c>
       <c r="F69" s="1">
         <v>379.602709</v>
@@ -2076,7 +2163,7 @@
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C70" s="1">
-        <v>164.92174600000001</v>
+        <v>197.59751399999999</v>
       </c>
       <c r="F70" s="1">
         <v>270.03387700000002</v>
@@ -2084,7 +2171,7 @@
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C71" s="1">
-        <v>74.953810000000004</v>
+        <v>122.105531</v>
       </c>
       <c r="F71" s="1">
         <v>301.204003</v>
@@ -2092,7 +2179,7 @@
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C72" s="1">
-        <v>242.40723600000001</v>
+        <v>137.523517</v>
       </c>
       <c r="F72" s="1">
         <v>340.72620000000001</v>
@@ -2100,7 +2187,7 @@
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C73" s="1">
-        <v>272.907375</v>
+        <v>25.721999</v>
       </c>
       <c r="F73" s="1">
         <v>178.08257900000001</v>
@@ -2108,7 +2195,7 @@
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C74" s="1">
-        <v>49.648094</v>
+        <v>354.03517399999998</v>
       </c>
       <c r="F74" s="1">
         <v>216.59512100000001</v>
@@ -2116,7 +2203,7 @@
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C75" s="1">
-        <v>84.878213000000002</v>
+        <v>219.52115800000001</v>
       </c>
       <c r="F75" s="1">
         <v>291.59285199999999</v>
@@ -2124,7 +2211,7 @@
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C76" s="1">
-        <v>142.75420399999999</v>
+        <v>49.124619000000003</v>
       </c>
       <c r="F76" s="1">
         <v>335.05869100000001</v>
@@ -2132,7 +2219,7 @@
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C77" s="1">
-        <v>101.29188000000001</v>
+        <v>269.32563699999997</v>
       </c>
       <c r="F77" s="1">
         <v>360.834588</v>
@@ -2140,7 +2227,7 @@
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C78" s="1">
-        <v>100.697361</v>
+        <v>48.271422999999999</v>
       </c>
       <c r="F78" s="1">
         <v>250.75783100000001</v>
@@ -2148,7 +2235,7 @@
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C79" s="1">
-        <v>11.248621</v>
+        <v>70.464414000000005</v>
       </c>
       <c r="F79" s="1">
         <v>184.42745199999999</v>
@@ -2156,7 +2243,7 @@
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C80" s="1">
-        <v>107.99018100000001</v>
+        <v>83.494001999999995</v>
       </c>
       <c r="F80" s="1">
         <v>263.16324900000001</v>
@@ -2164,7 +2251,7 @@
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C81" s="1">
-        <v>26.504963</v>
+        <v>35.495311999999998</v>
       </c>
       <c r="F81" s="1">
         <v>992.49164800000005</v>
@@ -2172,7 +2259,7 @@
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C82" s="1">
-        <v>10.079395</v>
+        <v>100.78412400000001</v>
       </c>
       <c r="F82" s="1">
         <v>181.47258199999999</v>
@@ -2180,7 +2267,7 @@
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C83" s="1">
-        <v>125.16450399999999</v>
+        <v>19.046806</v>
       </c>
       <c r="F83" s="1">
         <v>264.411967</v>
@@ -2188,7 +2275,7 @@
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C84" s="1">
-        <v>50.980071000000002</v>
+        <v>119.62922500000001</v>
       </c>
       <c r="F84" s="1">
         <v>375.11273799999998</v>
@@ -2196,7 +2283,7 @@
     </row>
     <row r="85" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C85" s="1">
-        <v>75.458844999999997</v>
+        <v>428.07271200000002</v>
       </c>
       <c r="F85" s="1">
         <v>417.73812099999998</v>
@@ -2204,7 +2291,7 @@
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C86" s="1">
-        <v>373.56803200000002</v>
+        <v>46.778733000000003</v>
       </c>
       <c r="F86" s="1">
         <v>147.28743800000001</v>
@@ -2212,7 +2299,7 @@
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C87" s="1">
-        <v>46.228282</v>
+        <v>140.19809900000001</v>
       </c>
       <c r="F87" s="1">
         <v>183.72757200000001</v>
@@ -2220,7 +2307,7 @@
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" s="1">
-        <v>885.84030099999995</v>
+        <v>67.280837000000005</v>
       </c>
       <c r="F88" s="1">
         <v>181.97882100000001</v>
@@ -2228,7 +2315,7 @@
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C89" s="1">
-        <v>150.06518800000001</v>
+        <v>63.141834000000003</v>
       </c>
       <c r="F89" s="1">
         <v>123.463576</v>
@@ -2236,7 +2323,7 @@
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C90" s="1">
-        <v>206.93074300000001</v>
+        <v>11.677039000000001</v>
       </c>
       <c r="F90" s="1">
         <v>154.46245999999999</v>
@@ -2244,7 +2331,7 @@
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C91" s="1">
-        <v>140.97378800000001</v>
+        <v>154.36384799999999</v>
       </c>
       <c r="F91" s="1">
         <v>389.79014100000001</v>
@@ -2252,7 +2339,7 @@
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C92" s="1">
-        <v>13.18491</v>
+        <v>167.225651</v>
       </c>
       <c r="F92" s="1">
         <v>413.17756500000002</v>
@@ -2260,7 +2347,7 @@
     </row>
     <row r="93" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C93" s="1">
-        <v>239.14221800000001</v>
+        <v>162.38195400000001</v>
       </c>
       <c r="F93" s="1">
         <v>337.65977299999997</v>
@@ -2268,7 +2355,7 @@
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C94" s="1">
-        <v>128.82283000000001</v>
+        <v>25.706403000000002</v>
       </c>
       <c r="F94" s="1">
         <v>381.82409000000001</v>
@@ -2276,7 +2363,7 @@
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C95" s="1">
-        <v>153.32668699999999</v>
+        <v>84.043467000000007</v>
       </c>
       <c r="F95" s="1">
         <v>153.07201900000001</v>
@@ -2284,7 +2371,7 @@
     </row>
     <row r="96" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C96" s="1">
-        <v>98.413523999999995</v>
+        <v>154.35294300000001</v>
       </c>
       <c r="F96" s="1">
         <v>249.132147</v>
@@ -2292,7 +2379,7 @@
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C97" s="1">
-        <v>76.255419000000003</v>
+        <v>55.253841999999999</v>
       </c>
       <c r="F97" s="1">
         <v>500.262337</v>
@@ -2300,7 +2387,7 @@
     </row>
     <row r="98" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C98" s="1">
-        <v>94.133804999999995</v>
+        <v>154.10551899999999</v>
       </c>
       <c r="F98" s="1">
         <v>480.64124099999998</v>
@@ -2308,7 +2395,7 @@
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C99" s="1">
-        <v>229.77990399999999</v>
+        <v>119.052325</v>
       </c>
       <c r="F99" s="1">
         <v>231.66653400000001</v>
@@ -2316,7 +2403,7 @@
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C100" s="1">
-        <v>247.00486100000001</v>
+        <v>93.002403000000001</v>
       </c>
       <c r="F100" s="1">
         <v>332.805226</v>
@@ -2324,7 +2411,7 @@
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C101" s="1">
-        <v>458.249101</v>
+        <v>113.451914</v>
       </c>
       <c r="F101" s="1">
         <v>185.55849699999999</v>
@@ -2332,7 +2419,7 @@
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C102" s="1">
-        <v>62.913960000000003</v>
+        <v>274.73750200000001</v>
       </c>
       <c r="F102" s="1">
         <v>199.94978599999999</v>
@@ -2340,7 +2427,7 @@
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C103" s="1">
-        <v>17.769185</v>
+        <v>27.313300999999999</v>
       </c>
       <c r="F103" s="1">
         <v>296.60464200000001</v>
@@ -2348,7 +2435,7 @@
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C104" s="1">
-        <v>83.980046000000002</v>
+        <v>45.799416999999998</v>
       </c>
       <c r="F104" s="1">
         <v>225.72413900000001</v>
@@ -2356,7 +2443,7 @@
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C105" s="1">
-        <v>88.808040000000005</v>
+        <v>17.404906</v>
       </c>
       <c r="F105" s="1">
         <v>279.05048799999997</v>
@@ -2364,7 +2451,7 @@
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C106" s="1">
-        <v>20.440418999999999</v>
+        <v>18.193701999999998</v>
       </c>
       <c r="F106" s="1">
         <v>244.45578599999999</v>
@@ -2372,7 +2459,7 @@
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C107" s="1">
-        <v>8.4326659999999993</v>
+        <v>47.889814000000001</v>
       </c>
       <c r="F107" s="1">
         <v>205.81721300000001</v>
@@ -2380,7 +2467,7 @@
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C108" s="1">
-        <v>8.355537</v>
+        <v>9.9362010000000005</v>
       </c>
       <c r="F108" s="1">
         <v>477.32026500000001</v>
@@ -2388,7 +2475,7 @@
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C109" s="1">
-        <v>87.473427999999998</v>
+        <v>40.955706999999997</v>
       </c>
       <c r="F109" s="1">
         <v>450.737167</v>
@@ -2396,7 +2483,7 @@
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C110" s="1">
-        <v>67.995665000000002</v>
+        <v>93.984127999999998</v>
       </c>
       <c r="F110" s="1">
         <v>133.883678</v>
@@ -2404,7 +2491,7 @@
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C111" s="1">
-        <v>85.86327</v>
+        <v>230.83404100000001</v>
       </c>
       <c r="F111" s="1">
         <v>240.97975199999999</v>
@@ -2412,7 +2499,7 @@
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C112" s="1">
-        <v>102.41871</v>
+        <v>79.354203999999996</v>
       </c>
       <c r="F112" s="1">
         <v>344.46748100000002</v>
@@ -2420,7 +2507,7 @@
     </row>
     <row r="113" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C113" s="1">
-        <v>31.865361</v>
+        <v>105.61591300000001</v>
       </c>
       <c r="F113" s="1">
         <v>272.99954400000001</v>
@@ -2428,7 +2515,7 @@
     </row>
     <row r="114" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C114" s="1">
-        <v>50.715525999999997</v>
+        <v>157.701424</v>
       </c>
       <c r="F114" s="1">
         <v>201.51666599999999</v>
@@ -2436,7 +2523,7 @@
     </row>
     <row r="115" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C115" s="1">
-        <v>59.439869999999999</v>
+        <v>3.9518</v>
       </c>
       <c r="F115" s="1">
         <v>296.62879400000003</v>
@@ -2444,7 +2531,7 @@
     </row>
     <row r="116" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C116" s="1">
-        <v>62.791584</v>
+        <v>163.575413</v>
       </c>
       <c r="F116" s="1">
         <v>495.27131100000003</v>
@@ -2452,7 +2539,7 @@
     </row>
     <row r="117" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C117" s="1">
-        <v>82.150096000000005</v>
+        <v>60.827976999999997</v>
       </c>
       <c r="F117" s="1">
         <v>275.33469100000002</v>
@@ -2460,7 +2547,7 @@
     </row>
     <row r="118" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C118" s="1">
-        <v>377.26592799999997</v>
+        <v>90.806218999999999</v>
       </c>
       <c r="F118" s="1">
         <v>371.07413700000001</v>
@@ -2468,7 +2555,7 @@
     </row>
     <row r="119" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C119" s="1">
-        <v>406.625315</v>
+        <v>33.705117000000001</v>
       </c>
       <c r="F119" s="1">
         <v>263.06450899999999</v>
@@ -2476,7 +2563,7 @@
     </row>
     <row r="120" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C120" s="1">
-        <v>100.492698</v>
+        <v>23.329505999999999</v>
       </c>
       <c r="F120" s="1">
         <v>358.72747099999998</v>
@@ -2484,7 +2571,7 @@
     </row>
     <row r="121" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C121" s="1">
-        <v>66.349676000000002</v>
+        <v>178.523504</v>
       </c>
       <c r="F121" s="1">
         <v>253.64488499999999</v>
@@ -2492,7 +2579,7 @@
     </row>
     <row r="122" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C122" s="1">
-        <v>73.317097000000004</v>
+        <v>99.203309000000004</v>
       </c>
       <c r="F122" s="1">
         <v>201.923439</v>
@@ -2500,7 +2587,7 @@
     </row>
     <row r="123" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C123" s="1">
-        <v>84.613101999999998</v>
+        <v>25.102499000000002</v>
       </c>
       <c r="F123" s="1">
         <v>163.99395699999999</v>
@@ -2508,7 +2595,7 @@
     </row>
     <row r="124" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C124" s="1">
-        <v>156.87094099999999</v>
+        <v>115.63291599999999</v>
       </c>
       <c r="F124" s="1">
         <v>328.47298799999999</v>
@@ -2516,7 +2603,7 @@
     </row>
     <row r="125" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C125" s="1">
-        <v>13.413942</v>
+        <v>296.963504</v>
       </c>
       <c r="F125" s="1">
         <v>69.729194000000007</v>
@@ -2524,7 +2611,7 @@
     </row>
     <row r="126" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C126" s="1">
-        <v>11.710501000000001</v>
+        <v>214.23239100000001</v>
       </c>
       <c r="F126" s="1">
         <v>322.07892700000002</v>
@@ -2532,7 +2619,7 @@
     </row>
     <row r="127" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C127" s="1">
-        <v>77.507221000000001</v>
+        <v>61.388308000000002</v>
       </c>
       <c r="F127" s="1">
         <v>211.107641</v>
@@ -2540,7 +2627,7 @@
     </row>
     <row r="128" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C128" s="1">
-        <v>76.024349999999998</v>
+        <v>204.567306</v>
       </c>
       <c r="F128" s="1">
         <v>226.94239899999999</v>
@@ -2548,7 +2635,7 @@
     </row>
     <row r="129" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C129" s="1">
-        <v>42.997985999999997</v>
+        <v>55.796880000000002</v>
       </c>
       <c r="F129" s="1">
         <v>298.41189800000001</v>
@@ -2556,7 +2643,7 @@
     </row>
     <row r="130" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C130" s="1">
-        <v>39.187252999999998</v>
+        <v>83.520527999999999</v>
       </c>
       <c r="F130" s="1">
         <v>319.72611000000001</v>
@@ -2564,7 +2651,7 @@
     </row>
     <row r="131" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C131" s="1">
-        <v>58.149337000000003</v>
+        <v>188.91844499999999</v>
       </c>
       <c r="F131" s="1">
         <v>265.29162000000002</v>
@@ -2572,7 +2659,7 @@
     </row>
     <row r="132" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C132" s="1">
-        <v>114.850928</v>
+        <v>16.629498999999999</v>
       </c>
       <c r="F132" s="1">
         <v>217.17701</v>
@@ -2580,7 +2667,7 @@
     </row>
     <row r="133" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C133" s="1">
-        <v>145.699984</v>
+        <v>21.583752</v>
       </c>
       <c r="F133" s="1">
         <v>362.65866599999998</v>
@@ -2588,7 +2675,7 @@
     </row>
     <row r="134" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C134" s="1">
-        <v>3.8672520000000001</v>
+        <v>35.016319000000003</v>
       </c>
       <c r="F134" s="1">
         <v>278.73262499999998</v>
@@ -2596,7 +2683,7 @@
     </row>
     <row r="135" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C135" s="1">
-        <v>18.485512</v>
+        <v>61.945131000000003</v>
       </c>
       <c r="F135" s="1">
         <v>195.43145200000001</v>
@@ -2604,7 +2691,7 @@
     </row>
     <row r="136" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C136" s="1">
-        <v>220.80864</v>
+        <v>96.429326000000003</v>
       </c>
       <c r="F136" s="1">
         <v>218.024475</v>
@@ -2612,7 +2699,7 @@
     </row>
     <row r="137" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C137" s="1">
-        <v>33.457802999999998</v>
+        <v>54.450800999999998</v>
       </c>
       <c r="F137" s="1">
         <v>279.67837900000001</v>
@@ -2620,7 +2707,7 @@
     </row>
     <row r="138" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C138" s="1">
-        <v>146.695525</v>
+        <v>48.113804000000002</v>
       </c>
       <c r="F138" s="1">
         <v>296.61825099999999</v>
@@ -2628,7 +2715,7 @@
     </row>
     <row r="139" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C139" s="1">
-        <v>43.445858000000001</v>
+        <v>72.630221000000006</v>
       </c>
       <c r="F139" s="1">
         <v>392.464313</v>
@@ -2636,7 +2723,7 @@
     </row>
     <row r="140" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C140" s="1">
-        <v>25.179499</v>
+        <v>52.326104999999998</v>
       </c>
       <c r="F140" s="1">
         <v>226.53227000000001</v>
@@ -2644,7 +2731,7 @@
     </row>
     <row r="141" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C141" s="1">
-        <v>226.36260799999999</v>
+        <v>20.925598000000001</v>
       </c>
       <c r="F141" s="1">
         <v>245.34950900000001</v>
@@ -2652,7 +2739,7 @@
     </row>
     <row r="142" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C142" s="1">
-        <v>40.150731999999998</v>
+        <v>183.617209</v>
       </c>
       <c r="F142" s="1">
         <v>479.80807600000003</v>
@@ -2660,7 +2747,7 @@
     </row>
     <row r="143" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C143" s="1">
-        <v>18.163647000000001</v>
+        <v>40.866219999999998</v>
       </c>
       <c r="F143" s="1">
         <v>320.87656299999998</v>
@@ -2668,7 +2755,7 @@
     </row>
     <row r="144" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C144" s="1">
-        <v>101.17142800000001</v>
+        <v>37.944916999999997</v>
       </c>
       <c r="F144" s="1">
         <v>462.070651</v>
@@ -2676,7 +2763,7 @@
     </row>
     <row r="145" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C145" s="1">
-        <v>63.429082000000001</v>
+        <v>24.019404999999999</v>
       </c>
       <c r="F145" s="1">
         <v>342.641142</v>
@@ -2684,7 +2771,7 @@
     </row>
     <row r="146" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C146" s="1">
-        <v>56.444858000000004</v>
+        <v>116.750823</v>
       </c>
       <c r="F146" s="1">
         <v>443.30903799999999</v>
@@ -2692,7 +2779,7 @@
     </row>
     <row r="147" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C147" s="1">
-        <v>28.172332000000001</v>
+        <v>37.997608</v>
       </c>
       <c r="F147" s="1">
         <v>432.611965</v>
@@ -2700,7 +2787,7 @@
     </row>
     <row r="148" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C148" s="1">
-        <v>4.9654509999999998</v>
+        <v>8.5417000000000005</v>
       </c>
       <c r="F148" s="1">
         <v>288.53789999999998</v>
@@ -2708,7 +2795,7 @@
     </row>
     <row r="149" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C149" s="1">
-        <v>177.07753</v>
+        <v>54.397145000000002</v>
       </c>
       <c r="F149" s="1">
         <v>70.466008000000002</v>
@@ -2716,7 +2803,7 @@
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C150" s="1">
-        <v>77.767161999999999</v>
+        <v>131.481864</v>
       </c>
       <c r="F150" s="1">
         <v>256.95496000000003</v>
@@ -2724,7 +2811,7 @@
     </row>
     <row r="151" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C151" s="1">
-        <v>92.447012000000001</v>
+        <v>5.8723999999999998</v>
       </c>
       <c r="F151" s="1">
         <v>254.58699999999999</v>
@@ -2732,7 +2819,7 @@
     </row>
     <row r="152" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C152" s="1">
-        <v>326.34818999999999</v>
+        <v>95.441305</v>
       </c>
       <c r="F152" s="1">
         <v>251.063546</v>
@@ -2740,7 +2827,7 @@
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C153" s="1">
-        <v>80.332570000000004</v>
+        <v>25.569203000000002</v>
       </c>
       <c r="F153" s="1">
         <v>181.215023</v>
@@ -2748,7 +2835,7 @@
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C154" s="1">
-        <v>95.256159999999994</v>
+        <v>243.16862399999999</v>
       </c>
       <c r="F154" s="1">
         <v>250.01202900000001</v>
@@ -2756,7 +2843,7 @@
     </row>
     <row r="155" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C155" s="1">
-        <v>101.12153600000001</v>
+        <v>29.369304</v>
       </c>
       <c r="F155" s="1">
         <v>290.99572999999998</v>
@@ -2764,7 +2851,7 @@
     </row>
     <row r="156" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C156" s="1">
-        <v>219.020644</v>
+        <v>131.14221699999999</v>
       </c>
       <c r="F156" s="1">
         <v>226.42253199999999</v>
@@ -2772,7 +2859,7 @@
     </row>
     <row r="157" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C157" s="1">
-        <v>61.766091000000003</v>
+        <v>84.962710999999999</v>
       </c>
       <c r="F157" s="1">
         <v>205.000316</v>
@@ -2780,7 +2867,7 @@
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C158" s="1">
-        <v>81.999671000000006</v>
+        <v>35.606651999999997</v>
       </c>
       <c r="F158" s="1">
         <v>159.893339</v>
@@ -2788,7 +2875,7 @@
     </row>
     <row r="159" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C159" s="1">
-        <v>23.722010999999998</v>
+        <v>89.451314999999994</v>
       </c>
       <c r="F159" s="1">
         <v>196.61783399999999</v>
@@ -2796,7 +2883,7 @@
     </row>
     <row r="160" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C160" s="1">
-        <v>124.077699</v>
+        <v>154.75241</v>
       </c>
       <c r="F160" s="1">
         <v>348.94189999999998</v>
@@ -2804,7 +2891,7 @@
     </row>
     <row r="161" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C161" s="1">
-        <v>155.269868</v>
+        <v>156.15386799999999</v>
       </c>
       <c r="F161" s="1">
         <v>526.72490600000003</v>
@@ -2812,7 +2899,7 @@
     </row>
     <row r="162" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C162" s="1">
-        <v>98.198441000000003</v>
+        <v>92.215320000000006</v>
       </c>
       <c r="F162" s="1">
         <v>221.03537600000001</v>
@@ -2820,7 +2907,7 @@
     </row>
     <row r="163" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C163" s="1">
-        <v>48.878141999999997</v>
+        <v>14.459102</v>
       </c>
       <c r="F163" s="1">
         <v>370.65513399999998</v>
@@ -2828,7 +2915,7 @@
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C164" s="1">
-        <v>37.906449000000002</v>
+        <v>26.900003999999999</v>
       </c>
       <c r="F164" s="1">
         <v>164.845945</v>
@@ -2836,7 +2923,7 @@
     </row>
     <row r="165" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C165" s="1">
-        <v>139.80186699999999</v>
+        <v>39.002403999999999</v>
       </c>
       <c r="F165" s="1">
         <v>405.65650900000003</v>
@@ -2844,7 +2931,7 @@
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C166" s="1">
-        <v>141.064303</v>
+        <v>325.55557099999999</v>
       </c>
       <c r="F166" s="1">
         <v>298.91337600000003</v>
@@ -2852,7 +2939,7 @@
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C167" s="1">
-        <v>13.17634</v>
+        <v>3.3408000000000002</v>
       </c>
       <c r="F167" s="1">
         <v>516.72090500000002</v>
@@ -2860,7 +2947,7 @@
     </row>
     <row r="168" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C168" s="1">
-        <v>18.59085</v>
+        <v>251.17550800000001</v>
       </c>
       <c r="F168" s="1">
         <v>157.73048800000001</v>
@@ -2868,7 +2955,7 @@
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C169" s="1">
-        <v>31.361785999999999</v>
+        <v>1.2081010000000001</v>
       </c>
       <c r="F169" s="1">
         <v>357.94362799999999</v>
@@ -2876,7 +2963,7 @@
     </row>
     <row r="170" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C170" s="1">
-        <v>357.92156999999997</v>
+        <v>137.303324</v>
       </c>
       <c r="F170" s="1">
         <v>397.67623400000002</v>
@@ -2884,7 +2971,7 @@
     </row>
     <row r="171" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C171" s="1">
-        <v>220.71282099999999</v>
+        <v>3.4184999999999999</v>
       </c>
       <c r="F171" s="1">
         <v>146.81394800000001</v>
@@ -2892,7 +2979,7 @@
     </row>
     <row r="172" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C172" s="1">
-        <v>0.14036399999999999</v>
+        <v>60.315626000000002</v>
       </c>
       <c r="F172" s="1">
         <v>288.50435700000003</v>
@@ -2900,7 +2987,7 @@
     </row>
     <row r="173" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C173" s="1">
-        <v>66.387067000000002</v>
+        <v>12.192000999999999</v>
       </c>
       <c r="F173" s="1">
         <v>269.10320899999999</v>
@@ -2908,7 +2995,7 @@
     </row>
     <row r="174" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C174" s="1">
-        <v>59.649042999999999</v>
+        <v>29.209828999999999</v>
       </c>
       <c r="F174" s="1">
         <v>197.376577</v>
@@ -2916,7 +3003,7 @@
     </row>
     <row r="175" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C175" s="1">
-        <v>107.38088399999999</v>
+        <v>34.998185999999997</v>
       </c>
       <c r="F175" s="1">
         <v>294.21914800000002</v>
@@ -2924,7 +3011,7 @@
     </row>
     <row r="176" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C176" s="1">
-        <v>5.2753709999999998</v>
+        <v>214.358846</v>
       </c>
       <c r="F176" s="1">
         <v>263.78592800000001</v>
@@ -2932,7 +3019,7 @@
     </row>
     <row r="177" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C177" s="1">
-        <v>65.200112000000004</v>
+        <v>19.645192999999999</v>
       </c>
       <c r="F177" s="1">
         <v>385.146612</v>
@@ -2940,7 +3027,7 @@
     </row>
     <row r="178" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C178" s="1">
-        <v>111.42179400000001</v>
+        <v>140.182694</v>
       </c>
       <c r="F178" s="1">
         <v>313.59743800000001</v>
@@ -2948,7 +3035,7 @@
     </row>
     <row r="179" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C179" s="1">
-        <v>43.405259000000001</v>
+        <v>235.102146</v>
       </c>
       <c r="F179" s="1">
         <v>450.94314400000002</v>
@@ -2956,7 +3043,7 @@
     </row>
     <row r="180" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C180" s="1">
-        <v>107.40193499999999</v>
+        <v>45.453904999999999</v>
       </c>
       <c r="F180" s="1">
         <v>294.09659399999998</v>
@@ -2964,7 +3051,7 @@
     </row>
     <row r="181" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C181" s="1">
-        <v>162.45958099999999</v>
+        <v>181.76612499999999</v>
       </c>
       <c r="F181" s="1">
         <v>500.60762899999997</v>
@@ -2972,7 +3059,7 @@
     </row>
     <row r="182" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C182" s="1">
-        <v>24.526741000000001</v>
+        <v>247.463258</v>
       </c>
       <c r="F182" s="1">
         <v>113.233042</v>
@@ -2980,7 +3067,7 @@
     </row>
     <row r="183" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C183" s="1">
-        <v>4.1847130000000003</v>
+        <v>100.340418</v>
       </c>
       <c r="F183" s="1">
         <v>324.36593800000003</v>
@@ -2988,7 +3075,7 @@
     </row>
     <row r="184" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C184" s="1">
-        <v>141.156712</v>
+        <v>109.338319</v>
       </c>
       <c r="F184" s="1">
         <v>353.90953500000001</v>
@@ -2996,7 +3083,7 @@
     </row>
     <row r="185" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C185" s="1">
-        <v>55.915657000000003</v>
+        <v>42.435507000000001</v>
       </c>
       <c r="F185" s="1">
         <v>200.954354</v>
@@ -3004,7 +3091,7 @@
     </row>
     <row r="186" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C186" s="1">
-        <v>48.228262999999998</v>
+        <v>225.654438</v>
       </c>
       <c r="F186" s="1">
         <v>199.077945</v>
@@ -3012,7 +3099,7 @@
     </row>
     <row r="187" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C187" s="1">
-        <v>2.3531770000000001</v>
+        <v>84.288815</v>
       </c>
       <c r="F187" s="1">
         <v>189.13161700000001</v>
@@ -3020,7 +3107,7 @@
     </row>
     <row r="188" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C188" s="1">
-        <v>19.357794999999999</v>
+        <v>26.783003999999998</v>
       </c>
       <c r="F188" s="1">
         <v>517.35128799999995</v>
@@ -3028,7 +3115,7 @@
     </row>
     <row r="189" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C189" s="1">
-        <v>42.82038</v>
+        <v>118.604315</v>
       </c>
       <c r="F189" s="1">
         <v>203.00179499999999</v>
@@ -3036,7 +3123,7 @@
     </row>
     <row r="190" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C190" s="1">
-        <v>17.563545999999999</v>
+        <v>130.10850099999999</v>
       </c>
       <c r="F190" s="1">
         <v>385.43466799999999</v>
@@ -3044,7 +3131,7 @@
     </row>
     <row r="191" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C191" s="1">
-        <v>177.79840999999999</v>
+        <v>54.890501999999998</v>
       </c>
       <c r="F191" s="1">
         <v>139.61221499999999</v>
@@ -3052,7 +3139,7 @@
     </row>
     <row r="192" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C192" s="1">
-        <v>77.106414000000001</v>
+        <v>14.291698</v>
       </c>
       <c r="F192" s="1">
         <v>112.896895</v>
@@ -3060,7 +3147,7 @@
     </row>
     <row r="193" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C193" s="1">
-        <v>352.12376399999999</v>
+        <v>94.586701000000005</v>
       </c>
       <c r="F193" s="1">
         <v>237.222677</v>
@@ -3068,7 +3155,7 @@
     </row>
     <row r="194" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C194" s="1">
-        <v>253.607764</v>
+        <v>61.061802999999998</v>
       </c>
       <c r="F194" s="1">
         <v>254.21345299999999</v>
@@ -3076,7 +3163,7 @@
     </row>
     <row r="195" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C195" s="1">
-        <v>3.5880610000000002</v>
+        <v>264.31662699999998</v>
       </c>
       <c r="F195" s="1">
         <v>172.91710599999999</v>
@@ -3084,7 +3171,7 @@
     </row>
     <row r="196" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C196" s="1">
-        <v>122.76665300000001</v>
+        <v>67.152006</v>
       </c>
       <c r="F196" s="1">
         <v>571.21227299999998</v>
@@ -3092,7 +3179,7 @@
     </row>
     <row r="197" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C197" s="1">
-        <v>24.972529000000002</v>
+        <v>105.80681199999999</v>
       </c>
       <c r="F197" s="1">
         <v>215.200514</v>
@@ -3100,7 +3187,7 @@
     </row>
     <row r="198" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C198" s="1">
-        <v>119.62988199999999</v>
+        <v>169.259713</v>
       </c>
       <c r="F198" s="1">
         <v>512.99201200000005</v>
@@ -3108,7 +3195,7 @@
     </row>
     <row r="199" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C199" s="1">
-        <v>12.872457000000001</v>
+        <v>80.913511</v>
       </c>
       <c r="F199" s="1">
         <v>192.98369600000001</v>
@@ -3116,7 +3203,7 @@
     </row>
     <row r="200" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C200" s="1">
-        <v>456.88598200000001</v>
+        <v>183.60622799999999</v>
       </c>
       <c r="F200" s="1">
         <v>188.23911899999999</v>
@@ -3124,7 +3211,7 @@
     </row>
     <row r="201" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C201" s="1">
-        <v>96.465553</v>
+        <v>112.638409</v>
       </c>
       <c r="F201" s="1">
         <v>190.999414</v>
@@ -3132,7 +3219,7 @@
     </row>
     <row r="202" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C202" s="1">
-        <v>21.662606</v>
+        <v>5.5998999999999999</v>
       </c>
       <c r="F202" s="1">
         <v>227.45056199999999</v>
@@ -3140,7 +3227,7 @@
     </row>
     <row r="203" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C203" s="1">
-        <v>233.971991</v>
+        <v>527.50090399999999</v>
       </c>
       <c r="F203" s="1">
         <v>350.51942400000001</v>
@@ -3148,7 +3235,7 @@
     </row>
     <row r="204" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C204" s="1">
-        <v>7.5426820000000001</v>
+        <v>51.958702000000002</v>
       </c>
       <c r="F204" s="1">
         <v>249.46060199999999</v>
@@ -3156,7 +3243,7 @@
     </row>
     <row r="205" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C205" s="1">
-        <v>20.586789</v>
+        <v>45.282398999999998</v>
       </c>
       <c r="F205" s="1">
         <v>156.4999</v>
@@ -3164,7 +3251,7 @@
     </row>
     <row r="206" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C206" s="1">
-        <v>2.6775730000000002</v>
+        <v>33.475606999999997</v>
       </c>
       <c r="F206" s="1">
         <v>441.29271999999997</v>
@@ -3172,7 +3259,7 @@
     </row>
     <row r="207" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C207" s="1">
-        <v>39.841923999999999</v>
+        <v>116.485947</v>
       </c>
       <c r="F207" s="1">
         <v>272.65055000000001</v>
@@ -3180,7 +3267,7 @@
     </row>
     <row r="208" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C208" s="1">
-        <v>50.539850000000001</v>
+        <v>66.978582000000003</v>
       </c>
       <c r="F208" s="1">
         <v>291.33525600000002</v>
@@ -3188,7 +3275,7 @@
     </row>
     <row r="209" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C209" s="1">
-        <v>5.7319579999999997</v>
+        <v>142.099816</v>
       </c>
       <c r="F209" s="1">
         <v>303.530935</v>
@@ -3207,7 +3294,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC0B1E4-3940-4D24-B51A-8D72DD1958F1}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3228,104 +3317,347 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="D5" s="5">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5">
+        <v>40</v>
+      </c>
+      <c r="G5" s="5">
+        <v>50</v>
+      </c>
+      <c r="H5" s="5">
+        <v>60</v>
+      </c>
+      <c r="I5" s="5">
+        <v>70</v>
+      </c>
+      <c r="J5" s="5">
+        <v>80</v>
+      </c>
+      <c r="K5" s="5">
+        <v>90</v>
+      </c>
+      <c r="L5" s="5">
+        <v>100</v>
+      </c>
+      <c r="M5" s="5">
+        <v>120</v>
+      </c>
+      <c r="N5" s="5">
+        <v>150</v>
+      </c>
+      <c r="O5" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6">
-        <v>30</v>
-      </c>
-      <c r="F5" s="6">
-        <v>40</v>
-      </c>
-      <c r="G5" s="6">
-        <v>50</v>
-      </c>
-      <c r="H5" s="6">
-        <v>60</v>
-      </c>
-      <c r="I5" s="6">
-        <v>70</v>
-      </c>
-      <c r="J5" s="6">
-        <v>80</v>
-      </c>
-      <c r="K5" s="6">
-        <v>90</v>
-      </c>
-      <c r="L5" s="6">
-        <v>100</v>
-      </c>
-      <c r="M5" s="6">
-        <v>120</v>
-      </c>
-      <c r="N5" s="6">
-        <v>150</v>
-      </c>
-      <c r="O5" s="6">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.3</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.35</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0.65</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>0.7</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0.8</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>0.83</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>0.92</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>0.95</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>0.97</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>1</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <v>1</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
-        <v>13</v>
+      <c r="B27" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48113D0-2E19-465F-B537-955B0BDCB680}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <f>AVERAGE(C9:C208)</f>
+        <v>21.1822655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <f>_xlfn.STDEV.S(C9:C208)</f>
+        <v>12.98568440341057</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>30.364530999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8C459E-50BE-4541-BF26-DC91DCC5390E}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CAF787-759A-49CC-8F4A-93698220D9F1}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: Santa busy probability (v1) for 10, 20, 30 and 40 number of elves
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fedebrando\SORTproject\SantaClausProblem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832B5C1F-C609-4A65-B556-D140A644AD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C4BD52-5A93-4523-8901-1AEE1221FD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="43">
   <si>
     <t>Delivery time (v1, v2)</t>
   </si>
@@ -96,16 +96,10 @@
     <t>Samples</t>
   </si>
   <si>
-    <t>Average and Standard Deviation of 200 time measurments for each reasonable (#santa, #elves) pair, 9 reindeer and 3 elves in a consulting group</t>
-  </si>
-  <si>
     <t>Average and Standard Deviation for 200 delivery times in v1 and v2 executed with 9 reindeer, 10 elves and 3 elves in a consulting group</t>
   </si>
   <si>
     <t>Average and Standard Deviation of 200 measurements in v1 with 9 reindeer, 10 elves and 3 elves in a consulting group</t>
-  </si>
-  <si>
-    <t>Each probability point is a statistic probability computed with 200 samples executing v1 with 9 reindeer, 10 elves and 3 elves in a consulting group</t>
   </si>
   <si>
     <t>Information</t>
@@ -163,6 +157,18 @@
   </si>
   <si>
     <t>15,8 Gbyte</t>
+  </si>
+  <si>
+    <t>Each probability point is a statistic probability computed with 200 samples executing v1 with 9 reindeer and 3 elves in a consulting group</t>
+  </si>
+  <si>
+    <t>Santa is free!</t>
+  </si>
+  <si>
+    <t>Santa is busy!</t>
+  </si>
+  <si>
+    <t>Average and Standard Deviation of 200 time measurments in v3 for each reasonable (#santa, #elves) pair, 9 reindeer and 3 elves in a consulting group</t>
   </si>
 </sst>
 </file>
@@ -249,11 +255,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -412,43 +418,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3</c:v>
+                  <c:v>0.17499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1630,18 +1636,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -3292,17 +3298,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC0B1E4-3940-4D24-B51A-8D72DD1958F1}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
@@ -3317,7 +3324,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3369,48 +3376,2859 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <v>0.2</v>
+        <f>COUNTIF(C$27:C$1048576,"Santa is busy!")/COUNTA(C$27:C$1048576)</f>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D6" s="5">
-        <v>0.3</v>
+        <f t="shared" ref="D6:O6" si="0">COUNTIF(D$27:D$1048576,"Santa is busy!")/COUNTA(D$27:D$1048576)</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="E6" s="5">
-        <v>0.35</v>
+        <f t="shared" si="0"/>
+        <v>0.25</v>
       </c>
       <c r="F6" s="5">
-        <v>0.65</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.92</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="M6" s="5">
-        <v>1</v>
-      </c>
-      <c r="N6" s="5">
-        <v>1</v>
-      </c>
-      <c r="O6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="G6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C77" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C78" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C79" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C81" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C83" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C84" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C85" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C86" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C87" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C89" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C91" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C95" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C97" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C98" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C99" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C100" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="112" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C119" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="123" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="128" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="129" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="132" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="133" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="134" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="135" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="136" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="137" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="138" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="139" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="140" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="141" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="143" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="144" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C144" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="145" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C145" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="146" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C146" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="147" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C147" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="148" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C148" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="149" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="150" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C150" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="151" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C151" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="152" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C152" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="153" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="154" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C154" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="155" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C155" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="156" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C156" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="157" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C157" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="158" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C158" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="159" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C159" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C160" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="161" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C161" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="162" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C162" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="163" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C163" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="164" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C164" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="165" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C165" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="166" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C166" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="167" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C167" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="168" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C168" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="169" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C169" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="170" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C170" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="171" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C171" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="172" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C172" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="173" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C173" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="174" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C174" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="175" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C175" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="176" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C176" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="177" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C177" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="178" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C178" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="179" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C179" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="180" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C180" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="181" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C181" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="182" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C182" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="183" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C183" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="184" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C184" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="185" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C185" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="186" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C186" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="187" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C187" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="188" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C188" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="189" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C189" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="190" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C190" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="191" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C191" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="192" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C192" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="193" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C193" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="194" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C194" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="195" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C195" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="196" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C196" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="197" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C197" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="198" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C198" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="199" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C199" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="200" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C200" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="201" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C201" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="202" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C202" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="203" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C203" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="204" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C204" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="205" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C205" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="206" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C206" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="207" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="208" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="209" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C209" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="210" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C210" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="211" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C211" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="212" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C212" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="213" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C213" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="214" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C214" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="215" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C215" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="216" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C216" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="217" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C217" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="218" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C218" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="219" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C219" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="220" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C220" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="221" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C221" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="222" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C222" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="223" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C223" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="224" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C224" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="225" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C225" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="226" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C226" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3424,7 +6242,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3446,7 +6264,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3490,7 +6308,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3510,7 +6328,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3564,93 +6382,93 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="7">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="6"/>
+      <c r="B13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: stats of delivery delay (v3) updated
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr/>
+  <workbookPr codeName="Questa_cartella_di_lavoro" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fedebrando\SORTproject\SantaClausProblem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E81C3D5-CDF3-4646-AC90-379463D55AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1222CD32-BEE9-4471-ADA5-1C3CD7BF31B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery time (v1, v2)" sheetId="1" r:id="rId1"/>
@@ -165,17 +165,17 @@
     <t>Santa is busy!</t>
   </si>
   <si>
-    <t>Average and Standard Deviation of 200 time measurments in v3 for each reasonable (#santa, #elves) pair, 9 reindeer and 3 elves in a consulting group</t>
+    <t>Busy probability</t>
   </si>
   <si>
-    <t>Busy probability</t>
+    <t>Average and Standard Deviation of 200 time measurments in v3 for each reasonable (#elves, #santa) pair, 9 reindeer and 3 elves in a consulting group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +209,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,7 +254,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,6 +267,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1618,9 +1625,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3306,9 +3316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC0B1E4-3940-4D24-B51A-8D72DD1958F1}">
+  <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:O226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
@@ -3381,7 +3392,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5">
         <f>COUNTIF(C$27:C$1048576,"Santa is busy!")/COUNTA(C$27:C$1048576)</f>
@@ -11652,10 +11663,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48113D0-2E19-465F-B537-955B0BDCB680}">
-  <dimension ref="A1:C10"/>
+  <sheetPr codeName="Foglio3"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11686,7 +11698,7 @@
       </c>
       <c r="C6" s="4">
         <f>AVERAGE(C9:C208)</f>
-        <v>21.1822655</v>
+        <v>1.5662098350000004</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -11695,7 +11707,7 @@
       </c>
       <c r="C7" s="4">
         <f>_xlfn.STDEV.S(C9:C208)</f>
-        <v>12.98568440341057</v>
+        <v>3.6989565136699372</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -11703,12 +11715,1002 @@
         <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>30.364530999999999</v>
+        <v>0.89953899999999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
-        <v>12</v>
+        <v>0.56607099999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>0.806921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
+        <v>0.77014800000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>0.72470500000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>0.88613500000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>0.74787800000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>0.87796099999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <v>0.83605700000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>0.71562599999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>0.73613899999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <v>0.91674900000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>0.83732499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <v>0.78798199999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
+        <v>0.81328999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <v>0.68173799999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <v>0.80890799999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <v>0.81513100000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <v>0.87594000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <v>0.72524999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="1">
+        <v>0.76004700000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="1">
+        <v>0.76394399999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="1">
+        <v>0.66620400000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="1">
+        <v>0.90010800000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="1">
+        <v>0.77495000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="1">
+        <v>0.70294500000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <v>0.65187399999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="1">
+        <v>0.700434</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="1">
+        <v>8.2950149999999994</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="1">
+        <v>0.75334400000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="1">
+        <v>0.72122299999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="1">
+        <v>0.97014900000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="1">
+        <v>0.71394500000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="1">
+        <v>0.831287</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="1">
+        <v>0.86885500000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="1">
+        <v>0.77392799999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="1">
+        <v>0.77515999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <v>16.484152000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="1">
+        <v>0.29975000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="1">
+        <v>0.77457699999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="1">
+        <v>0.97766900000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="1">
+        <v>0.96605700000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="1">
+        <v>0.72944299999999995</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="1">
+        <v>0.86923700000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="1">
+        <v>0.74339299999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="1">
+        <v>0.81727099999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="1">
+        <v>0.94900799999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="1">
+        <v>0.76571199999999995</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="1">
+        <v>0.91015999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="1">
+        <v>0.55913100000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="1">
+        <v>0.79149899999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="1">
+        <v>0.84788300000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="1">
+        <v>0.51627000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="1">
+        <v>0.71580600000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C63" s="1">
+        <v>0.85259799999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C64" s="1">
+        <v>0.80904399999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="1">
+        <v>0.92898000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="1">
+        <v>0.70672800000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" s="1">
+        <v>0.70482299999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C68" s="1">
+        <v>0.92903500000000006</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C69" s="1">
+        <v>0.673736</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C70" s="1">
+        <v>0.65914600000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C71" s="1">
+        <v>0.75058899999999995</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C72" s="1">
+        <v>0.56911900000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="1">
+        <v>0.79816600000000004</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" s="1">
+        <v>0.80300400000000005</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C75" s="1">
+        <v>0.78770399999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C76" s="1">
+        <v>0.82439700000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C77" s="1">
+        <v>0.772092</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C78" s="1">
+        <v>0.84594899999999995</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C79" s="1">
+        <v>0.87636400000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C80" s="1">
+        <v>0.70897100000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C81" s="1">
+        <v>0.77209000000000005</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C82" s="1">
+        <v>0.749587</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C83" s="1">
+        <v>0.78146599999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C84" s="1">
+        <v>0.79715499999999995</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C85" s="1">
+        <v>0.83097600000000005</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C86" s="1">
+        <v>0.68577999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C87" s="1">
+        <v>0.89621700000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C88" s="1">
+        <v>0.89743499999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C89" s="1">
+        <v>0.70790600000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C90" s="1">
+        <v>0.84925799999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C91" s="1">
+        <v>25.741855000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C92" s="1">
+        <v>0.75526199999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C93" s="1">
+        <v>0.699631</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C94" s="1">
+        <v>0.68254800000000004</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C95" s="1">
+        <v>5.0868659999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C96" s="1">
+        <v>0.80479500000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" s="1">
+        <v>0.86571900000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C98" s="1">
+        <v>0.87273500000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" s="1">
+        <v>0.436473</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C100" s="1">
+        <v>0.66339499999999996</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C101" s="1">
+        <v>0.75317100000000003</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C102" s="1">
+        <v>0.84028400000000003</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C103" s="1">
+        <v>0.84155000000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C104" s="1">
+        <v>0.718414</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C105" s="1">
+        <v>0.95473799999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C106" s="1">
+        <v>0.76412199999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C107" s="1">
+        <v>0.77709399999999995</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C108" s="1">
+        <v>0.63712899999999995</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C109" s="1">
+        <v>0.69756099999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C110" s="1">
+        <v>0.86540799999999996</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C111" s="1">
+        <v>0.76120399999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C112" s="1">
+        <v>0.76786399999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C113" s="1">
+        <v>0.76592000000000005</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C114" s="1">
+        <v>0.79005199999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C115" s="1">
+        <v>0.890289</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C116" s="1">
+        <v>5.4568620000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C117" s="1">
+        <v>0.83787699999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C118" s="1">
+        <v>0.91625100000000004</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C119" s="1">
+        <v>0.91480499999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C120" s="1">
+        <v>0.73175000000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C121" s="1">
+        <v>1.143367</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C122" s="1">
+        <v>0.49485499999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C123" s="1">
+        <v>0.78622400000000003</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C124" s="1">
+        <v>0.75978599999999996</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C125" s="1">
+        <v>0.86228800000000005</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C126" s="1">
+        <v>0.60887800000000003</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C127" s="1">
+        <v>0.73449500000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C128" s="1">
+        <v>0.684195</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C129" s="1">
+        <v>0.68864800000000004</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C130" s="1">
+        <v>0.71634799999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C131" s="1">
+        <v>0.72391000000000005</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C132" s="1">
+        <v>0.96448199999999995</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C133" s="1">
+        <v>0.82994599999999996</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C134" s="1">
+        <v>0.87391399999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C135" s="1">
+        <v>0.81043799999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C136" s="1">
+        <v>0.79677600000000004</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C137" s="1">
+        <v>6.6014489999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C138" s="1">
+        <v>0.683249</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C139" s="1">
+        <v>0.86094199999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C140" s="1">
+        <v>0.82875500000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C141" s="1">
+        <v>0.88877399999999995</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C142" s="1">
+        <v>0.84404199999999996</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C143" s="1">
+        <v>0.82478200000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C144" s="1">
+        <v>0.71515099999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C145" s="1">
+        <v>0.97732600000000003</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C146" s="1">
+        <v>0.93217899999999998</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C147" s="1">
+        <v>0.79352599999999995</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C148" s="1">
+        <v>26.120366000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C149" s="1">
+        <v>19.862010000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C150" s="1">
+        <v>0.68977999999999995</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C151" s="1">
+        <v>0.64329899999999995</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C152" s="1">
+        <v>0.92438299999999995</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C153" s="1">
+        <v>0.79296900000000003</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C154" s="1">
+        <v>0.76335500000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C155" s="1">
+        <v>0.66445100000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C156" s="1">
+        <v>0.71656299999999995</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C157" s="1">
+        <v>0.84496700000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C158" s="1">
+        <v>0.75405699999999998</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C159" s="1">
+        <v>0.64842100000000003</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C160" s="1">
+        <v>0.74186300000000005</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C161" s="1">
+        <v>0.25758999999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C162" s="1">
+        <v>0.31756699999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C163" s="1">
+        <v>19.760725000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C164" s="1">
+        <v>17.238271000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C165" s="1">
+        <v>0.74012199999999995</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C166" s="1">
+        <v>3.976321</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C167" s="1">
+        <v>0.74709199999999998</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C168" s="1">
+        <v>0.85518300000000003</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C169" s="1">
+        <v>1.0491760000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C170" s="1">
+        <v>0.87124599999999996</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C171" s="1">
+        <v>0.81723699999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C172" s="1">
+        <v>0.60705699999999996</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C173" s="1">
+        <v>0.74136100000000005</v>
+      </c>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C174" s="1">
+        <v>0.74976699999999996</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C175" s="1">
+        <v>1.6947000000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C176" s="1">
+        <v>0.70160299999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C177" s="1">
+        <v>0.80848299999999995</v>
+      </c>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C178" s="1">
+        <v>0.65185099999999996</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C179" s="1">
+        <v>0.72399400000000003</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C180" s="1">
+        <v>0.79406399999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C181" s="1">
+        <v>0.55848200000000003</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C182" s="1">
+        <v>0.81512700000000005</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C183" s="1">
+        <v>0.75330200000000003</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C184" s="1">
+        <v>0.70169700000000002</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C185" s="1">
+        <v>0.33163199999999998</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C186" s="1">
+        <v>0.41650300000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C187" s="1">
+        <v>0.85991399999999996</v>
+      </c>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C188" s="1">
+        <v>0.52826799999999996</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C189" s="1">
+        <v>0.42892799999999998</v>
+      </c>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C190" s="1">
+        <v>0.74541599999999997</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C191" s="1">
+        <v>0.43427300000000002</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C192" s="1">
+        <v>0.73137799999999997</v>
+      </c>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C193" s="1">
+        <v>0.66078400000000004</v>
+      </c>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C194" s="1">
+        <v>0.78944800000000004</v>
+      </c>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C195" s="1">
+        <v>0.82201100000000005</v>
+      </c>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C196" s="1">
+        <v>0.79840699999999998</v>
+      </c>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C197" s="1">
+        <v>0.77349500000000004</v>
+      </c>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C198" s="1">
+        <v>0.73170299999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C199" s="1">
+        <v>0.77692300000000003</v>
+      </c>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C200" s="1">
+        <v>0.41524100000000003</v>
+      </c>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C201" s="1">
+        <v>0.748502</v>
+      </c>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C202" s="1">
+        <v>0.84039200000000003</v>
+      </c>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C203" s="1">
+        <v>0.79086500000000004</v>
+      </c>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C204" s="1">
+        <v>0.81306299999999998</v>
+      </c>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C205" s="1">
+        <v>0.69176000000000004</v>
+      </c>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C206" s="1">
+        <v>0.79701</v>
+      </c>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C207" s="1">
+        <v>14.713991</v>
+      </c>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C208" s="1">
+        <v>0.64497099999999996</v>
       </c>
     </row>
   </sheetData>
@@ -11718,55 +12720,3048 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8C459E-50BE-4541-BF26-DC91DCC5390E}">
-  <dimension ref="A1:B25"/>
+  <sheetPr codeName="Foglio4"/>
+  <dimension ref="A1:AX226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="50" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7</v>
+      </c>
+      <c r="N6" s="1">
+        <v>7</v>
+      </c>
+      <c r="O6" s="1">
+        <v>8</v>
+      </c>
+      <c r="P6" s="8">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>8</v>
+      </c>
+      <c r="R6" s="1">
+        <v>9</v>
+      </c>
+      <c r="S6" s="1">
+        <v>9</v>
+      </c>
+      <c r="T6" s="1">
+        <v>9</v>
+      </c>
+      <c r="U6" s="1">
+        <v>9</v>
+      </c>
+      <c r="V6" s="1">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1">
+        <v>10</v>
+      </c>
+      <c r="X6" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>11</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>11</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>12</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>12</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>12</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>12</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>13</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>13</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>13</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>13</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>13</v>
+      </c>
+      <c r="AN6" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="AO6" s="1">
+        <v>14</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>14</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>14</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>14</v>
+      </c>
+      <c r="AS6" s="1">
+        <v>15</v>
+      </c>
+      <c r="AT6" s="1">
+        <v>15</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>15</v>
+      </c>
+      <c r="AV6" s="1">
+        <v>15</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>15</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>3</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1">
+        <v>2</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3</v>
+      </c>
+      <c r="U7" s="1">
+        <v>4</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1</v>
+      </c>
+      <c r="W7" s="1">
+        <v>2</v>
+      </c>
+      <c r="X7" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AS7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AW7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AX7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
+        <f>AVERAGE(C$27:C$1048576)</f>
+        <v>0.82391370499999994</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:AX8" si="0">AVERAGE(D$27:D$1048576)</f>
+        <v>0.79885325999999945</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98085913999999963</v>
+      </c>
+      <c r="F8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AO8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AP8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AQ8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AT8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AU8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AV8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AW8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AX8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
+      <c r="C9" s="1">
+        <f>_xlfn.STDEV.S(C$27:C$1048576)</f>
+        <v>0.53838206038084879</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:AX9" si="1">_xlfn.STDEV.S(D$27:D$1048576)</f>
+        <v>0.10093503436375729</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>2.5127499731578418</v>
+      </c>
+      <c r="F9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AO9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AP9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AQ9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AT9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AU9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AV9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AW9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AX9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.827824</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.71983399999999997</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.74736000000000002</v>
+      </c>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <v>0.65968700000000002</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.78872299999999995</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.1517310000000001</v>
+      </c>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C29" s="1">
+        <v>0.81600200000000001</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.73148199999999997</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.68399799999999999</v>
+      </c>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C30" s="1">
+        <v>0.70269700000000002</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.78634400000000004</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.82786599999999999</v>
+      </c>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C31" s="1">
+        <v>0.76926899999999998</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.68206199999999995</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.76253300000000002</v>
+      </c>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C32" s="1">
+        <v>0.65143600000000002</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.68428599999999995</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.71306999999999998</v>
+      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C33" s="1">
+        <v>0.75826199999999999</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.68426100000000001</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.83709299999999998</v>
+      </c>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C34" s="1">
+        <v>0.71073200000000003</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.75511399999999995</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.83309599999999995</v>
+      </c>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <v>0.75869200000000003</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.79099600000000003</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.81879599999999997</v>
+      </c>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C36" s="1">
+        <v>0.877193</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.78749800000000003</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.85767400000000005</v>
+      </c>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C37" s="1">
+        <v>1.0374650000000001</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.89396900000000001</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.78981800000000002</v>
+      </c>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C38" s="1">
+        <v>0.57443999999999995</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.73783799999999999</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.81206800000000001</v>
+      </c>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+    </row>
+    <row r="39" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C39" s="1">
+        <v>0.72754799999999997</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.88449699999999998</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.88261900000000004</v>
+      </c>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+    </row>
+    <row r="40" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C40" s="1">
+        <v>0.72323800000000005</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.67844300000000002</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1.0099309999999999</v>
+      </c>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C41" s="1">
+        <v>0.81661499999999998</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.90853899999999999</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.75866400000000001</v>
+      </c>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C42" s="1">
+        <v>0.65046700000000002</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.85821099999999995</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.68484400000000001</v>
+      </c>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+    </row>
+    <row r="43" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C43" s="1">
+        <v>0.84608700000000003</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.95888099999999998</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.93547100000000005</v>
+      </c>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+    </row>
+    <row r="44" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C44" s="1">
+        <v>0.54974900000000004</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.74816800000000006</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.87048400000000004</v>
+      </c>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+    </row>
+    <row r="45" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C45" s="1">
+        <v>0.70909900000000003</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.800404</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.70616999999999996</v>
+      </c>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+    </row>
+    <row r="46" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <v>0.79455699999999996</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.82126399999999999</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.61653100000000005</v>
+      </c>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C47" s="1">
+        <v>0.84162899999999996</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.84445499999999996</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.68147999999999997</v>
+      </c>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C48" s="1">
+        <v>0.68845699999999999</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.71262700000000001</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.69737899999999997</v>
+      </c>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+    </row>
+    <row r="49" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C49" s="1">
+        <v>0.69594699999999998</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.78192799999999996</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.68743699999999996</v>
+      </c>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+    </row>
+    <row r="50" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C50" s="1">
+        <v>0.76068999999999998</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.83186499999999997</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.75838499999999998</v>
+      </c>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+    </row>
+    <row r="51" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C51" s="1">
+        <v>0.75489799999999996</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.48831200000000002</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.73604700000000001</v>
+      </c>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+    </row>
+    <row r="52" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C52" s="1">
+        <v>0.81734799999999996</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.88574200000000003</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.70753900000000003</v>
+      </c>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+    </row>
+    <row r="53" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C53" s="1">
+        <v>5.1958710000000004</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.86305699999999996</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.86324299999999998</v>
+      </c>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+    </row>
+    <row r="54" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C54" s="1">
+        <v>0.80102700000000004</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.77959400000000001</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0.87070899999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C55" s="1">
+        <v>0.80646300000000004</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.85656500000000002</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.73032399999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C56" s="1">
+        <v>0.66240500000000002</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.97995600000000005</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.720082</v>
+      </c>
+    </row>
+    <row r="57" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C57" s="1">
+        <v>0.78305599999999997</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.72700200000000004</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0.475605</v>
+      </c>
+    </row>
+    <row r="58" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C58" s="1">
+        <v>0.76363700000000001</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.81148299999999995</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.81139499999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C59" s="1">
+        <v>0.763428</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.78968700000000003</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.74488799999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C60" s="1">
+        <v>0.81897699999999996</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.79185300000000003</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.711565</v>
+      </c>
+    </row>
+    <row r="61" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C61" s="1">
+        <v>0.84216000000000002</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.820295</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.76876</v>
+      </c>
+    </row>
+    <row r="62" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C62" s="1">
+        <v>0.80127000000000004</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.68446300000000004</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0.78238700000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C63" s="1">
+        <v>0.91460300000000005</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.76589099999999999</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.85808399999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C64" s="1">
+        <v>0.81279599999999996</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.87660499999999997</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.81832099999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C65" s="1">
+        <v>0.81935999999999998</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.87973500000000004</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.75904899999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C66" s="1">
+        <v>0.91157999999999995</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.840804</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.78934599999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C67" s="1">
+        <v>0.75906600000000002</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.86058000000000001</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0.68471800000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C68" s="1">
+        <v>0.64944400000000002</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.84057899999999997</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.87670700000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C69" s="1">
+        <v>0.71206100000000006</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.78001799999999999</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0.67848799999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C70" s="1">
+        <v>0.89208200000000004</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.70729500000000001</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0.69185099999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C71" s="1">
+        <v>0.762683</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0.76885000000000003</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0.64890099999999995</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C72" s="1">
+        <v>0.86239399999999999</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.80780099999999999</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0.87242200000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C73" s="1">
+        <v>0.83010200000000001</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.73196300000000003</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0.74698100000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C74" s="1">
+        <v>0.64752100000000001</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.84347000000000005</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.86506400000000006</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C75" s="1">
+        <v>0.76133399999999996</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.755915</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.74003399999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C76" s="1">
+        <v>0.71553199999999995</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.76158400000000004</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.77296399999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C77" s="1">
+        <v>0.72136</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.71175200000000005</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0.77819799999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C78" s="1">
+        <v>0.84052400000000005</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.78805700000000001</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.737514</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C79" s="1">
+        <v>0.69303700000000001</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.83025199999999999</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0.80888899999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C80" s="1">
+        <v>0.54903500000000005</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.88735299999999995</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0.73319299999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C81" s="1">
+        <v>0.88204800000000005</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.82707399999999998</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0.78371199999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C82" s="1">
+        <v>0.74553899999999995</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0.80031799999999997</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0.86318600000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C83" s="1">
+        <v>0.68112499999999998</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.70693499999999998</v>
+      </c>
+      <c r="E83" s="1">
+        <v>0.88345799999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C84" s="1">
+        <v>0.92895000000000005</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.87590299999999999</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0.79976400000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C85" s="1">
+        <v>0.78721200000000002</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1.547882</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C86" s="1">
+        <v>0.78351199999999999</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.896702</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0.73259200000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C87" s="1">
+        <v>0.68715700000000002</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.81715300000000002</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0.76471</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C88" s="1">
+        <v>1.112044</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.76773599999999997</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.68297600000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C89" s="1">
+        <v>0.83216100000000004</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.84317299999999995</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0.79974699999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C90" s="1">
+        <v>0.78481699999999999</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.90661700000000001</v>
+      </c>
+      <c r="E90" s="1">
+        <v>0.77412899999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C91" s="1">
+        <v>0.86673299999999998</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0.76480899999999996</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0.70535899999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C92" s="1">
+        <v>0.68374699999999999</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.61605100000000002</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0.68293999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C93" s="1">
+        <v>0.70189000000000001</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.91196699999999997</v>
+      </c>
+      <c r="E93" s="1">
+        <v>0.79358099999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C94" s="1">
+        <v>0.72456799999999999</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0.66966199999999998</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0.72667800000000005</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C95" s="1">
+        <v>0.76644500000000004</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0.80672699999999997</v>
+      </c>
+      <c r="E95" s="1">
+        <v>0.75847500000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C96" s="1">
+        <v>0.67802799999999996</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.72011000000000003</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0.9002</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C97" s="1">
+        <v>0.64792700000000003</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0.755803</v>
+      </c>
+      <c r="E97" s="1">
+        <v>0.79461099999999996</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C98" s="1">
+        <v>0.85885400000000001</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.85155199999999998</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0.67509799999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C99" s="1">
+        <v>0.69564599999999999</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0.81748600000000005</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.84537499999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C100" s="1">
+        <v>0.88511700000000004</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0.87455099999999997</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.90619300000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C101" s="1">
+        <v>0.90761400000000003</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0.780358</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.79499399999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C102" s="1">
+        <v>0.76038899999999998</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.75966599999999995</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.90713600000000005</v>
+      </c>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C103" s="1">
+        <v>0.33665699999999998</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0.85116700000000001</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.70008999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C104" s="1">
+        <v>0.79938100000000001</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0.83945599999999998</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.81062100000000004</v>
+      </c>
+    </row>
+    <row r="105" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C105" s="1">
+        <v>0.79464599999999996</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0.75396399999999997</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.885351</v>
+      </c>
+    </row>
+    <row r="106" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C106" s="1">
+        <v>0.90524499999999997</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0.82709600000000005</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.72577999999999998</v>
+      </c>
+    </row>
+    <row r="107" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C107" s="1">
+        <v>0.84301199999999998</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0.84051600000000004</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.83210399999999995</v>
+      </c>
+    </row>
+    <row r="108" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C108" s="1">
+        <v>0.75378199999999995</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0.87383299999999997</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.70525300000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C109" s="1">
+        <v>0.70543699999999998</v>
+      </c>
+      <c r="D109" s="1">
+        <v>0.88353999999999999</v>
+      </c>
+      <c r="E109" s="1">
+        <v>0.600943</v>
+      </c>
+    </row>
+    <row r="110" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C110" s="1">
+        <v>0.68185200000000001</v>
+      </c>
+      <c r="D110" s="1">
+        <v>0.49198599999999998</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.85359300000000005</v>
+      </c>
+    </row>
+    <row r="111" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C111" s="1">
+        <v>0.78667399999999998</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0.615676</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0.82006999999999997</v>
+      </c>
+    </row>
+    <row r="112" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C112" s="1">
+        <v>0.81468799999999997</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0.81904299999999997</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0.77262200000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C113" s="1">
+        <v>0.90632199999999996</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0.63421400000000006</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0.76948099999999997</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C114" s="1">
+        <v>0.69210400000000005</v>
+      </c>
+      <c r="D114" s="1">
+        <v>0.83632300000000004</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.81840100000000005</v>
+      </c>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C115" s="1">
+        <v>0.71613499999999997</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0.85229999999999995</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0.35300799999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C116" s="1">
+        <v>0.780671</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0.80859400000000003</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.947322</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C117" s="1">
+        <v>0.72570000000000001</v>
+      </c>
+      <c r="D117" s="1">
+        <v>0.70904699999999998</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0.75663899999999995</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C118" s="1">
+        <v>0.84208799999999995</v>
+      </c>
+      <c r="D118" s="1">
+        <v>0.84763699999999997</v>
+      </c>
+      <c r="E118" s="1">
+        <v>0.74223600000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C119" s="1">
+        <v>0.79130800000000001</v>
+      </c>
+      <c r="D119" s="1">
+        <v>0.74385500000000004</v>
+      </c>
+      <c r="E119" s="1">
+        <v>0.80823299999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C120" s="1">
+        <v>0.82641699999999996</v>
+      </c>
+      <c r="D120" s="1">
+        <v>0.939276</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0.784501</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C121" s="1">
+        <v>0.72867000000000004</v>
+      </c>
+      <c r="D121" s="1">
+        <v>0.77961100000000005</v>
+      </c>
+      <c r="E121" s="1">
+        <v>0.73262499999999997</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C122" s="1">
+        <v>0.67852599999999996</v>
+      </c>
+      <c r="D122" s="1">
+        <v>0.79623500000000003</v>
+      </c>
+      <c r="E122" s="1">
+        <v>0.73019299999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C123" s="1">
+        <v>0.83281700000000003</v>
+      </c>
+      <c r="D123" s="1">
+        <v>0.84047700000000003</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0.75409099999999996</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C124" s="1">
+        <v>0.78771800000000003</v>
+      </c>
+      <c r="D124" s="1">
+        <v>0.87905500000000003</v>
+      </c>
+      <c r="E124" s="1">
+        <v>0.801373</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C125" s="1">
+        <v>0.90821300000000005</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0.73153999999999997</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.78613999999999995</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C126" s="1">
+        <v>0.74535600000000002</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0.80560500000000002</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.750197</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C127" s="1">
+        <v>0.76771500000000004</v>
+      </c>
+      <c r="D127" s="1">
+        <v>0.77979799999999999</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.82649899999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C128" s="1">
+        <v>0.87634999999999996</v>
+      </c>
+      <c r="D128" s="1">
+        <v>0.75269600000000003</v>
+      </c>
+      <c r="E128" s="1">
+        <v>0.75872799999999996</v>
+      </c>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C129" s="1">
+        <v>0.86241599999999996</v>
+      </c>
+      <c r="D129" s="1">
+        <v>0.79251000000000005</v>
+      </c>
+      <c r="E129" s="1">
+        <v>0.83432899999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C130" s="1">
+        <v>0.85241699999999998</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0.83745800000000004</v>
+      </c>
+      <c r="E130" s="1">
+        <v>0.68447499999999994</v>
+      </c>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C131" s="1">
+        <v>6.8071210000000004</v>
+      </c>
+      <c r="D131" s="1">
+        <v>0.86410799999999999</v>
+      </c>
+      <c r="E131" s="1">
+        <v>0.84056399999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C132" s="1">
+        <v>0.75847699999999996</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0.94306800000000002</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0.72329399999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C133" s="1">
+        <v>0.78572600000000004</v>
+      </c>
+      <c r="D133" s="1">
+        <v>0.70957400000000004</v>
+      </c>
+      <c r="E133" s="1">
+        <v>0.77060099999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C134" s="1">
+        <v>0.75404300000000002</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0.87002699999999999</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0.84450700000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C135" s="1">
+        <v>0.80219200000000002</v>
+      </c>
+      <c r="D135" s="1">
+        <v>0.72088799999999997</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.80886100000000005</v>
+      </c>
+    </row>
+    <row r="136" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C136" s="1">
+        <v>0.82962100000000005</v>
+      </c>
+      <c r="D136" s="1">
+        <v>0.86143000000000003</v>
+      </c>
+      <c r="E136" s="1">
+        <v>0.76247799999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C137" s="1">
+        <v>0.77792600000000001</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0.835036</v>
+      </c>
+      <c r="E137" s="1">
+        <v>0.84668299999999996</v>
+      </c>
+    </row>
+    <row r="138" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C138" s="1">
+        <v>0.71061099999999999</v>
+      </c>
+      <c r="D138" s="1">
+        <v>0.78979500000000002</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0.78949899999999995</v>
+      </c>
+    </row>
+    <row r="139" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C139" s="1">
+        <v>0.68410300000000002</v>
+      </c>
+      <c r="D139" s="1">
+        <v>0.87890800000000002</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0.77627500000000005</v>
+      </c>
+    </row>
+    <row r="140" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C140" s="1">
+        <v>0.72754099999999999</v>
+      </c>
+      <c r="D140" s="1">
+        <v>0.56814699999999996</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0.73770100000000005</v>
+      </c>
+    </row>
+    <row r="141" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C141" s="1">
+        <v>0.80937499999999996</v>
+      </c>
+      <c r="D141" s="1">
+        <v>0.64236400000000005</v>
+      </c>
+      <c r="E141" s="1">
+        <v>0.82902500000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C142" s="1">
+        <v>0.70611000000000002</v>
+      </c>
+      <c r="D142" s="1">
+        <v>0.71666799999999997</v>
+      </c>
+      <c r="E142" s="1">
+        <v>35.456567999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C143" s="1">
+        <v>0.50608600000000004</v>
+      </c>
+      <c r="D143" s="1">
+        <v>0.74762499999999998</v>
+      </c>
+      <c r="E143" s="1">
+        <v>0.724298</v>
+      </c>
+    </row>
+    <row r="144" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C144" s="1">
+        <v>0.74977499999999997</v>
+      </c>
+      <c r="D144" s="1">
+        <v>0.66429700000000003</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0.760382</v>
+      </c>
+    </row>
+    <row r="145" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C145" s="1">
+        <v>0.74443700000000002</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0.91012099999999996</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0.70494100000000004</v>
+      </c>
+    </row>
+    <row r="146" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C146" s="1">
+        <v>0.83455599999999996</v>
+      </c>
+      <c r="D146" s="1">
+        <v>1.0828739999999999</v>
+      </c>
+      <c r="E146" s="1">
+        <v>0.69096800000000003</v>
+      </c>
+    </row>
+    <row r="147" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C147" s="1">
+        <v>0.94970600000000005</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0.89036099999999996</v>
+      </c>
+      <c r="E147" s="1">
+        <v>0.75394899999999998</v>
+      </c>
+    </row>
+    <row r="148" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C148" s="1">
+        <v>0.65429899999999996</v>
+      </c>
+      <c r="D148" s="1">
+        <v>0.808145</v>
+      </c>
+      <c r="E148" s="1">
+        <v>0.78361899999999995</v>
+      </c>
+    </row>
+    <row r="149" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C149" s="1">
+        <v>0.76465300000000003</v>
+      </c>
+      <c r="D149" s="1">
+        <v>0.891764</v>
+      </c>
+      <c r="E149" s="1">
+        <v>0.67184299999999997</v>
+      </c>
+    </row>
+    <row r="150" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C150" s="1">
+        <v>0.63072799999999996</v>
+      </c>
+      <c r="D150" s="1">
+        <v>0.85550199999999998</v>
+      </c>
+      <c r="E150" s="1">
+        <v>0.67306900000000003</v>
+      </c>
+    </row>
+    <row r="151" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C151" s="1">
+        <v>0.60566699999999996</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0.813998</v>
+      </c>
+      <c r="E151" s="1">
+        <v>0.82058600000000004</v>
+      </c>
+    </row>
+    <row r="152" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C152" s="1">
+        <v>0.62484499999999998</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0.74471399999999999</v>
+      </c>
+      <c r="E152" s="1">
+        <v>0.69089500000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C153" s="1">
+        <v>0.88849199999999995</v>
+      </c>
+      <c r="D153" s="1">
+        <v>0.88053700000000001</v>
+      </c>
+      <c r="E153" s="1">
+        <v>0.62897899999999995</v>
+      </c>
+    </row>
+    <row r="154" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C154" s="1">
+        <v>0.74446100000000004</v>
+      </c>
+      <c r="D154" s="1">
+        <v>0.86239299999999997</v>
+      </c>
+      <c r="E154" s="1">
+        <v>0.80046200000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C155" s="1">
+        <v>0.68325599999999997</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0.80231200000000003</v>
+      </c>
+      <c r="E155" s="1">
+        <v>0.67437899999999995</v>
+      </c>
+    </row>
+    <row r="156" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C156" s="1">
+        <v>0.75120900000000002</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0.68737400000000004</v>
+      </c>
+      <c r="E156" s="1">
+        <v>0.84059700000000004</v>
+      </c>
+    </row>
+    <row r="157" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C157" s="1">
+        <v>0.79538200000000003</v>
+      </c>
+      <c r="D157" s="1">
+        <v>0.74476900000000001</v>
+      </c>
+      <c r="E157" s="1">
+        <v>0.79325199999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C158" s="1">
+        <v>0.82598499999999997</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0.91693500000000006</v>
+      </c>
+      <c r="E158" s="1">
+        <v>0.70333500000000004</v>
+      </c>
+    </row>
+    <row r="159" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C159" s="1">
+        <v>0.72479800000000005</v>
+      </c>
+      <c r="D159" s="1">
+        <v>0.908192</v>
+      </c>
+      <c r="E159" s="1">
+        <v>0.83552300000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C160" s="1">
+        <v>0.74166500000000002</v>
+      </c>
+      <c r="D160" s="1">
+        <v>0.89255700000000004</v>
+      </c>
+      <c r="E160" s="1">
+        <v>0.72162999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C161" s="1">
+        <v>0.686199</v>
+      </c>
+      <c r="D161" s="1">
+        <v>0.88103100000000001</v>
+      </c>
+      <c r="E161" s="1">
+        <v>0.71606400000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C162" s="1">
+        <v>0.83666099999999999</v>
+      </c>
+      <c r="D162" s="1">
+        <v>1.077545</v>
+      </c>
+      <c r="E162" s="1">
+        <v>0.66725199999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C163" s="1">
+        <v>0.80331399999999997</v>
+      </c>
+      <c r="D163" s="1">
+        <v>0.86197699999999999</v>
+      </c>
+      <c r="E163" s="1">
+        <v>0.76930799999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C164" s="1">
+        <v>0.73815900000000001</v>
+      </c>
+      <c r="D164" s="1">
+        <v>0.83322200000000002</v>
+      </c>
+      <c r="E164" s="1">
+        <v>0.69089</v>
+      </c>
+    </row>
+    <row r="165" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C165" s="1">
+        <v>0.81269199999999997</v>
+      </c>
+      <c r="D165" s="1">
+        <v>0.77183800000000002</v>
+      </c>
+      <c r="E165" s="1">
+        <v>0.80845400000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C166" s="1">
+        <v>0.67544300000000002</v>
+      </c>
+      <c r="D166" s="1">
+        <v>0.775837</v>
+      </c>
+      <c r="E166" s="1">
+        <v>0.633691</v>
+      </c>
+    </row>
+    <row r="167" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C167" s="1">
+        <v>1.0024580000000001</v>
+      </c>
+      <c r="D167" s="1">
+        <v>0.709565</v>
+      </c>
+      <c r="E167" s="1">
+        <v>0.77123299999999995</v>
+      </c>
+    </row>
+    <row r="168" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C168" s="1">
+        <v>0.66915000000000002</v>
+      </c>
+      <c r="D168" s="1">
+        <v>0.92624300000000004</v>
+      </c>
+      <c r="E168" s="1">
+        <v>0.88032999999999995</v>
+      </c>
+    </row>
+    <row r="169" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C169" s="1">
+        <v>0.76775899999999997</v>
+      </c>
+      <c r="D169" s="1">
+        <v>0.83856299999999995</v>
+      </c>
+      <c r="E169" s="1">
+        <v>0.29853200000000002</v>
+      </c>
+    </row>
+    <row r="170" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C170" s="1">
+        <v>0.68912700000000005</v>
+      </c>
+      <c r="D170" s="1">
+        <v>0.76655099999999998</v>
+      </c>
+      <c r="E170" s="1">
+        <v>0.90427299999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C171" s="1">
+        <v>0.63176299999999996</v>
+      </c>
+      <c r="D171" s="1">
+        <v>0.94045199999999995</v>
+      </c>
+      <c r="E171" s="1">
+        <v>0.78938600000000003</v>
+      </c>
+    </row>
+    <row r="172" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C172" s="1">
+        <v>0.77114499999999997</v>
+      </c>
+      <c r="D172" s="1">
+        <v>0.85161900000000001</v>
+      </c>
+      <c r="E172" s="1">
+        <v>0.623359</v>
+      </c>
+    </row>
+    <row r="173" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C173" s="1">
+        <v>0.78473400000000004</v>
+      </c>
+      <c r="D173" s="1">
+        <v>0.80432099999999995</v>
+      </c>
+      <c r="E173" s="1">
+        <v>0.65181999999999995</v>
+      </c>
+    </row>
+    <row r="174" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C174" s="1">
+        <v>0.82504699999999997</v>
+      </c>
+      <c r="D174" s="1">
+        <v>0.93775200000000003</v>
+      </c>
+      <c r="E174" s="1">
+        <v>0.88998600000000005</v>
+      </c>
+    </row>
+    <row r="175" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C175" s="1">
+        <v>0.71214299999999997</v>
+      </c>
+      <c r="D175" s="1">
+        <v>0.75922599999999996</v>
+      </c>
+      <c r="E175" s="1">
+        <v>0.76144800000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C176" s="1">
+        <v>0.80823900000000004</v>
+      </c>
+      <c r="D176" s="1">
+        <v>0.85911199999999999</v>
+      </c>
+      <c r="E176" s="1">
+        <v>0.80663700000000005</v>
+      </c>
+    </row>
+    <row r="177" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C177" s="1">
+        <v>0.77197099999999996</v>
+      </c>
+      <c r="D177" s="1">
+        <v>0.83351200000000003</v>
+      </c>
+      <c r="E177" s="1">
+        <v>0.77683899999999995</v>
+      </c>
+    </row>
+    <row r="178" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C178" s="1">
+        <v>0.70584499999999994</v>
+      </c>
+      <c r="D178" s="1">
+        <v>0.79469800000000002</v>
+      </c>
+      <c r="E178" s="1">
+        <v>0.86972799999999995</v>
+      </c>
+    </row>
+    <row r="179" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C179" s="1">
+        <v>0.83099199999999995</v>
+      </c>
+      <c r="D179" s="1">
+        <v>0.89733099999999999</v>
+      </c>
+      <c r="E179" s="1">
+        <v>0.81690700000000005</v>
+      </c>
+    </row>
+    <row r="180" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C180" s="1">
+        <v>0.805674</v>
+      </c>
+      <c r="D180" s="1">
+        <v>0.62378400000000001</v>
+      </c>
+      <c r="E180" s="1">
+        <v>0.91868399999999995</v>
+      </c>
+    </row>
+    <row r="181" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C181" s="1">
+        <v>0.81303499999999995</v>
+      </c>
+      <c r="D181" s="1">
+        <v>0.80554999999999999</v>
+      </c>
+      <c r="E181" s="1">
+        <v>0.88416499999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C182" s="1">
+        <v>0.85013899999999998</v>
+      </c>
+      <c r="D182" s="1">
+        <v>0.799736</v>
+      </c>
+      <c r="E182" s="1">
+        <v>0.83289000000000002</v>
+      </c>
+    </row>
+    <row r="183" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C183" s="1">
+        <v>0.77280300000000002</v>
+      </c>
+      <c r="D183" s="1">
+        <v>0.74090699999999998</v>
+      </c>
+      <c r="E183" s="1">
+        <v>0.69267599999999996</v>
+      </c>
+    </row>
+    <row r="184" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C184" s="1">
+        <v>0.78658899999999998</v>
+      </c>
+      <c r="D184" s="1">
+        <v>0.839638</v>
+      </c>
+      <c r="E184" s="1">
+        <v>8.4773429999999994</v>
+      </c>
+    </row>
+    <row r="185" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C185" s="1">
+        <v>0.73600900000000002</v>
+      </c>
+      <c r="D185" s="1">
+        <v>0.83928400000000003</v>
+      </c>
+      <c r="E185" s="1">
+        <v>0.72121599999999997</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C186" s="1">
+        <v>0.92170600000000003</v>
+      </c>
+      <c r="D186" s="1">
+        <v>0.77676100000000003</v>
+      </c>
+      <c r="E186" s="1">
+        <v>0.71726199999999996</v>
+      </c>
+    </row>
+    <row r="187" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C187" s="1">
+        <v>0.93893700000000002</v>
+      </c>
+      <c r="D187" s="1">
+        <v>0.68766899999999997</v>
+      </c>
+      <c r="E187" s="1">
+        <v>0.80535699999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C188" s="1">
+        <v>0.80275600000000003</v>
+      </c>
+      <c r="D188" s="1">
+        <v>0.84344799999999998</v>
+      </c>
+      <c r="E188" s="1">
+        <v>0.83602799999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C189" s="1">
+        <v>0.73965800000000004</v>
+      </c>
+      <c r="D189" s="1">
+        <v>0.91036300000000003</v>
+      </c>
+      <c r="E189" s="1">
+        <v>0.71397200000000005</v>
+      </c>
+    </row>
+    <row r="190" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C190" s="1">
+        <v>0.77812499999999996</v>
+      </c>
+      <c r="D190" s="1">
+        <v>0.85965899999999995</v>
+      </c>
+      <c r="E190" s="1">
+        <v>0.76131499999999996</v>
+      </c>
+    </row>
+    <row r="191" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C191" s="1">
+        <v>1.4319539999999999</v>
+      </c>
+      <c r="D191" s="1">
+        <v>0.740707</v>
+      </c>
+      <c r="E191" s="1">
+        <v>0.81703899999999996</v>
+      </c>
+    </row>
+    <row r="192" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C192" s="1">
+        <v>0.79108800000000001</v>
+      </c>
+      <c r="D192" s="1">
+        <v>0.77483199999999997</v>
+      </c>
+      <c r="E192" s="1">
+        <v>0.72248299999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C193" s="1">
+        <v>0.81469899999999995</v>
+      </c>
+      <c r="D193" s="1">
+        <v>0.73581300000000005</v>
+      </c>
+      <c r="E193" s="1">
+        <v>0.81614600000000004</v>
+      </c>
+    </row>
+    <row r="194" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C194" s="1">
+        <v>0.79129799999999995</v>
+      </c>
+      <c r="D194" s="1">
+        <v>0.86807800000000002</v>
+      </c>
+      <c r="E194" s="1">
+        <v>0.95389599999999997</v>
+      </c>
+    </row>
+    <row r="195" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C195" s="1">
+        <v>0.76603600000000005</v>
+      </c>
+      <c r="D195" s="1">
+        <v>0.83402500000000002</v>
+      </c>
+      <c r="E195" s="1">
+        <v>0.65790800000000005</v>
+      </c>
+    </row>
+    <row r="196" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C196" s="1">
+        <v>0.68838600000000005</v>
+      </c>
+      <c r="D196" s="1">
+        <v>0.90095999999999998</v>
+      </c>
+      <c r="E196" s="1">
+        <v>0.73436699999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C197" s="1">
+        <v>0.77167699999999995</v>
+      </c>
+      <c r="D197" s="1">
+        <v>0.75257600000000002</v>
+      </c>
+      <c r="E197" s="1">
+        <v>0.90441000000000005</v>
+      </c>
+    </row>
+    <row r="198" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C198" s="1">
+        <v>0.79523999999999995</v>
+      </c>
+      <c r="D198" s="1">
+        <v>0.77257500000000001</v>
+      </c>
+      <c r="E198" s="1">
+        <v>0.94897100000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C199" s="1">
+        <v>0.83272400000000002</v>
+      </c>
+      <c r="D199" s="1">
+        <v>0.79180700000000004</v>
+      </c>
+      <c r="E199" s="1">
+        <v>0.91170099999999998</v>
+      </c>
+    </row>
+    <row r="200" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C200" s="1">
+        <v>0.74222399999999999</v>
+      </c>
+      <c r="D200" s="1">
+        <v>0.80095099999999997</v>
+      </c>
+      <c r="E200" s="1">
+        <v>1.0023899999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C201" s="1">
+        <v>0.777563</v>
+      </c>
+      <c r="D201" s="1">
+        <v>0.78809600000000002</v>
+      </c>
+      <c r="E201" s="1">
+        <v>0.71531999999999996</v>
+      </c>
+    </row>
+    <row r="202" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C202" s="1">
+        <v>0.74151800000000001</v>
+      </c>
+      <c r="D202" s="1">
+        <v>0.85196000000000005</v>
+      </c>
+      <c r="E202" s="1">
+        <v>0.73211499999999996</v>
+      </c>
+    </row>
+    <row r="203" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C203" s="1">
+        <v>0.73907500000000004</v>
+      </c>
+      <c r="D203" s="1">
+        <v>0.85433099999999995</v>
+      </c>
+      <c r="E203" s="1">
+        <v>0.83703700000000003</v>
+      </c>
+    </row>
+    <row r="204" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C204" s="1">
+        <v>0.771505</v>
+      </c>
+      <c r="D204" s="1">
+        <v>0.88715699999999997</v>
+      </c>
+      <c r="E204" s="1">
+        <v>0.69959899999999997</v>
+      </c>
+    </row>
+    <row r="205" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C205" s="1">
+        <v>0.73191499999999998</v>
+      </c>
+      <c r="D205" s="1">
+        <v>0.78221600000000002</v>
+      </c>
+      <c r="E205" s="1">
+        <v>0.92889900000000003</v>
+      </c>
+    </row>
+    <row r="206" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C206" s="1">
+        <v>0.67251399999999995</v>
+      </c>
+      <c r="D206" s="1">
+        <v>0.84105200000000002</v>
+      </c>
+      <c r="E206" s="1">
+        <v>0.83557000000000003</v>
+      </c>
+    </row>
+    <row r="207" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C207" s="1">
+        <v>0.44656699999999999</v>
+      </c>
+      <c r="D207" s="1">
+        <v>0.76929400000000003</v>
+      </c>
+      <c r="E207" s="1">
+        <v>0.61683900000000003</v>
+      </c>
+    </row>
+    <row r="208" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C208" s="1">
+        <v>0.64500400000000002</v>
+      </c>
+      <c r="D208" s="1">
+        <v>0.87575099999999995</v>
+      </c>
+      <c r="E208" s="1">
+        <v>0.70646299999999995</v>
+      </c>
+    </row>
+    <row r="209" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C209" s="1">
+        <v>0.73963000000000001</v>
+      </c>
+      <c r="D209" s="1">
+        <v>0.82649099999999998</v>
+      </c>
+      <c r="E209" s="1">
+        <v>0.29358299999999998</v>
+      </c>
+    </row>
+    <row r="210" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C210" s="1">
+        <v>0.68988000000000005</v>
+      </c>
+      <c r="D210" s="1">
+        <v>0.74294700000000002</v>
+      </c>
+      <c r="E210" s="1">
+        <v>0.78344100000000005</v>
+      </c>
+    </row>
+    <row r="211" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C211" s="1">
+        <v>0.77331899999999998</v>
+      </c>
+      <c r="D211" s="1">
+        <v>0.87756500000000004</v>
+      </c>
+      <c r="E211" s="1">
+        <v>0.67334099999999997</v>
+      </c>
+    </row>
+    <row r="212" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C212" s="1">
+        <v>0.65244100000000005</v>
+      </c>
+      <c r="D212" s="1">
+        <v>0.84000600000000003</v>
+      </c>
+      <c r="E212" s="1">
+        <v>0.68389699999999998</v>
+      </c>
+    </row>
+    <row r="213" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C213" s="1">
+        <v>0.79516100000000001</v>
+      </c>
+      <c r="D213" s="1">
+        <v>0.69176599999999999</v>
+      </c>
+      <c r="E213" s="1">
+        <v>0.78646700000000003</v>
+      </c>
+    </row>
+    <row r="214" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C214" s="1">
+        <v>0.88055899999999998</v>
+      </c>
+      <c r="D214" s="1">
+        <v>0.46248</v>
+      </c>
+      <c r="E214" s="1">
+        <v>0.68656499999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C215" s="1">
+        <v>0.71553699999999998</v>
+      </c>
+      <c r="D215" s="1">
+        <v>0.98769300000000004</v>
+      </c>
+      <c r="E215" s="1">
+        <v>0.79135500000000003</v>
+      </c>
+    </row>
+    <row r="216" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C216" s="1">
+        <v>0.82155500000000004</v>
+      </c>
+      <c r="D216" s="1">
+        <v>0.83369599999999999</v>
+      </c>
+      <c r="E216" s="1">
+        <v>0.79961599999999999</v>
+      </c>
+    </row>
+    <row r="217" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C217" s="1">
+        <v>0.72851500000000002</v>
+      </c>
+      <c r="D217" s="1">
+        <v>0.76056199999999996</v>
+      </c>
+      <c r="E217" s="1">
+        <v>0.63454299999999997</v>
+      </c>
+    </row>
+    <row r="218" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C218" s="1">
+        <v>0.69589999999999996</v>
+      </c>
+      <c r="D218" s="1">
+        <v>0.78183100000000005</v>
+      </c>
+      <c r="E218" s="1">
+        <v>0.561859</v>
+      </c>
+    </row>
+    <row r="219" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C219" s="1">
+        <v>0.97849200000000003</v>
+      </c>
+      <c r="D219" s="1">
+        <v>0.95539200000000002</v>
+      </c>
+      <c r="E219" s="1">
+        <v>0.41889399999999999</v>
+      </c>
+    </row>
+    <row r="220" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C220" s="1">
+        <v>0.88471999999999995</v>
+      </c>
+      <c r="D220" s="1">
+        <v>0.763903</v>
+      </c>
+      <c r="E220" s="1">
+        <v>0.68810499999999997</v>
+      </c>
+    </row>
+    <row r="221" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C221" s="1">
+        <v>0.72514900000000004</v>
+      </c>
+      <c r="D221" s="1">
+        <v>0.76099399999999995</v>
+      </c>
+      <c r="E221" s="1">
+        <v>0.68955999999999995</v>
+      </c>
+    </row>
+    <row r="222" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C222" s="1">
+        <v>0.76282399999999995</v>
+      </c>
+      <c r="D222" s="1">
+        <v>0.28909899999999999</v>
+      </c>
+      <c r="E222" s="1">
+        <v>0.79119499999999998</v>
+      </c>
+    </row>
+    <row r="223" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C223" s="1">
+        <v>0.76976900000000004</v>
+      </c>
+      <c r="D223" s="1">
+        <v>0.83818599999999999</v>
+      </c>
+      <c r="E223" s="1">
+        <v>0.78285400000000005</v>
+      </c>
+    </row>
+    <row r="224" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C224" s="1">
+        <v>0.83145100000000005</v>
+      </c>
+      <c r="D224" s="1">
+        <v>0.81164700000000001</v>
+      </c>
+      <c r="E224" s="1">
+        <v>0.71130400000000005</v>
+      </c>
+    </row>
+    <row r="225" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C225" s="1">
+        <v>0.79926799999999998</v>
+      </c>
+      <c r="D225" s="1">
+        <v>0.34890100000000002</v>
+      </c>
+      <c r="E225" s="1">
+        <v>0.75627100000000003</v>
+      </c>
+    </row>
+    <row r="226" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C226" s="1">
+        <v>0.98978999999999995</v>
+      </c>
+      <c r="D226" s="1">
+        <v>0.80882200000000004</v>
+      </c>
+      <c r="E226" s="1">
+        <v>0.77655700000000005</v>
       </c>
     </row>
   </sheetData>
@@ -11776,14 +15771,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CAF787-759A-49CC-8F4A-93698220D9F1}">
-  <sheetPr>
+  <sheetPr codeName="Foglio5">
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
docs: update stats of delivery delay (v3)
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fedebrando\SORTproject\SantaClausProblem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1222CD32-BEE9-4471-ADA5-1C3CD7BF31B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344D2698-401B-4369-BF63-9DEB4D78777B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,10 +264,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1658,14 +1658,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="8"/>
+      <c r="E6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -12790,10 +12790,10 @@
       <c r="O6" s="1">
         <v>8</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <v>8</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="7">
         <v>8</v>
       </c>
       <c r="R6" s="1">
@@ -12939,10 +12939,10 @@
       <c r="O7" s="1">
         <v>1</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="7">
         <v>2</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="7">
         <v>3</v>
       </c>
       <c r="R7" s="1">
@@ -13061,17 +13061,17 @@
         <f t="shared" si="0"/>
         <v>0.98085913999999963</v>
       </c>
-      <c r="F8" s="1" t="e">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="1" t="e">
+        <v>1.3800737449999998</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="1" t="e">
+        <v>1.9725799850000003</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.8737630049999998</v>
       </c>
       <c r="I8" s="1" t="e">
         <f t="shared" si="0"/>
@@ -13258,17 +13258,17 @@
         <f t="shared" si="1"/>
         <v>2.5127499731578418</v>
       </c>
-      <c r="F9" s="1" t="e">
+      <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" s="1" t="e">
+        <v>0.74086503196182063</v>
+      </c>
+      <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="1" t="e">
+        <v>2.7859707026448528</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.58798413744582112</v>
       </c>
       <c r="I9" s="1" t="e">
         <f t="shared" si="1"/>
@@ -13440,72 +13440,72 @@
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
@@ -13520,8 +13520,17 @@
       <c r="E27" s="1">
         <v>0.74736000000000002</v>
       </c>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
+      <c r="F27" s="1">
+        <v>0.77510000000000001</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.76629999999999998</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2.3079999999999998</v>
+      </c>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C28" s="1">
@@ -13533,8 +13542,17 @@
       <c r="E28" s="1">
         <v>1.1517310000000001</v>
       </c>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
+      <c r="F28" s="1">
+        <v>2.107691</v>
+      </c>
+      <c r="G28" s="1">
+        <v>12.4968</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2.1040999999999999</v>
+      </c>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C29" s="1">
@@ -13546,8 +13564,17 @@
       <c r="E29" s="1">
         <v>0.68399799999999999</v>
       </c>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
+      <c r="F29" s="1">
+        <v>2.0876169999999998</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.72809999999999997</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.9603999999999999</v>
+      </c>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C30" s="1">
@@ -13559,8 +13586,17 @@
       <c r="E30" s="1">
         <v>0.82786599999999999</v>
       </c>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
+      <c r="F30" s="1">
+        <v>2.2530000000000001</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2.1469999999999998</v>
+      </c>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C31" s="1">
@@ -13572,8 +13608,17 @@
       <c r="E31" s="1">
         <v>0.76253300000000002</v>
       </c>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
+      <c r="F31" s="1">
+        <v>2.2984</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.76990000000000003</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2.0367999999999999</v>
+      </c>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C32" s="1">
@@ -13585,8 +13630,17 @@
       <c r="E32" s="1">
         <v>0.71306999999999998</v>
       </c>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
+      <c r="F32" s="1">
+        <v>2.0421999999999998</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.7671</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2.2027000000000001</v>
+      </c>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
@@ -13598,8 +13652,17 @@
       <c r="E33" s="1">
         <v>0.83709299999999998</v>
       </c>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
+      <c r="F33" s="1">
+        <v>2.1005410000000002</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.40310000000000001</v>
+      </c>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C34" s="1">
@@ -13611,8 +13674,17 @@
       <c r="E34" s="1">
         <v>0.83309599999999995</v>
       </c>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
+      <c r="F34" s="1">
+        <v>0.738788</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.75549999999999995</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1.9756</v>
+      </c>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C35" s="1">
@@ -13624,8 +13696,17 @@
       <c r="E35" s="1">
         <v>0.81879599999999997</v>
       </c>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
+      <c r="F35" s="1">
+        <v>2.2745760000000002</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.52370000000000005</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2.1783000000000001</v>
+      </c>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
     </row>
     <row r="36" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C36" s="1">
@@ -13637,8 +13718,17 @@
       <c r="E36" s="1">
         <v>0.85767400000000005</v>
       </c>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
+      <c r="F36" s="1">
+        <v>1.9666159999999999</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.73209999999999997</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2.2086999999999999</v>
+      </c>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
@@ -13650,8 +13740,17 @@
       <c r="E37" s="1">
         <v>0.78981800000000002</v>
       </c>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
+      <c r="F37" s="1">
+        <v>2.4028</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.63949999999999996</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2.1539000000000001</v>
+      </c>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C38" s="1">
@@ -13663,8 +13762,17 @@
       <c r="E38" s="1">
         <v>0.81206800000000001</v>
       </c>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
+      <c r="F38" s="1">
+        <v>0.72119599999999995</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.7732</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2.3005</v>
+      </c>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C39" s="1">
@@ -13676,8 +13784,17 @@
       <c r="E39" s="1">
         <v>0.88261900000000004</v>
       </c>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
+      <c r="F39" s="1">
+        <v>2.0304160000000002</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.78349999999999997</v>
+      </c>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C40" s="1">
@@ -13689,8 +13806,17 @@
       <c r="E40" s="1">
         <v>1.0099309999999999</v>
       </c>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
+      <c r="F40" s="1">
+        <v>2.0845919999999998</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.69130000000000003</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1.601299</v>
+      </c>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C41" s="1">
@@ -13702,8 +13828,17 @@
       <c r="E41" s="1">
         <v>0.75866400000000001</v>
       </c>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
+      <c r="F41" s="1">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.76659999999999995</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C42" s="1">
@@ -13715,8 +13850,17 @@
       <c r="E42" s="1">
         <v>0.68484400000000001</v>
       </c>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
+      <c r="F42" s="1">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="G42" s="1">
+        <v>6.0312999999999999</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1.6814</v>
+      </c>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C43" s="1">
@@ -13728,8 +13872,17 @@
       <c r="E43" s="1">
         <v>0.93547100000000005</v>
       </c>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
+      <c r="F43" s="1">
+        <v>2.04325</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.77569999999999995</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1.3019000000000001</v>
+      </c>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C44" s="1">
@@ -13741,8 +13894,17 @@
       <c r="E44" s="1">
         <v>0.87048400000000004</v>
       </c>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
+      <c r="F44" s="1">
+        <v>2.0391249999999999</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1.1633</v>
+      </c>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
     </row>
     <row r="45" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C45" s="1">
@@ -13754,8 +13916,17 @@
       <c r="E45" s="1">
         <v>0.70616999999999996</v>
       </c>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
+      <c r="F45" s="1">
+        <v>2.3022</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.73440000000000005</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2.3062</v>
+      </c>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C46" s="1">
@@ -13767,8 +13938,17 @@
       <c r="E46" s="1">
         <v>0.61653100000000005</v>
       </c>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
+      <c r="F46" s="1">
+        <v>2.2795000000000001</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.73760000000000003</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2.2505000000000002</v>
+      </c>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C47" s="1">
@@ -13780,8 +13960,17 @@
       <c r="E47" s="1">
         <v>0.68147999999999997</v>
       </c>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
+      <c r="F47" s="1">
+        <v>2.2747999999999999</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="H47" s="1">
+        <v>2.1368999999999998</v>
+      </c>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C48" s="1">
@@ -13793,8 +13982,17 @@
       <c r="E48" s="1">
         <v>0.69737899999999997</v>
       </c>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
+      <c r="F48" s="1">
+        <v>2.014834</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.72509999999999997</v>
+      </c>
+      <c r="H48" s="1">
+        <v>2.2858000000000001</v>
+      </c>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
     </row>
     <row r="49" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C49" s="1">
@@ -13806,8 +14004,17 @@
       <c r="E49" s="1">
         <v>0.68743699999999996</v>
       </c>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
+      <c r="F49" s="1">
+        <v>2.0161169999999999</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.72050000000000003</v>
+      </c>
+      <c r="H49" s="1">
+        <v>2.2360000000000002</v>
+      </c>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
     </row>
     <row r="50" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C50" s="1">
@@ -13819,8 +14026,17 @@
       <c r="E50" s="1">
         <v>0.75838499999999998</v>
       </c>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
+      <c r="F50" s="1">
+        <v>0.57236699999999996</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.71879999999999999</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2.0972</v>
+      </c>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C51" s="1">
@@ -13832,8 +14048,17 @@
       <c r="E51" s="1">
         <v>0.73604700000000001</v>
       </c>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
+      <c r="F51" s="1">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1.8193999999999999</v>
+      </c>
+      <c r="H51" s="1">
+        <v>2.1655000000000002</v>
+      </c>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
     </row>
     <row r="52" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C52" s="1">
@@ -13845,8 +14070,17 @@
       <c r="E52" s="1">
         <v>0.70753900000000003</v>
       </c>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
+      <c r="F52" s="1">
+        <v>0.48649999999999999</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2.0087999999999999</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.44579999999999997</v>
+      </c>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
     </row>
     <row r="53" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C53" s="1">
@@ -13858,8 +14092,17 @@
       <c r="E53" s="1">
         <v>0.86324299999999998</v>
       </c>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
+      <c r="F53" s="1">
+        <v>0.75790000000000002</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1.9810000000000001</v>
+      </c>
+      <c r="H53" s="1">
+        <v>2.3292000000000002</v>
+      </c>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
     </row>
     <row r="54" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C54" s="1">
@@ -13871,6 +14114,15 @@
       <c r="E54" s="1">
         <v>0.87070899999999996</v>
       </c>
+      <c r="F54" s="1">
+        <v>0.45915800000000001</v>
+      </c>
+      <c r="G54" s="1">
+        <v>2.1907999999999999</v>
+      </c>
+      <c r="H54" s="1">
+        <v>2.3065000000000002</v>
+      </c>
     </row>
     <row r="55" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C55" s="1">
@@ -13882,6 +14134,15 @@
       <c r="E55" s="1">
         <v>0.73032399999999997</v>
       </c>
+      <c r="F55" s="1">
+        <v>2.2147999999999999</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1.9759</v>
+      </c>
+      <c r="H55" s="1">
+        <v>2.3877999999999999</v>
+      </c>
     </row>
     <row r="56" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C56" s="1">
@@ -13893,6 +14154,15 @@
       <c r="E56" s="1">
         <v>0.720082</v>
       </c>
+      <c r="F56" s="1">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="G56" s="1">
+        <v>2.0566</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0.81130000000000002</v>
+      </c>
     </row>
     <row r="57" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C57" s="1">
@@ -13904,6 +14174,15 @@
       <c r="E57" s="1">
         <v>0.475605</v>
       </c>
+      <c r="F57" s="1">
+        <v>2.3986999999999998</v>
+      </c>
+      <c r="G57" s="1">
+        <v>2.0712000000000002</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1.9381999999999999</v>
+      </c>
     </row>
     <row r="58" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C58" s="1">
@@ -13915,6 +14194,15 @@
       <c r="E58" s="1">
         <v>0.81139499999999998</v>
       </c>
+      <c r="F58" s="1">
+        <v>2.3995869999999999</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.86639999999999995</v>
+      </c>
+      <c r="H58" s="1">
+        <v>2.3054000000000001</v>
+      </c>
     </row>
     <row r="59" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C59" s="1">
@@ -13926,6 +14214,15 @@
       <c r="E59" s="1">
         <v>0.74488799999999999</v>
       </c>
+      <c r="F59" s="1">
+        <v>0.74314100000000005</v>
+      </c>
+      <c r="G59" s="1">
+        <v>2.0196000000000001</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.84799999999999998</v>
+      </c>
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C60" s="1">
@@ -13937,6 +14234,15 @@
       <c r="E60" s="1">
         <v>0.711565</v>
       </c>
+      <c r="F60" s="1">
+        <v>2.167916</v>
+      </c>
+      <c r="G60" s="1">
+        <v>2.1758000000000002</v>
+      </c>
+      <c r="H60" s="1">
+        <v>2.1783999999999999</v>
+      </c>
     </row>
     <row r="61" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C61" s="1">
@@ -13948,6 +14254,15 @@
       <c r="E61" s="1">
         <v>0.76876</v>
       </c>
+      <c r="F61" s="1">
+        <v>2.3403</v>
+      </c>
+      <c r="G61" s="1">
+        <v>2.0691000000000002</v>
+      </c>
+      <c r="H61" s="1">
+        <v>2.1478000000000002</v>
+      </c>
     </row>
     <row r="62" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C62" s="1">
@@ -13959,6 +14274,15 @@
       <c r="E62" s="1">
         <v>0.78238700000000005</v>
       </c>
+      <c r="F62" s="1">
+        <v>2.3610000000000002</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2.0636990000000002</v>
+      </c>
+      <c r="H62" s="1">
+        <v>2.1589999999999998</v>
+      </c>
     </row>
     <row r="63" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C63" s="1">
@@ -13970,6 +14294,15 @@
       <c r="E63" s="1">
         <v>0.85808399999999996</v>
       </c>
+      <c r="F63" s="1">
+        <v>2.2134</v>
+      </c>
+      <c r="G63" s="1">
+        <v>2.0417990000000001</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1.6869000000000001</v>
+      </c>
     </row>
     <row r="64" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C64" s="1">
@@ -13981,8 +14314,17 @@
       <c r="E64" s="1">
         <v>0.81832099999999997</v>
       </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F64" s="1">
+        <v>0.78705800000000004</v>
+      </c>
+      <c r="G64" s="1">
+        <v>2.0641060000000002</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1.0106999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C65" s="1">
         <v>0.81935999999999998</v>
       </c>
@@ -13992,8 +14334,17 @@
       <c r="E65" s="1">
         <v>0.75904899999999997</v>
       </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="1">
+        <v>2.305107</v>
+      </c>
+      <c r="G65" s="1">
+        <v>2.1167020000000001</v>
+      </c>
+      <c r="H65" s="1">
+        <v>2.0745</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C66" s="1">
         <v>0.91157999999999995</v>
       </c>
@@ -14003,8 +14354,17 @@
       <c r="E66" s="1">
         <v>0.78934599999999999</v>
       </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="1">
+        <v>2.1936200000000001</v>
+      </c>
+      <c r="G66" s="1">
+        <v>2.1065</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1.9968999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C67" s="1">
         <v>0.75906600000000002</v>
       </c>
@@ -14014,8 +14374,17 @@
       <c r="E67" s="1">
         <v>0.68471800000000005</v>
       </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="1">
+        <v>1.462907</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0.78520000000000001</v>
+      </c>
+      <c r="H67" s="1">
+        <v>2.1349</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C68" s="1">
         <v>0.64944400000000002</v>
       </c>
@@ -14025,8 +14394,17 @@
       <c r="E68" s="1">
         <v>0.87670700000000001</v>
       </c>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="1">
+        <v>2.2234020000000001</v>
+      </c>
+      <c r="G68" s="1">
+        <v>2.1053999999999999</v>
+      </c>
+      <c r="H68" s="1">
+        <v>2.3959000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C69" s="1">
         <v>0.71206100000000006</v>
       </c>
@@ -14036,8 +14414,17 @@
       <c r="E69" s="1">
         <v>0.67848799999999998</v>
       </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="1">
+        <v>2.155516</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="H69" s="1">
+        <v>2.4024000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C70" s="1">
         <v>0.89208200000000004</v>
       </c>
@@ -14047,8 +14434,17 @@
       <c r="E70" s="1">
         <v>0.69185099999999999</v>
       </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="1">
+        <v>2.068524</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1.9870000000000001</v>
+      </c>
+      <c r="H70" s="1">
+        <v>2.0179999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C71" s="1">
         <v>0.762683</v>
       </c>
@@ -14058,8 +14454,17 @@
       <c r="E71" s="1">
         <v>0.64890099999999995</v>
       </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="1">
+        <v>2.2396600000000002</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0.5786</v>
+      </c>
+      <c r="H71" s="1">
+        <v>2.0482</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C72" s="1">
         <v>0.86239399999999999</v>
       </c>
@@ -14069,8 +14474,17 @@
       <c r="E72" s="1">
         <v>0.87242200000000003</v>
       </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="1">
+        <v>0.52576800000000001</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0.57230000000000003</v>
+      </c>
+      <c r="H72" s="1">
+        <v>2.2622</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C73" s="1">
         <v>0.83010200000000001</v>
       </c>
@@ -14080,8 +14494,17 @@
       <c r="E73" s="1">
         <v>0.74698100000000001</v>
       </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="1">
+        <v>2.0760179999999999</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0.75160000000000005</v>
+      </c>
+      <c r="H73" s="1">
+        <v>2.4695999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C74" s="1">
         <v>0.64752100000000001</v>
       </c>
@@ -14091,8 +14514,17 @@
       <c r="E74" s="1">
         <v>0.86506400000000006</v>
       </c>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="1">
+        <v>0.68562299999999998</v>
+      </c>
+      <c r="G74" s="1">
+        <v>16.164003000000001</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0.78339999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C75" s="1">
         <v>0.76133399999999996</v>
       </c>
@@ -14102,8 +14534,17 @@
       <c r="E75" s="1">
         <v>0.74003399999999997</v>
       </c>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F75" s="1">
+        <v>2.1583320000000001</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0.44519999999999998</v>
+      </c>
+      <c r="H75" s="1">
+        <v>2.206</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C76" s="1">
         <v>0.71553199999999995</v>
       </c>
@@ -14113,8 +14554,17 @@
       <c r="E76" s="1">
         <v>0.77296399999999998</v>
       </c>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F76" s="1">
+        <v>0.71506199999999998</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1.6976</v>
+      </c>
+      <c r="H76" s="1">
+        <v>2.2722000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C77" s="1">
         <v>0.72136</v>
       </c>
@@ -14124,8 +14574,17 @@
       <c r="E77" s="1">
         <v>0.77819799999999995</v>
       </c>
-    </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F77" s="1">
+        <v>0.73415799999999998</v>
+      </c>
+      <c r="G77" s="1">
+        <v>2.1623999999999999</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0.62180000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C78" s="1">
         <v>0.84052400000000005</v>
       </c>
@@ -14135,8 +14594,17 @@
       <c r="E78" s="1">
         <v>0.737514</v>
       </c>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="1">
+        <v>0.72089999999999999</v>
+      </c>
+      <c r="G78" s="1">
+        <v>2.1713990000000001</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.71379999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C79" s="1">
         <v>0.69303700000000001</v>
       </c>
@@ -14146,8 +14614,17 @@
       <c r="E79" s="1">
         <v>0.80888899999999997</v>
       </c>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="1">
+        <v>0.68857000000000002</v>
+      </c>
+      <c r="G79" s="1">
+        <v>2.1038999999999999</v>
+      </c>
+      <c r="H79" s="1">
+        <v>2.0684999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C80" s="1">
         <v>0.54903500000000005</v>
       </c>
@@ -14157,8 +14634,17 @@
       <c r="E80" s="1">
         <v>0.73319299999999998</v>
       </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="1">
+        <v>0.51227699999999998</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1.9879</v>
+      </c>
+      <c r="H80" s="1">
+        <v>2.3719000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C81" s="1">
         <v>0.88204800000000005</v>
       </c>
@@ -14168,8 +14654,17 @@
       <c r="E81" s="1">
         <v>0.78371199999999996</v>
       </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="1">
+        <v>2.0269529999999998</v>
+      </c>
+      <c r="G81" s="1">
+        <v>2.1147999999999998</v>
+      </c>
+      <c r="H81" s="1">
+        <v>2.1154000000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C82" s="1">
         <v>0.74553899999999995</v>
       </c>
@@ -14179,8 +14674,17 @@
       <c r="E82" s="1">
         <v>0.86318600000000001</v>
       </c>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="1">
+        <v>0.61229999999999996</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0.75760000000000005</v>
+      </c>
+      <c r="H82" s="1">
+        <v>2.2669000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C83" s="1">
         <v>0.68112499999999998</v>
       </c>
@@ -14190,8 +14694,17 @@
       <c r="E83" s="1">
         <v>0.88345799999999997</v>
       </c>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="1">
+        <v>0.59530000000000005</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1.5176000000000001</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0.76049999999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C84" s="1">
         <v>0.92895000000000005</v>
       </c>
@@ -14201,8 +14714,17 @@
       <c r="E84" s="1">
         <v>0.79976400000000003</v>
       </c>
-    </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="1">
+        <v>0.32256499999999999</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0.72789999999999999</v>
+      </c>
+      <c r="H84" s="1">
+        <v>2.2892999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C85" s="1">
         <v>0.78721200000000002</v>
       </c>
@@ -14212,8 +14734,17 @@
       <c r="E85" s="1">
         <v>1.547882</v>
       </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F85" s="1">
+        <v>0.52096900000000002</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="H85" s="1">
+        <v>2.2492999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C86" s="1">
         <v>0.78351199999999999</v>
       </c>
@@ -14223,8 +14754,17 @@
       <c r="E86" s="1">
         <v>0.73259200000000002</v>
       </c>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F86" s="1">
+        <v>0.55114200000000002</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2.1200999999999999</v>
+      </c>
+      <c r="H86" s="1">
+        <v>2.1770999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C87" s="1">
         <v>0.68715700000000002</v>
       </c>
@@ -14234,8 +14774,17 @@
       <c r="E87" s="1">
         <v>0.76471</v>
       </c>
-    </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F87" s="1">
+        <v>2.109</v>
+      </c>
+      <c r="G87" s="1">
+        <v>2.1053999999999999</v>
+      </c>
+      <c r="H87" s="1">
+        <v>2.2799</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C88" s="1">
         <v>1.112044</v>
       </c>
@@ -14245,8 +14794,17 @@
       <c r="E88" s="1">
         <v>0.68297600000000003</v>
       </c>
-    </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F88" s="1">
+        <v>2.2658</v>
+      </c>
+      <c r="G88" s="1">
+        <v>2.1336010000000001</v>
+      </c>
+      <c r="H88" s="1">
+        <v>1.3001</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C89" s="1">
         <v>0.83216100000000004</v>
       </c>
@@ -14256,8 +14814,17 @@
       <c r="E89" s="1">
         <v>0.79974699999999999</v>
       </c>
-    </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F89" s="1">
+        <v>0.74682899999999997</v>
+      </c>
+      <c r="G89" s="1">
+        <v>2.1396000000000002</v>
+      </c>
+      <c r="H89" s="1">
+        <v>2.3134000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C90" s="1">
         <v>0.78481699999999999</v>
       </c>
@@ -14267,8 +14834,17 @@
       <c r="E90" s="1">
         <v>0.77412899999999996</v>
       </c>
-    </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F90" s="1">
+        <v>0.40058899999999997</v>
+      </c>
+      <c r="G90" s="1">
+        <v>2.0501</v>
+      </c>
+      <c r="H90" s="1">
+        <v>1.4937</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C91" s="1">
         <v>0.86673299999999998</v>
       </c>
@@ -14278,8 +14854,17 @@
       <c r="E91" s="1">
         <v>0.70535899999999996</v>
       </c>
-    </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F91" s="1">
+        <v>0.50132500000000002</v>
+      </c>
+      <c r="G91" s="1">
+        <v>1.917</v>
+      </c>
+      <c r="H91" s="1">
+        <v>2.2406999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C92" s="1">
         <v>0.68374699999999999</v>
       </c>
@@ -14289,8 +14874,17 @@
       <c r="E92" s="1">
         <v>0.68293999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F92" s="1">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="G92" s="1">
+        <v>2.1974</v>
+      </c>
+      <c r="H92" s="1">
+        <v>2.1758000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C93" s="1">
         <v>0.70189000000000001</v>
       </c>
@@ -14300,8 +14894,17 @@
       <c r="E93" s="1">
         <v>0.79358099999999998</v>
       </c>
-    </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F93" s="1">
+        <v>2.3065000000000002</v>
+      </c>
+      <c r="G93" s="1">
+        <v>1.1146</v>
+      </c>
+      <c r="H93" s="1">
+        <v>2.2966000000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C94" s="1">
         <v>0.72456799999999999</v>
       </c>
@@ -14311,8 +14914,17 @@
       <c r="E94" s="1">
         <v>0.72667800000000005</v>
       </c>
-    </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F94" s="1">
+        <v>0.77680000000000005</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.65080000000000005</v>
+      </c>
+      <c r="H94" s="1">
+        <v>2.3344</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C95" s="1">
         <v>0.76644500000000004</v>
       </c>
@@ -14322,8 +14934,17 @@
       <c r="E95" s="1">
         <v>0.75847500000000001</v>
       </c>
-    </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F95" s="1">
+        <v>0.761629</v>
+      </c>
+      <c r="G95" s="1">
+        <v>2.1427999999999998</v>
+      </c>
+      <c r="H95" s="1">
+        <v>1.1449</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C96" s="1">
         <v>0.67802799999999996</v>
       </c>
@@ -14333,8 +14954,17 @@
       <c r="E96" s="1">
         <v>0.9002</v>
       </c>
-    </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F96" s="1">
+        <v>0.36520000000000002</v>
+      </c>
+      <c r="G96" s="1">
+        <v>2.1303000000000001</v>
+      </c>
+      <c r="H96" s="1">
+        <v>2.2029000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C97" s="1">
         <v>0.64792700000000003</v>
       </c>
@@ -14344,8 +14974,17 @@
       <c r="E97" s="1">
         <v>0.79461099999999996</v>
       </c>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F97" s="1">
+        <v>0.59419999999999995</v>
+      </c>
+      <c r="G97" s="1">
+        <v>2.2231000000000001</v>
+      </c>
+      <c r="H97" s="1">
+        <v>2.168701</v>
+      </c>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C98" s="1">
         <v>0.85885400000000001</v>
       </c>
@@ -14355,8 +14994,17 @@
       <c r="E98" s="1">
         <v>0.67509799999999998</v>
       </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F98" s="1">
+        <v>0.70450000000000002</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0.69710000000000005</v>
+      </c>
+      <c r="H98" s="1">
+        <v>2.2319</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C99" s="1">
         <v>0.69564599999999999</v>
       </c>
@@ -14366,8 +15014,17 @@
       <c r="E99" s="1">
         <v>0.84537499999999999</v>
       </c>
-    </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F99" s="1">
+        <v>0.64224000000000003</v>
+      </c>
+      <c r="G99" s="1">
+        <v>1.2013</v>
+      </c>
+      <c r="H99" s="1">
+        <v>1.7444999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C100" s="1">
         <v>0.88511700000000004</v>
       </c>
@@ -14377,8 +15034,17 @@
       <c r="E100" s="1">
         <v>0.90619300000000003</v>
       </c>
-    </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F100" s="1">
+        <v>0.76395000000000002</v>
+      </c>
+      <c r="G100" s="1">
+        <v>7.8564999999999996</v>
+      </c>
+      <c r="H100" s="1">
+        <v>2.2395</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C101" s="1">
         <v>0.90761400000000003</v>
       </c>
@@ -14388,8 +15054,17 @@
       <c r="E101" s="1">
         <v>0.79499399999999998</v>
       </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F101" s="1">
+        <v>0.950125</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="H101" s="1">
+        <v>2.2126000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C102" s="1">
         <v>0.76038899999999998</v>
       </c>
@@ -14399,8 +15074,17 @@
       <c r="E102" s="1">
         <v>0.90713600000000005</v>
       </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F102" s="1">
+        <v>0.92120000000000002</v>
+      </c>
+      <c r="G102" s="1">
+        <v>2.0369000000000002</v>
+      </c>
+      <c r="H102" s="1">
+        <v>2.1875</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C103" s="1">
         <v>0.33665699999999998</v>
       </c>
@@ -14410,8 +15094,17 @@
       <c r="E103" s="1">
         <v>0.70008999999999999</v>
       </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F103" s="1">
+        <v>1.512</v>
+      </c>
+      <c r="G103" s="1">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="H103" s="1">
+        <v>2.1412</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C104" s="1">
         <v>0.79938100000000001</v>
       </c>
@@ -14421,8 +15114,17 @@
       <c r="E104" s="1">
         <v>0.81062100000000004</v>
       </c>
-    </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F104" s="1">
+        <v>0.97970000000000002</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1.9905999999999999</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0.66320000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C105" s="1">
         <v>0.79464599999999996</v>
       </c>
@@ -14432,8 +15134,17 @@
       <c r="E105" s="1">
         <v>0.885351</v>
       </c>
-    </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F105" s="1">
+        <v>0.73608399999999996</v>
+      </c>
+      <c r="G105" s="1">
+        <v>2.0085000000000002</v>
+      </c>
+      <c r="H105" s="1">
+        <v>2.1019000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C106" s="1">
         <v>0.90524499999999997</v>
       </c>
@@ -14443,8 +15154,17 @@
       <c r="E106" s="1">
         <v>0.72577999999999998</v>
       </c>
-    </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F106" s="1">
+        <v>0.51975000000000005</v>
+      </c>
+      <c r="G106" s="1">
+        <v>2.081</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C107" s="1">
         <v>0.84301199999999998</v>
       </c>
@@ -14454,8 +15174,17 @@
       <c r="E107" s="1">
         <v>0.83210399999999995</v>
       </c>
-    </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F107" s="1">
+        <v>0.68917300000000004</v>
+      </c>
+      <c r="G107" s="1">
+        <v>2.2107000000000001</v>
+      </c>
+      <c r="H107" s="1">
+        <v>2.1686000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C108" s="1">
         <v>0.75378199999999995</v>
       </c>
@@ -14465,8 +15194,17 @@
       <c r="E108" s="1">
         <v>0.70525300000000002</v>
       </c>
-    </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F108" s="1">
+        <v>0.673369</v>
+      </c>
+      <c r="G108" s="1">
+        <v>1.9679</v>
+      </c>
+      <c r="H108" s="1">
+        <v>2.1269999999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C109" s="1">
         <v>0.70543699999999998</v>
       </c>
@@ -14476,8 +15214,17 @@
       <c r="E109" s="1">
         <v>0.600943</v>
       </c>
-    </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F109" s="1">
+        <v>1.875577</v>
+      </c>
+      <c r="G109" s="1">
+        <v>2.2561</v>
+      </c>
+      <c r="H109" s="1">
+        <v>2.3087</v>
+      </c>
+    </row>
+    <row r="110" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C110" s="1">
         <v>0.68185200000000001</v>
       </c>
@@ -14487,8 +15234,17 @@
       <c r="E110" s="1">
         <v>0.85359300000000005</v>
       </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F110" s="1">
+        <v>0.60817200000000005</v>
+      </c>
+      <c r="G110" s="1">
+        <v>2.1078000000000001</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0.84019999999999995</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C111" s="1">
         <v>0.78667399999999998</v>
       </c>
@@ -14498,8 +15254,17 @@
       <c r="E111" s="1">
         <v>0.82006999999999997</v>
       </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F111" s="1">
+        <v>2.0904280000000002</v>
+      </c>
+      <c r="G111" s="1">
+        <v>2.1762990000000002</v>
+      </c>
+      <c r="H111" s="1">
+        <v>2.1025999999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C112" s="1">
         <v>0.81468799999999997</v>
       </c>
@@ -14509,8 +15274,17 @@
       <c r="E112" s="1">
         <v>0.77262200000000003</v>
       </c>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F112" s="1">
+        <v>0.86645300000000003</v>
+      </c>
+      <c r="G112" s="1">
+        <v>2.1686000000000001</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0.61309999999999998</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C113" s="1">
         <v>0.90632199999999996</v>
       </c>
@@ -14520,8 +15294,17 @@
       <c r="E113" s="1">
         <v>0.76948099999999997</v>
       </c>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F113" s="1">
+        <v>0.60338000000000003</v>
+      </c>
+      <c r="G113" s="1">
+        <v>2.157</v>
+      </c>
+      <c r="H113" s="1">
+        <v>2.2326999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C114" s="1">
         <v>0.69210400000000005</v>
       </c>
@@ -14531,8 +15314,17 @@
       <c r="E114" s="1">
         <v>0.81840100000000005</v>
       </c>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F114" s="1">
+        <v>0.79668000000000005</v>
+      </c>
+      <c r="G114" s="1">
+        <v>2.1954989999999999</v>
+      </c>
+      <c r="H114" s="1">
+        <v>2.2195</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C115" s="1">
         <v>0.71613499999999997</v>
       </c>
@@ -14542,8 +15334,17 @@
       <c r="E115" s="1">
         <v>0.35300799999999999</v>
       </c>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F115" s="1">
+        <v>0.377305</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1.9450000000000001</v>
+      </c>
+      <c r="H115" s="1">
+        <v>2.2075999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C116" s="1">
         <v>0.780671</v>
       </c>
@@ -14553,8 +15354,17 @@
       <c r="E116" s="1">
         <v>0.947322</v>
       </c>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F116" s="1">
+        <v>2.2788759999999999</v>
+      </c>
+      <c r="G116" s="1">
+        <v>1.9536009999999999</v>
+      </c>
+      <c r="H116" s="1">
+        <v>2.3584000000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C117" s="1">
         <v>0.72570000000000001</v>
       </c>
@@ -14564,8 +15374,17 @@
       <c r="E117" s="1">
         <v>0.75663899999999995</v>
       </c>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F117" s="1">
+        <v>1.9753069999999999</v>
+      </c>
+      <c r="G117" s="1">
+        <v>2.1021000000000001</v>
+      </c>
+      <c r="H117" s="1">
+        <v>2.3028</v>
+      </c>
+    </row>
+    <row r="118" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C118" s="1">
         <v>0.84208799999999995</v>
       </c>
@@ -14575,8 +15394,17 @@
       <c r="E118" s="1">
         <v>0.74223600000000001</v>
       </c>
-    </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F118" s="1">
+        <v>0.79130999999999996</v>
+      </c>
+      <c r="G118" s="1">
+        <v>2.0806</v>
+      </c>
+      <c r="H118" s="1">
+        <v>0.74909999999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C119" s="1">
         <v>0.79130800000000001</v>
       </c>
@@ -14586,8 +15414,17 @@
       <c r="E119" s="1">
         <v>0.80823299999999998</v>
       </c>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F119" s="1">
+        <v>2.0543390000000001</v>
+      </c>
+      <c r="G119" s="1">
+        <v>2.0813999999999999</v>
+      </c>
+      <c r="H119" s="1">
+        <v>2.105</v>
+      </c>
+    </row>
+    <row r="120" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C120" s="1">
         <v>0.82641699999999996</v>
       </c>
@@ -14597,8 +15434,17 @@
       <c r="E120" s="1">
         <v>0.784501</v>
       </c>
-    </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F120" s="1">
+        <v>1.25844</v>
+      </c>
+      <c r="G120" s="1">
+        <v>2.0510000000000002</v>
+      </c>
+      <c r="H120" s="1">
+        <v>2.2768000000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C121" s="1">
         <v>0.72867000000000004</v>
       </c>
@@ -14608,8 +15454,17 @@
       <c r="E121" s="1">
         <v>0.73262499999999997</v>
       </c>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F121" s="1">
+        <v>1.8656999999999999</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0.97050000000000003</v>
+      </c>
+      <c r="H121" s="1">
+        <v>2.274</v>
+      </c>
+    </row>
+    <row r="122" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C122" s="1">
         <v>0.67852599999999996</v>
       </c>
@@ -14619,8 +15474,17 @@
       <c r="E122" s="1">
         <v>0.73019299999999998</v>
       </c>
-    </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F122" s="1">
+        <v>0.75776600000000005</v>
+      </c>
+      <c r="G122" s="1">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="H122" s="1">
+        <v>2.0514999999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C123" s="1">
         <v>0.83281700000000003</v>
       </c>
@@ -14630,8 +15494,17 @@
       <c r="E123" s="1">
         <v>0.75409099999999996</v>
       </c>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F123" s="1">
+        <v>0.65702099999999997</v>
+      </c>
+      <c r="G123" s="1">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="H123" s="1">
+        <v>2.2823000000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C124" s="1">
         <v>0.78771800000000003</v>
       </c>
@@ -14641,8 +15514,17 @@
       <c r="E124" s="1">
         <v>0.801373</v>
       </c>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F124" s="1">
+        <v>0.82142999999999999</v>
+      </c>
+      <c r="G124" s="1">
+        <v>0.59540000000000004</v>
+      </c>
+      <c r="H124" s="1">
+        <v>2.1436999999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C125" s="1">
         <v>0.90821300000000005</v>
       </c>
@@ -14652,8 +15534,17 @@
       <c r="E125" s="1">
         <v>0.78613999999999995</v>
       </c>
-    </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F125" s="1">
+        <v>2.0169489999999999</v>
+      </c>
+      <c r="G125" s="1">
+        <v>0.51970000000000005</v>
+      </c>
+      <c r="H125" s="1">
+        <v>2.2155999999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C126" s="1">
         <v>0.74535600000000002</v>
       </c>
@@ -14663,8 +15554,17 @@
       <c r="E126" s="1">
         <v>0.750197</v>
       </c>
-    </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F126" s="1">
+        <v>0.46151999999999999</v>
+      </c>
+      <c r="G126" s="1">
+        <v>2.0362010000000001</v>
+      </c>
+      <c r="H126" s="1">
+        <v>2.2498990000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C127" s="1">
         <v>0.76771500000000004</v>
       </c>
@@ -14674,8 +15574,17 @@
       <c r="E127" s="1">
         <v>0.82649899999999998</v>
       </c>
-    </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F127" s="1">
+        <v>2.0331779999999999</v>
+      </c>
+      <c r="G127" s="1">
+        <v>2.1516000000000002</v>
+      </c>
+      <c r="H127" s="1">
+        <v>2.0825999999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C128" s="1">
         <v>0.87634999999999996</v>
       </c>
@@ -14685,8 +15594,17 @@
       <c r="E128" s="1">
         <v>0.75872799999999996</v>
       </c>
-    </row>
-    <row r="129" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F128" s="1">
+        <v>1.0439099999999999</v>
+      </c>
+      <c r="G128" s="1">
+        <v>2.0789</v>
+      </c>
+      <c r="H128" s="1">
+        <v>2.3508010000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C129" s="1">
         <v>0.86241599999999996</v>
       </c>
@@ -14696,8 +15614,17 @@
       <c r="E129" s="1">
         <v>0.83432899999999999</v>
       </c>
-    </row>
-    <row r="130" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F129" s="1">
+        <v>2.1260439999999998</v>
+      </c>
+      <c r="G129" s="1">
+        <v>1.4693000000000001</v>
+      </c>
+      <c r="H129" s="1">
+        <v>2.2077</v>
+      </c>
+    </row>
+    <row r="130" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C130" s="1">
         <v>0.85241699999999998</v>
       </c>
@@ -14707,8 +15634,17 @@
       <c r="E130" s="1">
         <v>0.68447499999999994</v>
       </c>
-    </row>
-    <row r="131" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F130" s="1">
+        <v>2.2300430000000002</v>
+      </c>
+      <c r="G130" s="1">
+        <v>0.89929999999999999</v>
+      </c>
+      <c r="H130" s="1">
+        <v>2.2349999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C131" s="1">
         <v>6.8071210000000004</v>
       </c>
@@ -14718,8 +15654,17 @@
       <c r="E131" s="1">
         <v>0.84056399999999998</v>
       </c>
-    </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F131" s="1">
+        <v>1.96461</v>
+      </c>
+      <c r="G131" s="1">
+        <v>2.1393</v>
+      </c>
+      <c r="H131" s="1">
+        <v>2.2162999999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C132" s="1">
         <v>0.75847699999999996</v>
       </c>
@@ -14729,8 +15674,17 @@
       <c r="E132" s="1">
         <v>0.72329399999999999</v>
       </c>
-    </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F132" s="1">
+        <v>2.0017459999999998</v>
+      </c>
+      <c r="G132" s="1">
+        <v>1.9209000000000001</v>
+      </c>
+      <c r="H132" s="1">
+        <v>2.0066999999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C133" s="1">
         <v>0.78572600000000004</v>
       </c>
@@ -14740,8 +15694,17 @@
       <c r="E133" s="1">
         <v>0.77060099999999998</v>
       </c>
-    </row>
-    <row r="134" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F133" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="G133" s="1">
+        <v>2.2395999999999998</v>
+      </c>
+      <c r="H133" s="1">
+        <v>2.1225000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C134" s="1">
         <v>0.75404300000000002</v>
       </c>
@@ -14751,8 +15714,17 @@
       <c r="E134" s="1">
         <v>0.84450700000000001</v>
       </c>
-    </row>
-    <row r="135" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F134" s="1">
+        <v>1.9410179999999999</v>
+      </c>
+      <c r="G134" s="1">
+        <v>2.1852</v>
+      </c>
+      <c r="H134" s="1">
+        <v>0.74680100000000005</v>
+      </c>
+    </row>
+    <row r="135" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C135" s="1">
         <v>0.80219200000000002</v>
       </c>
@@ -14762,8 +15734,17 @@
       <c r="E135" s="1">
         <v>0.80886100000000005</v>
       </c>
-    </row>
-    <row r="136" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F135" s="1">
+        <v>1.33677</v>
+      </c>
+      <c r="G135" s="1">
+        <v>2.1396999999999999</v>
+      </c>
+      <c r="H135" s="1">
+        <v>2.3085</v>
+      </c>
+    </row>
+    <row r="136" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C136" s="1">
         <v>0.82962100000000005</v>
       </c>
@@ -14773,8 +15754,17 @@
       <c r="E136" s="1">
         <v>0.76247799999999999</v>
       </c>
-    </row>
-    <row r="137" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F136" s="1">
+        <v>2.0282119999999999</v>
+      </c>
+      <c r="G136" s="1">
+        <v>0.73809999999999998</v>
+      </c>
+      <c r="H136" s="1">
+        <v>2.2968999999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C137" s="1">
         <v>0.77792600000000001</v>
       </c>
@@ -14784,8 +15774,17 @@
       <c r="E137" s="1">
         <v>0.84668299999999996</v>
       </c>
-    </row>
-    <row r="138" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F137" s="1">
+        <v>0.55415800000000004</v>
+      </c>
+      <c r="G137" s="1">
+        <v>2.0996000000000001</v>
+      </c>
+      <c r="H137" s="1">
+        <v>0.6573</v>
+      </c>
+    </row>
+    <row r="138" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C138" s="1">
         <v>0.71061099999999999</v>
       </c>
@@ -14795,8 +15794,17 @@
       <c r="E138" s="1">
         <v>0.78949899999999995</v>
       </c>
-    </row>
-    <row r="139" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F138" s="1">
+        <v>0.64344900000000005</v>
+      </c>
+      <c r="G138" s="1">
+        <v>2.1284999999999998</v>
+      </c>
+      <c r="H138" s="1">
+        <v>2.3155999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C139" s="1">
         <v>0.68410300000000002</v>
       </c>
@@ -14806,8 +15814,17 @@
       <c r="E139" s="1">
         <v>0.77627500000000005</v>
       </c>
-    </row>
-    <row r="140" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F139" s="1">
+        <v>2.0022489999999999</v>
+      </c>
+      <c r="G139" s="1">
+        <v>2.1345999999999998</v>
+      </c>
+      <c r="H139" s="1">
+        <v>2.1234999999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C140" s="1">
         <v>0.72754099999999999</v>
       </c>
@@ -14817,8 +15834,17 @@
       <c r="E140" s="1">
         <v>0.73770100000000005</v>
       </c>
-    </row>
-    <row r="141" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F140" s="1">
+        <v>1.790529</v>
+      </c>
+      <c r="G140" s="1">
+        <v>1.9153</v>
+      </c>
+      <c r="H140" s="1">
+        <v>2.311601</v>
+      </c>
+    </row>
+    <row r="141" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C141" s="1">
         <v>0.80937499999999996</v>
       </c>
@@ -14828,8 +15854,17 @@
       <c r="E141" s="1">
         <v>0.82902500000000001</v>
       </c>
-    </row>
-    <row r="142" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F141" s="1">
+        <v>0.73741900000000005</v>
+      </c>
+      <c r="G141" s="1">
+        <v>1.9724999999999999</v>
+      </c>
+      <c r="H141" s="1">
+        <v>2.2495989999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C142" s="1">
         <v>0.70611000000000002</v>
       </c>
@@ -14839,8 +15874,17 @@
       <c r="E142" s="1">
         <v>35.456567999999997</v>
       </c>
-    </row>
-    <row r="143" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F142" s="1">
+        <v>0.64052699999999996</v>
+      </c>
+      <c r="G142" s="1">
+        <v>2.1722000000000001</v>
+      </c>
+      <c r="H142" s="1">
+        <v>2.0322990000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C143" s="1">
         <v>0.50608600000000004</v>
       </c>
@@ -14850,8 +15894,17 @@
       <c r="E143" s="1">
         <v>0.724298</v>
       </c>
-    </row>
-    <row r="144" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F143" s="1">
+        <v>1.941883</v>
+      </c>
+      <c r="G143" s="1">
+        <v>2.2126999999999999</v>
+      </c>
+      <c r="H143" s="1">
+        <v>2.1385999999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C144" s="1">
         <v>0.74977499999999997</v>
       </c>
@@ -14861,8 +15914,17 @@
       <c r="E144" s="1">
         <v>0.760382</v>
       </c>
-    </row>
-    <row r="145" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F144" s="1">
+        <v>0.41566900000000001</v>
+      </c>
+      <c r="G144" s="1">
+        <v>2.1846999999999999</v>
+      </c>
+      <c r="H144" s="1">
+        <v>2.0459999999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C145" s="1">
         <v>0.74443700000000002</v>
       </c>
@@ -14872,8 +15934,17 @@
       <c r="E145" s="1">
         <v>0.70494100000000004</v>
       </c>
-    </row>
-    <row r="146" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F145" s="1">
+        <v>0.70222200000000001</v>
+      </c>
+      <c r="G145" s="1">
+        <v>0.3508</v>
+      </c>
+      <c r="H145" s="1">
+        <v>2.4889999999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C146" s="1">
         <v>0.83455599999999996</v>
       </c>
@@ -14883,8 +15954,17 @@
       <c r="E146" s="1">
         <v>0.69096800000000003</v>
       </c>
-    </row>
-    <row r="147" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F146" s="1">
+        <v>2.0372439999999998</v>
+      </c>
+      <c r="G146" s="1">
+        <v>1.9386000000000001</v>
+      </c>
+      <c r="H146" s="1">
+        <v>2.2873000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C147" s="1">
         <v>0.94970600000000005</v>
       </c>
@@ -14894,8 +15974,17 @@
       <c r="E147" s="1">
         <v>0.75394899999999998</v>
       </c>
-    </row>
-    <row r="148" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F147" s="1">
+        <v>2.1210819999999999</v>
+      </c>
+      <c r="G147" s="1">
+        <v>1.9834000000000001</v>
+      </c>
+      <c r="H147" s="1">
+        <v>1.9375009999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C148" s="1">
         <v>0.65429899999999996</v>
       </c>
@@ -14905,8 +15994,17 @@
       <c r="E148" s="1">
         <v>0.78361899999999995</v>
       </c>
-    </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F148" s="1">
+        <v>2.217632</v>
+      </c>
+      <c r="G148" s="1">
+        <v>2.0379</v>
+      </c>
+      <c r="H148" s="1">
+        <v>1.9755</v>
+      </c>
+    </row>
+    <row r="149" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C149" s="1">
         <v>0.76465300000000003</v>
       </c>
@@ -14916,8 +16014,17 @@
       <c r="E149" s="1">
         <v>0.67184299999999997</v>
       </c>
-    </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F149" s="1">
+        <v>2.0695939999999999</v>
+      </c>
+      <c r="G149" s="1">
+        <v>2.1572</v>
+      </c>
+      <c r="H149" s="1">
+        <v>2.2629000000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C150" s="1">
         <v>0.63072799999999996</v>
       </c>
@@ -14927,8 +16034,17 @@
       <c r="E150" s="1">
         <v>0.67306900000000003</v>
       </c>
-    </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F150" s="1">
+        <v>1.650528</v>
+      </c>
+      <c r="G150" s="1">
+        <v>0.75080000000000002</v>
+      </c>
+      <c r="H150" s="1">
+        <v>1.9174</v>
+      </c>
+    </row>
+    <row r="151" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C151" s="1">
         <v>0.60566699999999996</v>
       </c>
@@ -14938,8 +16054,17 @@
       <c r="E151" s="1">
         <v>0.82058600000000004</v>
       </c>
-    </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F151" s="1">
+        <v>1.9983709999999999</v>
+      </c>
+      <c r="G151" s="1">
+        <v>0.75280000000000002</v>
+      </c>
+      <c r="H151" s="1">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="152" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C152" s="1">
         <v>0.62484499999999998</v>
       </c>
@@ -14949,8 +16074,17 @@
       <c r="E152" s="1">
         <v>0.69089500000000004</v>
       </c>
-    </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F152" s="1">
+        <v>0.30229800000000001</v>
+      </c>
+      <c r="G152" s="1">
+        <v>0.6079</v>
+      </c>
+      <c r="H152" s="1">
+        <v>1.3368</v>
+      </c>
+    </row>
+    <row r="153" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C153" s="1">
         <v>0.88849199999999995</v>
       </c>
@@ -14960,8 +16094,17 @@
       <c r="E153" s="1">
         <v>0.62897899999999995</v>
       </c>
-    </row>
-    <row r="154" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F153" s="1">
+        <v>0.70255199999999995</v>
+      </c>
+      <c r="G153" s="1">
+        <v>0.47839999999999999</v>
+      </c>
+      <c r="H153" s="1">
+        <v>2.0316999999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C154" s="1">
         <v>0.74446100000000004</v>
       </c>
@@ -14971,8 +16114,17 @@
       <c r="E154" s="1">
         <v>0.80046200000000001</v>
       </c>
-    </row>
-    <row r="155" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F154" s="1">
+        <v>1.292068</v>
+      </c>
+      <c r="G154" s="1">
+        <v>0.74690000000000001</v>
+      </c>
+      <c r="H154" s="1">
+        <v>0.78680000000000005</v>
+      </c>
+    </row>
+    <row r="155" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C155" s="1">
         <v>0.68325599999999997</v>
       </c>
@@ -14982,8 +16134,17 @@
       <c r="E155" s="1">
         <v>0.67437899999999995</v>
       </c>
-    </row>
-    <row r="156" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F155" s="1">
+        <v>2.108085</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0.59470000000000001</v>
+      </c>
+      <c r="H155" s="1">
+        <v>2.1288999999999998</v>
+      </c>
+    </row>
+    <row r="156" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C156" s="1">
         <v>0.75120900000000002</v>
       </c>
@@ -14993,8 +16154,17 @@
       <c r="E156" s="1">
         <v>0.84059700000000004</v>
       </c>
-    </row>
-    <row r="157" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F156" s="1">
+        <v>0.65423399999999998</v>
+      </c>
+      <c r="G156" s="1">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="H156" s="1">
+        <v>0.78059999999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C157" s="1">
         <v>0.79538200000000003</v>
       </c>
@@ -15004,8 +16174,17 @@
       <c r="E157" s="1">
         <v>0.79325199999999996</v>
       </c>
-    </row>
-    <row r="158" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F157" s="1">
+        <v>0.71229299999999995</v>
+      </c>
+      <c r="G157" s="1">
+        <v>0.74390000000000001</v>
+      </c>
+      <c r="H157" s="1">
+        <v>2.3424999999999998</v>
+      </c>
+    </row>
+    <row r="158" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C158" s="1">
         <v>0.82598499999999997</v>
       </c>
@@ -15015,8 +16194,17 @@
       <c r="E158" s="1">
         <v>0.70333500000000004</v>
       </c>
-    </row>
-    <row r="159" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F158" s="1">
+        <v>2.0136409999999998</v>
+      </c>
+      <c r="G158" s="1">
+        <v>0.47060000000000002</v>
+      </c>
+      <c r="H158" s="1">
+        <v>0.50029999999999997</v>
+      </c>
+    </row>
+    <row r="159" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C159" s="1">
         <v>0.72479800000000005</v>
       </c>
@@ -15026,8 +16214,17 @@
       <c r="E159" s="1">
         <v>0.83552300000000002</v>
       </c>
-    </row>
-    <row r="160" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F159" s="1">
+        <v>2.354371</v>
+      </c>
+      <c r="G159" s="1">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="H159" s="1">
+        <v>2.3210000000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C160" s="1">
         <v>0.74166500000000002</v>
       </c>
@@ -15037,8 +16234,17 @@
       <c r="E160" s="1">
         <v>0.72162999999999999</v>
       </c>
-    </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F160" s="1">
+        <v>2.8368169999999999</v>
+      </c>
+      <c r="G160" s="1">
+        <v>0.51280000000000003</v>
+      </c>
+      <c r="H160" s="1">
+        <v>2.3532999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C161" s="1">
         <v>0.686199</v>
       </c>
@@ -15048,8 +16254,17 @@
       <c r="E161" s="1">
         <v>0.71606400000000003</v>
       </c>
-    </row>
-    <row r="162" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F161" s="1">
+        <v>2.4275319999999998</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0.63180000000000003</v>
+      </c>
+      <c r="H161" s="1">
+        <v>0.81610000000000005</v>
+      </c>
+    </row>
+    <row r="162" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C162" s="1">
         <v>0.83666099999999999</v>
       </c>
@@ -15059,8 +16274,17 @@
       <c r="E162" s="1">
         <v>0.66725199999999996</v>
       </c>
-    </row>
-    <row r="163" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F162" s="1">
+        <v>1.0018</v>
+      </c>
+      <c r="G162" s="1">
+        <v>25.616902</v>
+      </c>
+      <c r="H162" s="1">
+        <v>0.7944</v>
+      </c>
+    </row>
+    <row r="163" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C163" s="1">
         <v>0.80331399999999997</v>
       </c>
@@ -15070,8 +16294,17 @@
       <c r="E163" s="1">
         <v>0.76930799999999999</v>
       </c>
-    </row>
-    <row r="164" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F163" s="1">
+        <v>2.160301</v>
+      </c>
+      <c r="G163" s="1">
+        <v>0.5101</v>
+      </c>
+      <c r="H163" s="1">
+        <v>2.1894</v>
+      </c>
+    </row>
+    <row r="164" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C164" s="1">
         <v>0.73815900000000001</v>
       </c>
@@ -15081,8 +16314,17 @@
       <c r="E164" s="1">
         <v>0.69089</v>
       </c>
-    </row>
-    <row r="165" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F164" s="1">
+        <v>2.3610959999999999</v>
+      </c>
+      <c r="G164" s="1">
+        <v>0.50760000000000005</v>
+      </c>
+      <c r="H164" s="1">
+        <v>2.1751999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C165" s="1">
         <v>0.81269199999999997</v>
       </c>
@@ -15092,8 +16334,17 @@
       <c r="E165" s="1">
         <v>0.80845400000000001</v>
       </c>
-    </row>
-    <row r="166" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F165" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="G165" s="1">
+        <v>0.502</v>
+      </c>
+      <c r="H165" s="1">
+        <v>2.2301000000000002</v>
+      </c>
+    </row>
+    <row r="166" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C166" s="1">
         <v>0.67544300000000002</v>
       </c>
@@ -15103,8 +16354,17 @@
       <c r="E166" s="1">
         <v>0.633691</v>
       </c>
-    </row>
-    <row r="167" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F166" s="1">
+        <v>2.0699990000000001</v>
+      </c>
+      <c r="G166" s="1">
+        <v>0.35780000000000001</v>
+      </c>
+      <c r="H166" s="1">
+        <v>2.0655999999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C167" s="1">
         <v>1.0024580000000001</v>
       </c>
@@ -15114,8 +16374,17 @@
       <c r="E167" s="1">
         <v>0.77123299999999995</v>
       </c>
-    </row>
-    <row r="168" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F167" s="1">
+        <v>1.5863</v>
+      </c>
+      <c r="G167" s="1">
+        <v>0.60809999999999997</v>
+      </c>
+      <c r="H167" s="1">
+        <v>2.2338990000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C168" s="1">
         <v>0.66915000000000002</v>
       </c>
@@ -15125,8 +16394,17 @@
       <c r="E168" s="1">
         <v>0.88032999999999995</v>
       </c>
-    </row>
-    <row r="169" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F168" s="1">
+        <v>1.608501</v>
+      </c>
+      <c r="G168" s="1">
+        <v>0.50239999999999996</v>
+      </c>
+      <c r="H168" s="1">
+        <v>2.3045010000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C169" s="1">
         <v>0.76775899999999997</v>
       </c>
@@ -15136,8 +16414,17 @@
       <c r="E169" s="1">
         <v>0.29853200000000002</v>
       </c>
-    </row>
-    <row r="170" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F169" s="1">
+        <v>2.1899000000000002</v>
+      </c>
+      <c r="G169" s="1">
+        <v>0.62739999999999996</v>
+      </c>
+      <c r="H169" s="1">
+        <v>2.2978000000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C170" s="1">
         <v>0.68912700000000005</v>
       </c>
@@ -15147,8 +16434,17 @@
       <c r="E170" s="1">
         <v>0.90427299999999999</v>
       </c>
-    </row>
-    <row r="171" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F170" s="1">
+        <v>2.2985000000000002</v>
+      </c>
+      <c r="G170" s="1">
+        <v>0.73089999999999999</v>
+      </c>
+      <c r="H170" s="1">
+        <v>1.5597000000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C171" s="1">
         <v>0.63176299999999996</v>
       </c>
@@ -15158,8 +16454,17 @@
       <c r="E171" s="1">
         <v>0.78938600000000003</v>
       </c>
-    </row>
-    <row r="172" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F171" s="1">
+        <v>2.2696000000000001</v>
+      </c>
+      <c r="G171" s="1">
+        <v>2.0369999999999999</v>
+      </c>
+      <c r="H171" s="1">
+        <v>1.6539999999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C172" s="1">
         <v>0.77114499999999997</v>
       </c>
@@ -15169,8 +16474,17 @@
       <c r="E172" s="1">
         <v>0.623359</v>
       </c>
-    </row>
-    <row r="173" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F172" s="1">
+        <v>2.1244930000000002</v>
+      </c>
+      <c r="G172" s="1">
+        <v>2.0705960000000001</v>
+      </c>
+      <c r="H172" s="1">
+        <v>2.3275000000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C173" s="1">
         <v>0.78473400000000004</v>
       </c>
@@ -15180,8 +16494,17 @@
       <c r="E173" s="1">
         <v>0.65181999999999995</v>
       </c>
-    </row>
-    <row r="174" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F173" s="1">
+        <v>2.1581969999999999</v>
+      </c>
+      <c r="G173" s="1">
+        <v>1.371796</v>
+      </c>
+      <c r="H173" s="1">
+        <v>1.3542000000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C174" s="1">
         <v>0.82504699999999997</v>
       </c>
@@ -15191,8 +16514,17 @@
       <c r="E174" s="1">
         <v>0.88998600000000005</v>
       </c>
-    </row>
-    <row r="175" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F174" s="1">
+        <v>0.71820099999999998</v>
+      </c>
+      <c r="G174" s="1">
+        <v>1.8816949999999999</v>
+      </c>
+      <c r="H174" s="1">
+        <v>2.0762010000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C175" s="1">
         <v>0.71214299999999997</v>
       </c>
@@ -15202,8 +16534,17 @@
       <c r="E175" s="1">
         <v>0.76144800000000001</v>
       </c>
-    </row>
-    <row r="176" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F175" s="1">
+        <v>1.3473999999999999</v>
+      </c>
+      <c r="G175" s="1">
+        <v>2.044899</v>
+      </c>
+      <c r="H175" s="1">
+        <v>2.1242999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C176" s="1">
         <v>0.80823900000000004</v>
       </c>
@@ -15213,8 +16554,17 @@
       <c r="E176" s="1">
         <v>0.80663700000000005</v>
       </c>
-    </row>
-    <row r="177" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F176" s="1">
+        <v>2.0982020000000001</v>
+      </c>
+      <c r="G176" s="1">
+        <v>2.2024940000000002</v>
+      </c>
+      <c r="H176" s="1">
+        <v>1.3803000000000001</v>
+      </c>
+    </row>
+    <row r="177" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C177" s="1">
         <v>0.77197099999999996</v>
       </c>
@@ -15224,8 +16574,17 @@
       <c r="E177" s="1">
         <v>0.77683899999999995</v>
       </c>
-    </row>
-    <row r="178" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F177" s="1">
+        <v>2.2303999999999999</v>
+      </c>
+      <c r="G177" s="1">
+        <v>2.3980009999999998</v>
+      </c>
+      <c r="H177" s="1">
+        <v>2.4626000000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C178" s="1">
         <v>0.70584499999999994</v>
       </c>
@@ -15235,8 +16594,17 @@
       <c r="E178" s="1">
         <v>0.86972799999999995</v>
       </c>
-    </row>
-    <row r="179" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F178" s="1">
+        <v>1.5438989999999999</v>
+      </c>
+      <c r="G178" s="1">
+        <v>5.0854990000000004</v>
+      </c>
+      <c r="H178" s="1">
+        <v>2.2204000000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C179" s="1">
         <v>0.83099199999999995</v>
       </c>
@@ -15246,8 +16614,17 @@
       <c r="E179" s="1">
         <v>0.81690700000000005</v>
       </c>
-    </row>
-    <row r="180" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F179" s="1">
+        <v>2.1716000000000002</v>
+      </c>
+      <c r="G179" s="1">
+        <v>2.0672000000000001</v>
+      </c>
+      <c r="H179" s="1">
+        <v>2.2381000000000002</v>
+      </c>
+    </row>
+    <row r="180" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C180" s="1">
         <v>0.805674</v>
       </c>
@@ -15257,8 +16634,17 @@
       <c r="E180" s="1">
         <v>0.91868399999999995</v>
       </c>
-    </row>
-    <row r="181" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F180" s="1">
+        <v>2.3789020000000001</v>
+      </c>
+      <c r="G180" s="1">
+        <v>2.1046</v>
+      </c>
+      <c r="H180" s="1">
+        <v>2.295601</v>
+      </c>
+    </row>
+    <row r="181" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C181" s="1">
         <v>0.81303499999999995</v>
       </c>
@@ -15268,8 +16654,17 @@
       <c r="E181" s="1">
         <v>0.88416499999999998</v>
       </c>
-    </row>
-    <row r="182" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F181" s="1">
+        <v>2.2780969999999998</v>
+      </c>
+      <c r="G181" s="1">
+        <v>2.0998009999999998</v>
+      </c>
+      <c r="H181" s="1">
+        <v>0.76680000000000004</v>
+      </c>
+    </row>
+    <row r="182" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C182" s="1">
         <v>0.85013899999999998</v>
       </c>
@@ -15279,8 +16674,17 @@
       <c r="E182" s="1">
         <v>0.83289000000000002</v>
       </c>
-    </row>
-    <row r="183" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F182" s="1">
+        <v>0.59009999999999996</v>
+      </c>
+      <c r="G182" s="1">
+        <v>2.1555</v>
+      </c>
+      <c r="H182" s="1">
+        <v>2.3540990000000002</v>
+      </c>
+    </row>
+    <row r="183" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C183" s="1">
         <v>0.77280300000000002</v>
       </c>
@@ -15290,8 +16694,17 @@
       <c r="E183" s="1">
         <v>0.69267599999999996</v>
       </c>
-    </row>
-    <row r="184" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F183" s="1">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="G183" s="1">
+        <v>1.4556</v>
+      </c>
+      <c r="H183" s="1">
+        <v>2.2579989999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C184" s="1">
         <v>0.78658899999999998</v>
       </c>
@@ -15301,8 +16714,17 @@
       <c r="E184" s="1">
         <v>8.4773429999999994</v>
       </c>
-    </row>
-    <row r="185" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F184" s="1">
+        <v>2.0423040000000001</v>
+      </c>
+      <c r="G184" s="1">
+        <v>1.7048000000000001</v>
+      </c>
+      <c r="H184" s="1">
+        <v>2.1796000000000002</v>
+      </c>
+    </row>
+    <row r="185" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C185" s="1">
         <v>0.73600900000000002</v>
       </c>
@@ -15312,8 +16734,17 @@
       <c r="E185" s="1">
         <v>0.72121599999999997</v>
       </c>
-    </row>
-    <row r="186" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F185" s="1">
+        <v>2.2271000000000001</v>
+      </c>
+      <c r="G185" s="1">
+        <v>1.5281</v>
+      </c>
+      <c r="H185" s="1">
+        <v>0.47170000000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C186" s="1">
         <v>0.92170600000000003</v>
       </c>
@@ -15323,8 +16754,17 @@
       <c r="E186" s="1">
         <v>0.71726199999999996</v>
       </c>
-    </row>
-    <row r="187" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F186" s="1">
+        <v>2.2826010000000001</v>
+      </c>
+      <c r="G186" s="1">
+        <v>2.0253999999999999</v>
+      </c>
+      <c r="H186" s="1">
+        <v>2.2625999999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C187" s="1">
         <v>0.93893700000000002</v>
       </c>
@@ -15334,8 +16774,17 @@
       <c r="E187" s="1">
         <v>0.80535699999999999</v>
       </c>
-    </row>
-    <row r="188" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F187" s="1">
+        <v>0.3579</v>
+      </c>
+      <c r="G187" s="1">
+        <v>1.9652000000000001</v>
+      </c>
+      <c r="H187" s="1">
+        <v>2.2311000000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C188" s="1">
         <v>0.80275600000000003</v>
       </c>
@@ -15345,8 +16794,17 @@
       <c r="E188" s="1">
         <v>0.83602799999999999</v>
       </c>
-    </row>
-    <row r="189" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F188" s="1">
+        <v>2.0979999999999999</v>
+      </c>
+      <c r="G188" s="1">
+        <v>1.9433</v>
+      </c>
+      <c r="H188" s="1">
+        <v>0.75790000000000002</v>
+      </c>
+    </row>
+    <row r="189" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C189" s="1">
         <v>0.73965800000000004</v>
       </c>
@@ -15356,8 +16814,17 @@
       <c r="E189" s="1">
         <v>0.71397200000000005</v>
       </c>
-    </row>
-    <row r="190" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F189" s="1">
+        <v>2.1581999999999999</v>
+      </c>
+      <c r="G189" s="1">
+        <v>1.9403030000000001</v>
+      </c>
+      <c r="H189" s="1">
+        <v>2.1185999999999998</v>
+      </c>
+    </row>
+    <row r="190" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C190" s="1">
         <v>0.77812499999999996</v>
       </c>
@@ -15367,8 +16834,17 @@
       <c r="E190" s="1">
         <v>0.76131499999999996</v>
       </c>
-    </row>
-    <row r="191" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F190" s="1">
+        <v>1.673</v>
+      </c>
+      <c r="G190" s="1">
+        <v>2.1528999999999998</v>
+      </c>
+      <c r="H190" s="1">
+        <v>1.5185010000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C191" s="1">
         <v>1.4319539999999999</v>
       </c>
@@ -15378,8 +16854,17 @@
       <c r="E191" s="1">
         <v>0.81703899999999996</v>
       </c>
-    </row>
-    <row r="192" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F191" s="1">
+        <v>1.0167999999999999</v>
+      </c>
+      <c r="G191" s="1">
+        <v>0.78339999999999999</v>
+      </c>
+      <c r="H191" s="1">
+        <v>1.7515000000000001</v>
+      </c>
+    </row>
+    <row r="192" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C192" s="1">
         <v>0.79108800000000001</v>
       </c>
@@ -15389,8 +16874,17 @@
       <c r="E192" s="1">
         <v>0.72248299999999999</v>
       </c>
-    </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F192" s="1">
+        <v>2.0448040000000001</v>
+      </c>
+      <c r="G192" s="1">
+        <v>0.7288</v>
+      </c>
+      <c r="H192" s="1">
+        <v>0.87960000000000005</v>
+      </c>
+    </row>
+    <row r="193" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C193" s="1">
         <v>0.81469899999999995</v>
       </c>
@@ -15400,8 +16894,17 @@
       <c r="E193" s="1">
         <v>0.81614600000000004</v>
       </c>
-    </row>
-    <row r="194" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F193" s="1">
+        <v>2.083599</v>
+      </c>
+      <c r="G193" s="1">
+        <v>2.1487989999999999</v>
+      </c>
+      <c r="H193" s="1">
+        <v>2.2279</v>
+      </c>
+    </row>
+    <row r="194" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C194" s="1">
         <v>0.79129799999999995</v>
       </c>
@@ -15411,8 +16914,17 @@
       <c r="E194" s="1">
         <v>0.95389599999999997</v>
       </c>
-    </row>
-    <row r="195" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F194" s="1">
+        <v>2.1879</v>
+      </c>
+      <c r="G194" s="1">
+        <v>1.5698000000000001</v>
+      </c>
+      <c r="H194" s="1">
+        <v>2.3132000000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C195" s="1">
         <v>0.76603600000000005</v>
       </c>
@@ -15422,8 +16934,17 @@
       <c r="E195" s="1">
         <v>0.65790800000000005</v>
       </c>
-    </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F195" s="1">
+        <v>2.2109000000000001</v>
+      </c>
+      <c r="G195" s="1">
+        <v>2.0415999999999999</v>
+      </c>
+      <c r="H195" s="1">
+        <v>2.2221000000000002</v>
+      </c>
+    </row>
+    <row r="196" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C196" s="1">
         <v>0.68838600000000005</v>
       </c>
@@ -15433,8 +16954,17 @@
       <c r="E196" s="1">
         <v>0.73436699999999999</v>
       </c>
-    </row>
-    <row r="197" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F196" s="1">
+        <v>1.9151009999999999</v>
+      </c>
+      <c r="G196" s="1">
+        <v>0.75460000000000005</v>
+      </c>
+      <c r="H196" s="1">
+        <v>0.73540000000000005</v>
+      </c>
+    </row>
+    <row r="197" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C197" s="1">
         <v>0.77167699999999995</v>
       </c>
@@ -15444,8 +16974,17 @@
       <c r="E197" s="1">
         <v>0.90441000000000005</v>
       </c>
-    </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F197" s="1">
+        <v>2.2055989999999999</v>
+      </c>
+      <c r="G197" s="1">
+        <v>2.2408000000000001</v>
+      </c>
+      <c r="H197" s="1">
+        <v>2.1332010000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C198" s="1">
         <v>0.79523999999999995</v>
       </c>
@@ -15455,8 +16994,17 @@
       <c r="E198" s="1">
         <v>0.94897100000000001</v>
       </c>
-    </row>
-    <row r="199" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F198" s="1">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="G198" s="1">
+        <v>2.2392050000000001</v>
+      </c>
+      <c r="H198" s="1">
+        <v>2.1549999999999998</v>
+      </c>
+    </row>
+    <row r="199" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C199" s="1">
         <v>0.83272400000000002</v>
       </c>
@@ -15466,8 +17014,17 @@
       <c r="E199" s="1">
         <v>0.91170099999999998</v>
       </c>
-    </row>
-    <row r="200" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F199" s="1">
+        <v>0.65080000000000005</v>
+      </c>
+      <c r="G199" s="1">
+        <v>1.0524990000000001</v>
+      </c>
+      <c r="H199" s="1">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="200" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C200" s="1">
         <v>0.74222399999999999</v>
       </c>
@@ -15477,8 +17034,17 @@
       <c r="E200" s="1">
         <v>1.0023899999999999</v>
       </c>
-    </row>
-    <row r="201" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F200" s="1">
+        <v>0.59060100000000004</v>
+      </c>
+      <c r="G200" s="1">
+        <v>0.61739999999999995</v>
+      </c>
+      <c r="H200" s="1">
+        <v>2.2385999999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C201" s="1">
         <v>0.777563</v>
       </c>
@@ -15488,8 +17054,17 @@
       <c r="E201" s="1">
         <v>0.71531999999999996</v>
       </c>
-    </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F201" s="1">
+        <v>0.4713</v>
+      </c>
+      <c r="G201" s="1">
+        <v>2.0953010000000001</v>
+      </c>
+      <c r="H201" s="1">
+        <v>2.2370000000000001</v>
+      </c>
+    </row>
+    <row r="202" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C202" s="1">
         <v>0.74151800000000001</v>
       </c>
@@ -15499,8 +17074,17 @@
       <c r="E202" s="1">
         <v>0.73211499999999996</v>
       </c>
-    </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F202" s="1">
+        <v>0.64139999999999997</v>
+      </c>
+      <c r="G202" s="1">
+        <v>2.1655980000000001</v>
+      </c>
+      <c r="H202" s="1">
+        <v>2.2031000000000001</v>
+      </c>
+    </row>
+    <row r="203" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C203" s="1">
         <v>0.73907500000000004</v>
       </c>
@@ -15510,8 +17094,17 @@
       <c r="E203" s="1">
         <v>0.83703700000000003</v>
       </c>
-    </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F203" s="1">
+        <v>0.62539999999999996</v>
+      </c>
+      <c r="G203" s="1">
+        <v>2.2035010000000002</v>
+      </c>
+      <c r="H203" s="1">
+        <v>2.1949999999999998</v>
+      </c>
+    </row>
+    <row r="204" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C204" s="1">
         <v>0.771505</v>
       </c>
@@ -15521,8 +17114,17 @@
       <c r="E204" s="1">
         <v>0.69959899999999997</v>
       </c>
-    </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F204" s="1">
+        <v>0.6008</v>
+      </c>
+      <c r="G204" s="1">
+        <v>2.2061000000000002</v>
+      </c>
+      <c r="H204" s="1">
+        <v>2.3313000000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C205" s="1">
         <v>0.73191499999999998</v>
       </c>
@@ -15532,8 +17134,17 @@
       <c r="E205" s="1">
         <v>0.92889900000000003</v>
       </c>
-    </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F205" s="1">
+        <v>0.60660000000000003</v>
+      </c>
+      <c r="G205" s="1">
+        <v>2.1854979999999999</v>
+      </c>
+      <c r="H205" s="1">
+        <v>0.75849999999999995</v>
+      </c>
+    </row>
+    <row r="206" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C206" s="1">
         <v>0.67251399999999995</v>
       </c>
@@ -15543,8 +17154,17 @@
       <c r="E206" s="1">
         <v>0.83557000000000003</v>
       </c>
-    </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F206" s="1">
+        <v>0.33529999999999999</v>
+      </c>
+      <c r="G206" s="1">
+        <v>14.603</v>
+      </c>
+      <c r="H206" s="1">
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="207" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C207" s="1">
         <v>0.44656699999999999</v>
       </c>
@@ -15554,8 +17174,17 @@
       <c r="E207" s="1">
         <v>0.61683900000000003</v>
       </c>
-    </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F207" s="1">
+        <v>0.43759999999999999</v>
+      </c>
+      <c r="G207" s="1">
+        <v>1.9117999999999999</v>
+      </c>
+      <c r="H207" s="1">
+        <v>2.1977000000000002</v>
+      </c>
+    </row>
+    <row r="208" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C208" s="1">
         <v>0.64500400000000002</v>
       </c>
@@ -15565,8 +17194,17 @@
       <c r="E208" s="1">
         <v>0.70646299999999995</v>
       </c>
-    </row>
-    <row r="209" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F208" s="1">
+        <v>0.60709900000000006</v>
+      </c>
+      <c r="G208" s="1">
+        <v>2.1983999999999999</v>
+      </c>
+      <c r="H208" s="1">
+        <v>2.2275999999999998</v>
+      </c>
+    </row>
+    <row r="209" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C209" s="1">
         <v>0.73963000000000001</v>
       </c>
@@ -15576,8 +17214,17 @@
       <c r="E209" s="1">
         <v>0.29358299999999998</v>
       </c>
-    </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F209" s="1">
+        <v>0.84150000000000003</v>
+      </c>
+      <c r="G209" s="1">
+        <v>0.77569999999999995</v>
+      </c>
+      <c r="H209" s="1">
+        <v>2.2863000000000002</v>
+      </c>
+    </row>
+    <row r="210" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C210" s="1">
         <v>0.68988000000000005</v>
       </c>
@@ -15587,8 +17234,17 @@
       <c r="E210" s="1">
         <v>0.78344100000000005</v>
       </c>
-    </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F210" s="1">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="G210" s="1">
+        <v>2.1726999999999999</v>
+      </c>
+      <c r="H210" s="1">
+        <v>2.2477</v>
+      </c>
+    </row>
+    <row r="211" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C211" s="1">
         <v>0.77331899999999998</v>
       </c>
@@ -15598,8 +17254,17 @@
       <c r="E211" s="1">
         <v>0.67334099999999997</v>
       </c>
-    </row>
-    <row r="212" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F211" s="1">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="G211" s="1">
+        <v>2.0773999999999999</v>
+      </c>
+      <c r="H211" s="1">
+        <v>2.2130999999999998</v>
+      </c>
+    </row>
+    <row r="212" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C212" s="1">
         <v>0.65244100000000005</v>
       </c>
@@ -15609,8 +17274,17 @@
       <c r="E212" s="1">
         <v>0.68389699999999998</v>
       </c>
-    </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F212" s="1">
+        <v>0.77959999999999996</v>
+      </c>
+      <c r="G212" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="H212" s="1">
+        <v>2.2669999999999999</v>
+      </c>
+    </row>
+    <row r="213" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C213" s="1">
         <v>0.79516100000000001</v>
       </c>
@@ -15620,8 +17294,17 @@
       <c r="E213" s="1">
         <v>0.78646700000000003</v>
       </c>
-    </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F213" s="1">
+        <v>0.80019899999999999</v>
+      </c>
+      <c r="G213" s="1">
+        <v>1.329302</v>
+      </c>
+      <c r="H213" s="1">
+        <v>0.74950000000000006</v>
+      </c>
+    </row>
+    <row r="214" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C214" s="1">
         <v>0.88055899999999998</v>
       </c>
@@ -15631,8 +17314,17 @@
       <c r="E214" s="1">
         <v>0.68656499999999998</v>
       </c>
-    </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F214" s="1">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="G214" s="1">
+        <v>19.864301000000001</v>
+      </c>
+      <c r="H214" s="1">
+        <v>0.97470000000000001</v>
+      </c>
+    </row>
+    <row r="215" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C215" s="1">
         <v>0.71553699999999998</v>
       </c>
@@ -15642,8 +17334,17 @@
       <c r="E215" s="1">
         <v>0.79135500000000003</v>
       </c>
-    </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F215" s="1">
+        <v>0.40710000000000002</v>
+      </c>
+      <c r="G215" s="1">
+        <v>2.1154999999999999</v>
+      </c>
+      <c r="H215" s="1">
+        <v>2.2033999999999998</v>
+      </c>
+    </row>
+    <row r="216" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C216" s="1">
         <v>0.82155500000000004</v>
       </c>
@@ -15653,8 +17354,17 @@
       <c r="E216" s="1">
         <v>0.79961599999999999</v>
       </c>
-    </row>
-    <row r="217" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F216" s="1">
+        <v>0.83930000000000005</v>
+      </c>
+      <c r="G216" s="1">
+        <v>1.9527000000000001</v>
+      </c>
+      <c r="H216" s="1">
+        <v>0.50039999999999996</v>
+      </c>
+    </row>
+    <row r="217" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C217" s="1">
         <v>0.72851500000000002</v>
       </c>
@@ -15664,8 +17374,17 @@
       <c r="E217" s="1">
         <v>0.63454299999999997</v>
       </c>
-    </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F217" s="1">
+        <v>2.2279</v>
+      </c>
+      <c r="G217" s="1">
+        <v>0.77590000000000003</v>
+      </c>
+      <c r="H217" s="1">
+        <v>2.0102000000000002</v>
+      </c>
+    </row>
+    <row r="218" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C218" s="1">
         <v>0.69589999999999996</v>
       </c>
@@ -15675,8 +17394,17 @@
       <c r="E218" s="1">
         <v>0.561859</v>
       </c>
-    </row>
-    <row r="219" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F218" s="1">
+        <v>0.76619999999999999</v>
+      </c>
+      <c r="G218" s="1">
+        <v>1.0994999999999999</v>
+      </c>
+      <c r="H218" s="1">
+        <v>2.1787000000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C219" s="1">
         <v>0.97849200000000003</v>
       </c>
@@ -15686,8 +17414,17 @@
       <c r="E219" s="1">
         <v>0.41889399999999999</v>
       </c>
-    </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F219" s="1">
+        <v>2.0523020000000001</v>
+      </c>
+      <c r="G219" s="1">
+        <v>1.0376000000000001</v>
+      </c>
+      <c r="H219" s="1">
+        <v>1.0767990000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C220" s="1">
         <v>0.88471999999999995</v>
       </c>
@@ -15697,8 +17434,17 @@
       <c r="E220" s="1">
         <v>0.68810499999999997</v>
       </c>
-    </row>
-    <row r="221" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F220" s="1">
+        <v>0.75589700000000004</v>
+      </c>
+      <c r="G220" s="1">
+        <v>0.7339</v>
+      </c>
+      <c r="H220" s="1">
+        <v>1.6238999999999999</v>
+      </c>
+    </row>
+    <row r="221" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C221" s="1">
         <v>0.72514900000000004</v>
       </c>
@@ -15708,8 +17454,17 @@
       <c r="E221" s="1">
         <v>0.68955999999999995</v>
       </c>
-    </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F221" s="1">
+        <v>0.5524</v>
+      </c>
+      <c r="G221" s="1">
+        <v>2.1248999999999998</v>
+      </c>
+      <c r="H221" s="1">
+        <v>1.0063</v>
+      </c>
+    </row>
+    <row r="222" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C222" s="1">
         <v>0.76282399999999995</v>
       </c>
@@ -15719,8 +17474,17 @@
       <c r="E222" s="1">
         <v>0.79119499999999998</v>
       </c>
-    </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F222" s="1">
+        <v>0.58830199999999999</v>
+      </c>
+      <c r="G222" s="1">
+        <v>2.0038010000000002</v>
+      </c>
+      <c r="H222" s="1">
+        <v>2.2656000000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C223" s="1">
         <v>0.76976900000000004</v>
       </c>
@@ -15730,8 +17494,17 @@
       <c r="E223" s="1">
         <v>0.78285400000000005</v>
       </c>
-    </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F223" s="1">
+        <v>0.76019999999999999</v>
+      </c>
+      <c r="G223" s="1">
+        <v>1.0403990000000001</v>
+      </c>
+      <c r="H223" s="1">
+        <v>2.1194999999999999</v>
+      </c>
+    </row>
+    <row r="224" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C224" s="1">
         <v>0.83145100000000005</v>
       </c>
@@ -15741,8 +17514,17 @@
       <c r="E224" s="1">
         <v>0.71130400000000005</v>
       </c>
-    </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F224" s="1">
+        <v>0.36170000000000002</v>
+      </c>
+      <c r="G224" s="1">
+        <v>2.0837979999999998</v>
+      </c>
+      <c r="H224" s="1">
+        <v>1.3709990000000001</v>
+      </c>
+    </row>
+    <row r="225" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C225" s="1">
         <v>0.79926799999999998</v>
       </c>
@@ -15752,8 +17534,17 @@
       <c r="E225" s="1">
         <v>0.75627100000000003</v>
       </c>
-    </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F225" s="1">
+        <v>0.7681</v>
+      </c>
+      <c r="G225" s="1">
+        <v>1.9497</v>
+      </c>
+      <c r="H225" s="1">
+        <v>2.1976</v>
+      </c>
+    </row>
+    <row r="226" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C226" s="1">
         <v>0.98978999999999995</v>
       </c>
@@ -15762,6 +17553,15 @@
       </c>
       <c r="E226" s="1">
         <v>0.77655700000000005</v>
+      </c>
+      <c r="F226" s="1">
+        <v>0.74960000000000004</v>
+      </c>
+      <c r="G226" s="1">
+        <v>0.63170000000000004</v>
+      </c>
+      <c r="H226" s="1">
+        <v>2.161</v>
       </c>
     </row>
   </sheetData>
@@ -15802,10 +17602,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -15848,10 +17648,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">

</xml_diff>

<commit_message>
docs: add delivery times stats for v1 and v2 in single-core mode
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="Questa_cartella_di_lavoro" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fedebrando\SORTproject\SantaClausProblem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B644583C-2187-4AB8-BBFA-BA4C0073073A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403809BE-B6E0-460B-A7CA-AD1C1DCA6F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="732" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="732" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery time (v1, v2)" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Delivery delay (v1)" sheetId="8" r:id="rId3"/>
     <sheet name="Delivery delay (v3)" sheetId="7" r:id="rId4"/>
     <sheet name="Info" sheetId="6" r:id="rId5"/>
+    <sheet name="Mono - Delivery time (v1, v2)" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2652" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2663" uniqueCount="44">
   <si>
     <t>Delivery time (v1, v2)</t>
   </si>
@@ -169,6 +170,9 @@
   </si>
   <si>
     <t>Ubuntu 24.04.1 LTS</t>
+  </si>
+  <si>
+    <t>Mono - Delivery time (v1, v2)</t>
   </si>
 </sst>
 </file>
@@ -51999,7 +52003,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -52107,4 +52111,1692 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB9C7B0-B1F8-4FE3-9454-2714BF9110A0}">
+  <dimension ref="A1:F209"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <f>AVERAGE(C10:C209)</f>
+        <v>97.030955270000064</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <f>AVERAGE(F10:F209)</f>
+        <v>296.25200717500002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <f>_xlfn.STDEV.P(C10:C209)</f>
+        <v>103.85421605575716</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <f>_xlfn.STDEV.P(F10:F209)</f>
+        <v>123.91215086265201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>80.143013999999994</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>533.242391</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>14.024865</v>
+      </c>
+      <c r="F11" s="1">
+        <v>165.046494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
+        <v>56.645995999999997</v>
+      </c>
+      <c r="F12" s="1">
+        <v>309.88448199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>0.978912</v>
+      </c>
+      <c r="F13" s="1">
+        <v>212.721521</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>62.968795</v>
+      </c>
+      <c r="F14" s="1">
+        <v>395.23120999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>14.86913</v>
+      </c>
+      <c r="F15" s="1">
+        <v>380.52380199999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>88.205753999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>562.64658299999996</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <v>9.7071799999999993</v>
+      </c>
+      <c r="F17" s="1">
+        <v>184.559605</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>0.84598799999999996</v>
+      </c>
+      <c r="F18" s="1">
+        <v>321.71781099999998</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>24.549844</v>
+      </c>
+      <c r="F19" s="1">
+        <v>156.83851000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <v>196.50927100000001</v>
+      </c>
+      <c r="F20" s="1">
+        <v>323.45954699999999</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>17.674596999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <v>195.669296</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <v>50.368941999999997</v>
+      </c>
+      <c r="F22" s="1">
+        <v>282.92290300000002</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
+        <v>86.112577000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <v>356.60150199999998</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <v>68.972820999999996</v>
+      </c>
+      <c r="F24" s="1">
+        <v>330.51209499999999</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <v>16.974917999999999</v>
+      </c>
+      <c r="F25" s="1">
+        <v>307.597398</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <v>44.503993000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>212.32091399999999</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <v>326.39471900000001</v>
+      </c>
+      <c r="F27" s="1">
+        <v>564.50740399999995</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <v>43.634785000000001</v>
+      </c>
+      <c r="F28" s="1">
+        <v>240.09353100000001</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="1">
+        <v>204.880495</v>
+      </c>
+      <c r="F29" s="1">
+        <v>349.18290000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="1">
+        <v>391.19032399999998</v>
+      </c>
+      <c r="F30" s="1">
+        <v>203.173857</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="1">
+        <v>70.080993000000007</v>
+      </c>
+      <c r="F31" s="1">
+        <v>179.78732600000001</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="1">
+        <v>79.071269000000001</v>
+      </c>
+      <c r="F32" s="1">
+        <v>383.33536400000003</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="1">
+        <v>91.526026999999999</v>
+      </c>
+      <c r="F33" s="1">
+        <v>289.42399399999999</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="1">
+        <v>5.4886109999999997</v>
+      </c>
+      <c r="F34" s="1">
+        <v>362.48081000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <v>47.585825</v>
+      </c>
+      <c r="F35" s="1">
+        <v>125.644406</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="1">
+        <v>388.92063100000001</v>
+      </c>
+      <c r="F36" s="1">
+        <v>120.699203</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="1">
+        <v>61.653886999999997</v>
+      </c>
+      <c r="F37" s="1">
+        <v>209.081839</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="1">
+        <v>51.301350999999997</v>
+      </c>
+      <c r="F38" s="1">
+        <v>428.00740400000001</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="1">
+        <v>180.33872099999999</v>
+      </c>
+      <c r="F39" s="1">
+        <v>358.22053399999999</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="1">
+        <v>140.830521</v>
+      </c>
+      <c r="F40" s="1">
+        <v>286.31291599999997</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="1">
+        <v>144.794601</v>
+      </c>
+      <c r="F41" s="1">
+        <v>265.17615999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="1">
+        <v>73.823051000000007</v>
+      </c>
+      <c r="F42" s="1">
+        <v>416.71453700000001</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="1">
+        <v>105.753854</v>
+      </c>
+      <c r="F43" s="1">
+        <v>255.210497</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="1">
+        <v>318.43550699999997</v>
+      </c>
+      <c r="F44" s="1">
+        <v>133.63425000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="1">
+        <v>9.301444</v>
+      </c>
+      <c r="F45" s="1">
+        <v>312.67304300000001</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <v>323.01961599999998</v>
+      </c>
+      <c r="F46" s="1">
+        <v>220.08216999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="1">
+        <v>99.454774999999998</v>
+      </c>
+      <c r="F47" s="1">
+        <v>152.55163300000001</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="1">
+        <v>96.673851999999997</v>
+      </c>
+      <c r="F48" s="1">
+        <v>248.467175</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="1">
+        <v>200.617706</v>
+      </c>
+      <c r="F49" s="1">
+        <v>343.61831899999999</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="1">
+        <v>22.893809000000001</v>
+      </c>
+      <c r="F50" s="1">
+        <v>373.77198299999998</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="1">
+        <v>278.167328</v>
+      </c>
+      <c r="F51" s="1">
+        <v>249.08391800000001</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="1">
+        <v>35.810136999999997</v>
+      </c>
+      <c r="F52" s="1">
+        <v>282.13696599999997</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="1">
+        <v>212.45859400000001</v>
+      </c>
+      <c r="F53" s="1">
+        <v>947.47135800000001</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="1">
+        <v>15.008429</v>
+      </c>
+      <c r="F54" s="1">
+        <v>322.53945800000002</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="1">
+        <v>241.05638400000001</v>
+      </c>
+      <c r="F55" s="1">
+        <v>200.80921000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="1">
+        <v>59.717348999999999</v>
+      </c>
+      <c r="F56" s="1">
+        <v>163.864114</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="1">
+        <v>67.408395999999996</v>
+      </c>
+      <c r="F57" s="1">
+        <v>157.38492299999999</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="1">
+        <v>85.576390000000004</v>
+      </c>
+      <c r="F58" s="1">
+        <v>385.09050300000001</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="1">
+        <v>69.682626999999997</v>
+      </c>
+      <c r="F59" s="1">
+        <v>259.89176600000002</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="1">
+        <v>22.952817</v>
+      </c>
+      <c r="F60" s="1">
+        <v>396.59077400000001</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C61" s="1">
+        <v>8.5188199999999998</v>
+      </c>
+      <c r="F61" s="1">
+        <v>240.886742</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="1">
+        <v>48.733960000000003</v>
+      </c>
+      <c r="F62" s="1">
+        <v>161.581109</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C63" s="1">
+        <v>70.787644999999998</v>
+      </c>
+      <c r="F63" s="1">
+        <v>206.29179099999999</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C64" s="1">
+        <v>326.16850299999999</v>
+      </c>
+      <c r="F64" s="1">
+        <v>215.184729</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C65" s="1">
+        <v>203.95152400000001</v>
+      </c>
+      <c r="F65" s="1">
+        <v>378.15400599999998</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C66" s="1">
+        <v>78.535073999999994</v>
+      </c>
+      <c r="F66" s="1">
+        <v>109.12318</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C67" s="1">
+        <v>104.368781</v>
+      </c>
+      <c r="F67" s="1">
+        <v>339.39714099999998</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C68" s="1">
+        <v>153.063762</v>
+      </c>
+      <c r="F68" s="1">
+        <v>180.041954</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="1">
+        <v>113.22761300000001</v>
+      </c>
+      <c r="F69" s="1">
+        <v>453.15302500000001</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="1">
+        <v>434.71728899999999</v>
+      </c>
+      <c r="F70" s="1">
+        <v>352.12995799999999</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="1">
+        <v>34.256276999999997</v>
+      </c>
+      <c r="F71" s="1">
+        <v>260.11660599999999</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="1">
+        <v>118.141498</v>
+      </c>
+      <c r="F72" s="1">
+        <v>408.157804</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="1">
+        <v>13.428765</v>
+      </c>
+      <c r="F73" s="1">
+        <v>407.52636100000001</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="1">
+        <v>135.32086000000001</v>
+      </c>
+      <c r="F74" s="1">
+        <v>375.16001499999999</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="1">
+        <v>93.117241000000007</v>
+      </c>
+      <c r="F75" s="1">
+        <v>647.26078299999995</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="1">
+        <v>86.870762999999997</v>
+      </c>
+      <c r="F76" s="1">
+        <v>289.16305899999998</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C77" s="1">
+        <v>57.950308999999997</v>
+      </c>
+      <c r="F77" s="1">
+        <v>170.120857</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C78" s="1">
+        <v>40.785545999999997</v>
+      </c>
+      <c r="F78" s="1">
+        <v>255.315618</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C79" s="1">
+        <v>258.90413000000001</v>
+      </c>
+      <c r="F79" s="1">
+        <v>199.652252</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C80" s="1">
+        <v>156.39234400000001</v>
+      </c>
+      <c r="F80" s="1">
+        <v>300.46394199999997</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C81" s="1">
+        <v>4.7556950000000002</v>
+      </c>
+      <c r="F81" s="1">
+        <v>315.05486000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C82" s="1">
+        <v>160.03752</v>
+      </c>
+      <c r="F82" s="1">
+        <v>419.59644300000002</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C83" s="1">
+        <v>28.783408000000001</v>
+      </c>
+      <c r="F83" s="1">
+        <v>567.85238200000003</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C84" s="1">
+        <v>115.506139</v>
+      </c>
+      <c r="F84" s="1">
+        <v>252.64737099999999</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C85" s="1">
+        <v>190.96290200000001</v>
+      </c>
+      <c r="F85" s="1">
+        <v>323.30109099999999</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C86" s="1">
+        <v>86.348844999999997</v>
+      </c>
+      <c r="F86" s="1">
+        <v>400.43598200000002</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C87" s="1">
+        <v>238.266345</v>
+      </c>
+      <c r="F87" s="1">
+        <v>216.57711800000001</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C88" s="1">
+        <v>29.683983000000001</v>
+      </c>
+      <c r="F88" s="1">
+        <v>329.92772600000001</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C89" s="1">
+        <v>61.694096999999999</v>
+      </c>
+      <c r="F89" s="1">
+        <v>377.77430600000002</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C90" s="1">
+        <v>2.6943800000000002</v>
+      </c>
+      <c r="F90" s="1">
+        <v>169.43219500000001</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C91" s="1">
+        <v>12.481166999999999</v>
+      </c>
+      <c r="F91" s="1">
+        <v>94.269502000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C92" s="1">
+        <v>151.88175200000001</v>
+      </c>
+      <c r="F92" s="1">
+        <v>242.01369299999999</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="1">
+        <v>3.3822359999999998</v>
+      </c>
+      <c r="F93" s="1">
+        <v>139.36834500000001</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C94" s="1">
+        <v>5.1283830000000004</v>
+      </c>
+      <c r="F94" s="1">
+        <v>264.82196099999999</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C95" s="1">
+        <v>22.447633</v>
+      </c>
+      <c r="F95" s="1">
+        <v>292.108856</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C96" s="1">
+        <v>115.35158800000001</v>
+      </c>
+      <c r="F96" s="1">
+        <v>371.52019100000001</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C97" s="1">
+        <v>12.765056</v>
+      </c>
+      <c r="F97" s="1">
+        <v>323.07462399999997</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C98" s="1">
+        <v>119.07070299999999</v>
+      </c>
+      <c r="F98" s="1">
+        <v>463.27650199999999</v>
+      </c>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C99" s="1">
+        <v>31.877600999999999</v>
+      </c>
+      <c r="F99" s="1">
+        <v>209.85039399999999</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C100" s="1">
+        <v>208.92201299999999</v>
+      </c>
+      <c r="F100" s="1">
+        <v>313.76198399999998</v>
+      </c>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C101" s="1">
+        <v>19.645424999999999</v>
+      </c>
+      <c r="F101" s="1">
+        <v>327.39261599999998</v>
+      </c>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C102" s="1">
+        <v>59.048861000000002</v>
+      </c>
+      <c r="F102" s="1">
+        <v>507.05940299999997</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C103" s="1">
+        <v>231.74169000000001</v>
+      </c>
+      <c r="F103" s="1">
+        <v>238.485365</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C104" s="1">
+        <v>607.61736099999996</v>
+      </c>
+      <c r="F104" s="1">
+        <v>212.98210399999999</v>
+      </c>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C105" s="1">
+        <v>45.208976999999997</v>
+      </c>
+      <c r="F105" s="1">
+        <v>398.94065599999999</v>
+      </c>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C106" s="1">
+        <v>39.673816000000002</v>
+      </c>
+      <c r="F106" s="1">
+        <v>262.29059999999998</v>
+      </c>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C107" s="1">
+        <v>5.1723359999999996</v>
+      </c>
+      <c r="F107" s="1">
+        <v>415.84832699999998</v>
+      </c>
+    </row>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C108" s="1">
+        <v>121.02436899999999</v>
+      </c>
+      <c r="F108" s="1">
+        <v>184.04142400000001</v>
+      </c>
+    </row>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C109" s="1">
+        <v>94.534620000000004</v>
+      </c>
+      <c r="F109" s="1">
+        <v>348.57924400000002</v>
+      </c>
+    </row>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C110" s="1">
+        <v>84.696506999999997</v>
+      </c>
+      <c r="F110" s="1">
+        <v>283.28152399999999</v>
+      </c>
+    </row>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C111" s="1">
+        <v>53.743983999999998</v>
+      </c>
+      <c r="F111" s="1">
+        <v>287.74733099999997</v>
+      </c>
+    </row>
+    <row r="112" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C112" s="1">
+        <v>14.824087</v>
+      </c>
+      <c r="F112" s="1">
+        <v>262.59267599999998</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C113" s="1">
+        <v>65.636634999999998</v>
+      </c>
+      <c r="F113" s="1">
+        <v>249.67773500000001</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C114" s="1">
+        <v>185.178946</v>
+      </c>
+      <c r="F114" s="1">
+        <v>319.23586899999998</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C115" s="1">
+        <v>18.238409000000001</v>
+      </c>
+      <c r="F115" s="1">
+        <v>305.61147499999998</v>
+      </c>
+    </row>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C116" s="1">
+        <v>1.5779069999999999</v>
+      </c>
+      <c r="F116" s="1">
+        <v>424.12918200000001</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C117" s="1">
+        <v>117.10802700000001</v>
+      </c>
+      <c r="F117" s="1">
+        <v>459.84619600000002</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C118" s="1">
+        <v>46.638258999999998</v>
+      </c>
+      <c r="F118" s="1">
+        <v>289.45657999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C119" s="1">
+        <v>35.591298000000002</v>
+      </c>
+      <c r="F119" s="1">
+        <v>324.418137</v>
+      </c>
+    </row>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C120" s="1">
+        <v>57.445183</v>
+      </c>
+      <c r="F120" s="1">
+        <v>344.93320499999999</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C121" s="1">
+        <v>198.613517</v>
+      </c>
+      <c r="F121" s="1">
+        <v>278.20789200000002</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C122" s="1">
+        <v>3.727417</v>
+      </c>
+      <c r="F122" s="1">
+        <v>125.776004</v>
+      </c>
+    </row>
+    <row r="123" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C123" s="1">
+        <v>36.506329999999998</v>
+      </c>
+      <c r="F123" s="1">
+        <v>553.97444700000005</v>
+      </c>
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C124" s="1">
+        <v>13.852943</v>
+      </c>
+      <c r="F124" s="1">
+        <v>263.79077699999999</v>
+      </c>
+    </row>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C125" s="1">
+        <v>2.0022310000000001</v>
+      </c>
+      <c r="F125" s="1">
+        <v>482.20359500000001</v>
+      </c>
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C126" s="1">
+        <v>95.348348000000001</v>
+      </c>
+      <c r="F126" s="1">
+        <v>222.34730300000001</v>
+      </c>
+    </row>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C127" s="1">
+        <v>31.689444000000002</v>
+      </c>
+      <c r="F127" s="1">
+        <v>174.07472300000001</v>
+      </c>
+    </row>
+    <row r="128" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C128" s="1">
+        <v>203.32939500000001</v>
+      </c>
+      <c r="F128" s="1">
+        <v>224.47784999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C129" s="1">
+        <v>78.051934000000003</v>
+      </c>
+      <c r="F129" s="1">
+        <v>280.105951</v>
+      </c>
+    </row>
+    <row r="130" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C130" s="1">
+        <v>12.322815</v>
+      </c>
+      <c r="F130" s="1">
+        <v>181.63274999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C131" s="1">
+        <v>17.975351</v>
+      </c>
+      <c r="F131" s="1">
+        <v>283.74100099999998</v>
+      </c>
+    </row>
+    <row r="132" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C132" s="1">
+        <v>53.402709999999999</v>
+      </c>
+      <c r="F132" s="1">
+        <v>365.52516100000003</v>
+      </c>
+    </row>
+    <row r="133" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C133" s="1">
+        <v>8.8620439999999991</v>
+      </c>
+      <c r="F133" s="1">
+        <v>552.50228700000002</v>
+      </c>
+    </row>
+    <row r="134" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C134" s="1">
+        <v>163.91554099999999</v>
+      </c>
+      <c r="F134" s="1">
+        <v>353.42206399999998</v>
+      </c>
+    </row>
+    <row r="135" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C135" s="1">
+        <v>119.901448</v>
+      </c>
+      <c r="F135" s="1">
+        <v>206.68205800000001</v>
+      </c>
+    </row>
+    <row r="136" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C136" s="1">
+        <v>232.16203899999999</v>
+      </c>
+      <c r="F136" s="1">
+        <v>482.61000999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C137" s="1">
+        <v>78.041884999999994</v>
+      </c>
+      <c r="F137" s="1">
+        <v>248.70953600000001</v>
+      </c>
+    </row>
+    <row r="138" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C138" s="1">
+        <v>6.3484030000000002</v>
+      </c>
+      <c r="F138" s="1">
+        <v>253.125922</v>
+      </c>
+    </row>
+    <row r="139" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C139" s="1">
+        <v>127.19806800000001</v>
+      </c>
+      <c r="F139" s="1">
+        <v>231.82560699999999</v>
+      </c>
+    </row>
+    <row r="140" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C140" s="1">
+        <v>248.3218</v>
+      </c>
+      <c r="F140" s="1">
+        <v>165.21378899999999</v>
+      </c>
+    </row>
+    <row r="141" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C141" s="1">
+        <v>41.833241999999998</v>
+      </c>
+      <c r="F141" s="1">
+        <v>278.08192100000002</v>
+      </c>
+    </row>
+    <row r="142" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C142" s="1">
+        <v>3.6821169999999999</v>
+      </c>
+      <c r="F142" s="1">
+        <v>184.790018</v>
+      </c>
+    </row>
+    <row r="143" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C143" s="1">
+        <v>12.654567999999999</v>
+      </c>
+      <c r="F143" s="1">
+        <v>418.98097200000001</v>
+      </c>
+    </row>
+    <row r="144" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C144" s="1">
+        <v>184.98943199999999</v>
+      </c>
+      <c r="F144" s="1">
+        <v>281.778482</v>
+      </c>
+    </row>
+    <row r="145" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C145" s="1">
+        <v>50.713078000000003</v>
+      </c>
+      <c r="F145" s="1">
+        <v>297.46616599999999</v>
+      </c>
+    </row>
+    <row r="146" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C146" s="1">
+        <v>82.580360999999996</v>
+      </c>
+      <c r="F146" s="1">
+        <v>257.52173099999999</v>
+      </c>
+    </row>
+    <row r="147" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C147" s="1">
+        <v>1.1840349999999999</v>
+      </c>
+      <c r="F147" s="1">
+        <v>135.72441000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C148" s="1">
+        <v>7.4888830000000004</v>
+      </c>
+      <c r="F148" s="1">
+        <v>242.70813999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C149" s="1">
+        <v>1.800861</v>
+      </c>
+      <c r="F149" s="1">
+        <v>342.82256000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C150" s="1">
+        <v>58.666276000000003</v>
+      </c>
+      <c r="F150" s="1">
+        <v>394.05094200000002</v>
+      </c>
+    </row>
+    <row r="151" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C151" s="1">
+        <v>100.48105200000001</v>
+      </c>
+      <c r="F151" s="1">
+        <v>88.083781000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C152" s="1">
+        <v>139.27873099999999</v>
+      </c>
+      <c r="F152" s="1">
+        <v>243.41771900000001</v>
+      </c>
+    </row>
+    <row r="153" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C153" s="1">
+        <v>2.1493000000000002</v>
+      </c>
+      <c r="F153" s="1">
+        <v>270.45802700000002</v>
+      </c>
+    </row>
+    <row r="154" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C154" s="1">
+        <v>0.117995</v>
+      </c>
+      <c r="F154" s="1">
+        <v>221.86003600000001</v>
+      </c>
+    </row>
+    <row r="155" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C155" s="1">
+        <v>0.67109700000000005</v>
+      </c>
+      <c r="F155" s="1">
+        <v>125.344852</v>
+      </c>
+    </row>
+    <row r="156" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C156" s="1">
+        <v>236.09945500000001</v>
+      </c>
+      <c r="F156" s="1">
+        <v>419.73859399999998</v>
+      </c>
+    </row>
+    <row r="157" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C157" s="1">
+        <v>34.074939999999998</v>
+      </c>
+      <c r="F157" s="1">
+        <v>230.909335</v>
+      </c>
+    </row>
+    <row r="158" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C158" s="1">
+        <v>8.7774319999999992</v>
+      </c>
+      <c r="F158" s="1">
+        <v>306.74425200000002</v>
+      </c>
+    </row>
+    <row r="159" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C159" s="1">
+        <v>418.16290800000002</v>
+      </c>
+      <c r="F159" s="1">
+        <v>300.97759300000001</v>
+      </c>
+    </row>
+    <row r="160" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C160" s="1">
+        <v>46.714239999999997</v>
+      </c>
+      <c r="F160" s="1">
+        <v>155.938301</v>
+      </c>
+    </row>
+    <row r="161" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C161" s="1">
+        <v>68.568438999999998</v>
+      </c>
+      <c r="F161" s="1">
+        <v>104.46444700000001</v>
+      </c>
+    </row>
+    <row r="162" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C162" s="1">
+        <v>72.735917000000001</v>
+      </c>
+      <c r="F162" s="1">
+        <v>208.56156999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C163" s="1">
+        <v>13.018898999999999</v>
+      </c>
+      <c r="F163" s="1">
+        <v>153.69057900000001</v>
+      </c>
+    </row>
+    <row r="164" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C164" s="1">
+        <v>3.0452349999999999</v>
+      </c>
+      <c r="F164" s="1">
+        <v>360.11909700000001</v>
+      </c>
+    </row>
+    <row r="165" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C165" s="1">
+        <v>248.037665</v>
+      </c>
+      <c r="F165" s="1">
+        <v>513.39609599999994</v>
+      </c>
+    </row>
+    <row r="166" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C166" s="1">
+        <v>13.727830000000001</v>
+      </c>
+      <c r="F166" s="1">
+        <v>159.25969000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C167" s="1">
+        <v>67.662137000000001</v>
+      </c>
+      <c r="F167" s="1">
+        <v>438.54501199999999</v>
+      </c>
+    </row>
+    <row r="168" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C168" s="1">
+        <v>25.267101</v>
+      </c>
+      <c r="F168" s="1">
+        <v>495.528211</v>
+      </c>
+    </row>
+    <row r="169" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C169" s="1">
+        <v>79.248892999999995</v>
+      </c>
+      <c r="F169" s="1">
+        <v>225.07273900000001</v>
+      </c>
+    </row>
+    <row r="170" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C170" s="1">
+        <v>185.04996</v>
+      </c>
+      <c r="F170" s="1">
+        <v>297.55053199999998</v>
+      </c>
+    </row>
+    <row r="171" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C171" s="1">
+        <v>14.51501</v>
+      </c>
+      <c r="F171" s="1">
+        <v>309.08976899999999</v>
+      </c>
+    </row>
+    <row r="172" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C172" s="1">
+        <v>90.522319999999993</v>
+      </c>
+      <c r="F172" s="1">
+        <v>381.50948</v>
+      </c>
+    </row>
+    <row r="173" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C173" s="1">
+        <v>28.337983999999999</v>
+      </c>
+      <c r="F173" s="1">
+        <v>238.89588699999999</v>
+      </c>
+    </row>
+    <row r="174" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C174" s="1">
+        <v>37.295679</v>
+      </c>
+      <c r="F174" s="1">
+        <v>259.65769599999999</v>
+      </c>
+    </row>
+    <row r="175" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C175" s="1">
+        <v>240.64601999999999</v>
+      </c>
+      <c r="F175" s="1">
+        <v>198.20449099999999</v>
+      </c>
+    </row>
+    <row r="176" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C176" s="1">
+        <v>118.72821</v>
+      </c>
+      <c r="F176" s="1">
+        <v>293.02556399999997</v>
+      </c>
+    </row>
+    <row r="177" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C177" s="1">
+        <v>270.74082099999998</v>
+      </c>
+      <c r="F177" s="1">
+        <v>230.25788499999999</v>
+      </c>
+    </row>
+    <row r="178" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C178" s="1">
+        <v>228.814649</v>
+      </c>
+      <c r="F178" s="1">
+        <v>222.06606099999999</v>
+      </c>
+    </row>
+    <row r="179" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C179" s="1">
+        <v>266.07480399999997</v>
+      </c>
+      <c r="F179" s="1">
+        <v>216.05853999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C180" s="1">
+        <v>64.582222999999999</v>
+      </c>
+      <c r="F180" s="1">
+        <v>160.845056</v>
+      </c>
+    </row>
+    <row r="181" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C181" s="1">
+        <v>28.114811</v>
+      </c>
+      <c r="F181" s="1">
+        <v>351.087132</v>
+      </c>
+    </row>
+    <row r="182" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C182" s="1">
+        <v>77.250056000000001</v>
+      </c>
+      <c r="F182" s="1">
+        <v>381.40286300000002</v>
+      </c>
+    </row>
+    <row r="183" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C183" s="1">
+        <v>149.47692699999999</v>
+      </c>
+      <c r="F183" s="1">
+        <v>262.77522900000002</v>
+      </c>
+    </row>
+    <row r="184" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C184" s="1">
+        <v>10.139818999999999</v>
+      </c>
+      <c r="F184" s="1">
+        <v>352.56961200000001</v>
+      </c>
+    </row>
+    <row r="185" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C185" s="1">
+        <v>13.794979</v>
+      </c>
+      <c r="F185" s="1">
+        <v>173.69791000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C186" s="1">
+        <v>194.53581</v>
+      </c>
+      <c r="F186" s="1">
+        <v>617.28961500000003</v>
+      </c>
+    </row>
+    <row r="187" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C187" s="1">
+        <v>45.217889999999997</v>
+      </c>
+      <c r="F187" s="1">
+        <v>199.125708</v>
+      </c>
+    </row>
+    <row r="188" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C188" s="1">
+        <v>15.774573999999999</v>
+      </c>
+      <c r="F188" s="1">
+        <v>521.05310199999997</v>
+      </c>
+    </row>
+    <row r="189" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C189" s="1">
+        <v>36.482402</v>
+      </c>
+      <c r="F189" s="1">
+        <v>156.51400599999999</v>
+      </c>
+    </row>
+    <row r="190" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C190" s="1">
+        <v>43.651746000000003</v>
+      </c>
+      <c r="F190" s="1">
+        <v>230.062254</v>
+      </c>
+    </row>
+    <row r="191" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C191" s="1">
+        <v>38.760736000000001</v>
+      </c>
+      <c r="F191" s="1">
+        <v>325.71643499999999</v>
+      </c>
+    </row>
+    <row r="192" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C192" s="1">
+        <v>342.83339799999999</v>
+      </c>
+      <c r="F192" s="1">
+        <v>279.218951</v>
+      </c>
+    </row>
+    <row r="193" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C193" s="1">
+        <v>1.975868</v>
+      </c>
+      <c r="F193" s="1">
+        <v>552.48265500000002</v>
+      </c>
+    </row>
+    <row r="194" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C194" s="1">
+        <v>35.747219999999999</v>
+      </c>
+      <c r="F194" s="1">
+        <v>759.88971400000003</v>
+      </c>
+    </row>
+    <row r="195" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C195" s="1">
+        <v>418.03801299999998</v>
+      </c>
+      <c r="F195" s="1">
+        <v>360.02332200000001</v>
+      </c>
+    </row>
+    <row r="196" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C196" s="1">
+        <v>123.441793</v>
+      </c>
+      <c r="F196" s="1">
+        <v>269.954295</v>
+      </c>
+    </row>
+    <row r="197" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C197" s="1">
+        <v>63.276328999999997</v>
+      </c>
+      <c r="F197" s="1">
+        <v>285.73082099999999</v>
+      </c>
+    </row>
+    <row r="198" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C198" s="1">
+        <v>3.7745410000000001</v>
+      </c>
+      <c r="F198" s="1">
+        <v>155.318106</v>
+      </c>
+    </row>
+    <row r="199" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C199" s="1">
+        <v>17.788315000000001</v>
+      </c>
+      <c r="F199" s="1">
+        <v>221.971766</v>
+      </c>
+    </row>
+    <row r="200" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C200" s="1">
+        <v>428.40855599999998</v>
+      </c>
+      <c r="F200" s="1">
+        <v>303.61791799999997</v>
+      </c>
+    </row>
+    <row r="201" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C201" s="1">
+        <v>47.808450999999998</v>
+      </c>
+      <c r="F201" s="1">
+        <v>137.82240999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C202" s="1">
+        <v>138.652535</v>
+      </c>
+      <c r="F202" s="1">
+        <v>290.24463400000002</v>
+      </c>
+    </row>
+    <row r="203" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C203" s="1">
+        <v>19.234815999999999</v>
+      </c>
+      <c r="F203" s="1">
+        <v>125.76108600000001</v>
+      </c>
+    </row>
+    <row r="204" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C204" s="1">
+        <v>46.264746000000002</v>
+      </c>
+      <c r="F204" s="1">
+        <v>271.21439600000002</v>
+      </c>
+    </row>
+    <row r="205" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C205" s="1">
+        <v>58.515027000000003</v>
+      </c>
+      <c r="F205" s="1">
+        <v>195.614439</v>
+      </c>
+    </row>
+    <row r="206" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C206" s="1">
+        <v>69.841836000000001</v>
+      </c>
+      <c r="F206" s="1">
+        <v>250.191541</v>
+      </c>
+    </row>
+    <row r="207" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C207" s="1">
+        <v>57.204557000000001</v>
+      </c>
+      <c r="F207" s="1">
+        <v>172.00312</v>
+      </c>
+    </row>
+    <row r="208" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C208" s="1">
+        <v>50.180343000000001</v>
+      </c>
+      <c r="F208" s="1">
+        <v>221.82815299999999</v>
+      </c>
+    </row>
+    <row r="209" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C209" s="1">
+        <v>86.501228999999995</v>
+      </c>
+      <c r="F209" s="1">
+        <v>332.76886500000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update graphs with affine interpolation
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="Questa_cartella_di_lavoro" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fedebrando\SORTproject\SantaClausProblem\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403809BE-B6E0-460B-A7CA-AD1C1DCA6F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3402A4BF-64EC-466A-9AEE-E4C6D447BE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="732" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery time (v1, v2)" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Delivery delay (v1)" sheetId="8" r:id="rId3"/>
     <sheet name="Delivery delay (v3)" sheetId="7" r:id="rId4"/>
     <sheet name="Info" sheetId="6" r:id="rId5"/>
-    <sheet name="Mono - Delivery time (v1, v2)" sheetId="9" r:id="rId6"/>
+    <sheet name="Single - Delivery time (v1, v2)" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -172,7 +172,7 @@
     <t>Ubuntu 24.04.1 LTS</t>
   </si>
   <si>
-    <t>Mono - Delivery time (v1, v2)</t>
+    <t>Single core - Delivery time (v1, v2)</t>
   </si>
 </sst>
 </file>
@@ -850,7 +850,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -880,7 +880,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:noFill/>
@@ -984,7 +984,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BC87-4D3E-8779-88CE4C02A306}"/>
@@ -1342,7 +1342,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1353,7 +1353,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1364,12 +1364,10 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1470,7 +1468,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-B657-4DBD-9411-F48751A41616}"/>
@@ -1843,7 +1841,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1862,7 +1860,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1873,12 +1871,10 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1991,7 +1987,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-191F-4EBB-A775-9B2BF2164F3D}"/>
@@ -2015,7 +2011,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2026,12 +2022,10 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -2144,7 +2138,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-191F-4EBB-A775-9B2BF2164F3D}"/>
@@ -2168,7 +2162,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2179,12 +2173,10 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -2297,7 +2289,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-191F-4EBB-A775-9B2BF2164F3D}"/>
@@ -2552,8 +2544,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.84128417356408325"/>
           <c:y val="0.35467829021372327"/>
-          <c:w val="6.7168296965136695E-2"/>
-          <c:h val="0.24580989876265466"/>
+          <c:w val="4.4856124267888965E-2"/>
+          <c:h val="0.25115157480314959"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5284,7 +5276,7 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6974,7 +6966,7 @@
   <dimension ref="A1:O226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15320,7 +15312,7 @@
   <dimension ref="A1:Q225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23840,7 +23832,7 @@
   <dimension ref="A1:AU226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52117,7 +52109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB9C7B0-B1F8-4FE3-9454-2714BF9110A0}">
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>